<commit_message>
scaled rates, updated rate computation in filters, new config
</commit_message>
<xml_diff>
--- a/Data/intermediate.xlsx
+++ b/Data/intermediate.xlsx
@@ -526,88 +526,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.008153506589149428</v>
+        <v>-3.062472067885806</v>
       </c>
       <c r="C2" t="n">
-        <v>0.256859853640089</v>
+        <v>-1.238964260942972</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3992947653942425</v>
+        <v>7.437373840288144</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5153936972083695</v>
+        <v>-10.72152501685048</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2117987696999733</v>
+        <v>-6.291011590403967</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2515253665356104</v>
+        <v>-5.122548905943133</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.1976498319019133</v>
+        <v>-12.09360305353633</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3360845478131744</v>
+        <v>-2.194374853749748</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5030629989280867</v>
+        <v>5.588484447958806</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2301770378182125</v>
+        <v>2.942436717004137</v>
       </c>
       <c r="L2" t="n">
-        <v>0.05441886968677331</v>
+        <v>16.97104816942395</v>
       </c>
       <c r="M2" t="n">
-        <v>0.04042893526986022</v>
+        <v>14.66687257116591</v>
       </c>
       <c r="N2" t="n">
-        <v>0.4654984224500882</v>
+        <v>-5.279801303487293</v>
       </c>
       <c r="O2" t="n">
-        <v>0.05184929446581922</v>
+        <v>-2.027855489921127</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.2158875371930763</v>
+        <v>-6.020561393380905</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.523916412453069</v>
+        <v>-7.19228927023893</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1780499740386647</v>
+        <v>-10.88254097223103</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.2515590923394776</v>
+        <v>-1.91471115892682</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6561410635417937</v>
+        <v>-13.10694981157039</v>
       </c>
       <c r="U2" t="n">
-        <v>0.01254740125506459</v>
+        <v>-17.32416129087358</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1713157985399073</v>
+        <v>-6.89214987764487</v>
       </c>
       <c r="W2" t="n">
-        <v>0.006634047708974661</v>
+        <v>-21.53375914133988</v>
       </c>
       <c r="X2" t="n">
-        <v>0.1945018527514511</v>
+        <v>-15.59812707021529</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.1682483635695977</v>
+        <v>-23.40566861543854</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.2459925000465174</v>
+        <v>-30.63856331673106</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.06571928551493866</v>
+        <v>-30.35127888996791</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.2372574148812835</v>
+        <v>-37.94820144614945</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.3253080600394416</v>
+        <v>-53.50836577097834</v>
       </c>
     </row>
     <row r="3">
@@ -615,88 +615,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4682901135194639</v>
+        <v>-1.139485085637585</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.2908264907356138</v>
+        <v>-1.241979489516393</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1244325396039242</v>
+        <v>5.59988776736893</v>
       </c>
       <c r="E3" t="n">
-        <v>0.004276275113576089</v>
+        <v>-10.20867042735266</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2527197531664596</v>
+        <v>-5.327468593538963</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.2780424432377684</v>
+        <v>-4.685846710856667</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.6542120292743182</v>
+        <v>-12.10355983859855</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.233723722409952</v>
+        <v>0.4370724523983638</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.01749069807722387</v>
+        <v>6.602389756637396</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.2578853734171602</v>
+        <v>3.73543412644946</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.470613075001344</v>
+        <v>14.68014145885492</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.4225854744952893</v>
+        <v>11.86278066764788</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.03311619675703015</v>
+        <v>-8.006074568606715</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.4292440560096271</v>
+        <v>-4.177002472873207</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.7596376376561288</v>
+        <v>-5.132740790948361</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.007909285529041687</v>
+        <v>-5.061576974475349</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.3205924024263873</v>
+        <v>-10.13486565098249</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.7715967077975732</v>
+        <v>-1.994121656626827</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1639962481233642</v>
+        <v>-14.97482099342375</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.58784861772125</v>
+        <v>-17.25606074705173</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.3352275982978978</v>
+        <v>-6.01774991476924</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.4628913912644134</v>
+        <v>-21.98781703417996</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.237016440879123</v>
+        <v>-14.28049012570534</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.3326317680296015</v>
+        <v>-24.60085862736441</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.72120734597751</v>
+        <v>-29.77937129340319</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.3704345050975256</v>
+        <v>-30.99139082150541</v>
       </c>
       <c r="AB3" t="n">
-        <v>-0.2872965716153822</v>
+        <v>-36.71630962320474</v>
       </c>
       <c r="AC3" t="n">
-        <v>-0.8224793093949382</v>
+        <v>-54.51464059041903</v>
       </c>
     </row>
     <row r="4">
@@ -704,88 +704,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0739927827671604</v>
+        <v>-0.4467285704480823</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1141092077972918</v>
+        <v>-1.168513231793739</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2619221766407498</v>
+        <v>7.697884648782734</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3457481421424305</v>
+        <v>-11.45940576018544</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1465329469716535</v>
+        <v>-7.420421936007324</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1371804730730564</v>
+        <v>-4.555631857672106</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.2836521071353876</v>
+        <v>-11.49305199086962</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1946706876197964</v>
+        <v>-0.5261801105283777</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3607440828407686</v>
+        <v>6.537566657249014</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1235620827888833</v>
+        <v>3.856865919024551</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.06302211670477983</v>
+        <v>15.27426585997895</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.02678133541134459</v>
+        <v>13.30410813477789</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2647128062844898</v>
+        <v>-6.82700796225998</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.04228088676581955</v>
+        <v>-5.75984944657945</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.3529770605454043</v>
+        <v>-4.370530604408938</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.4319976346396411</v>
+        <v>-6.163529070313156</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0539227375655595</v>
+        <v>-11.39575175159627</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.3482098861916704</v>
+        <v>-1.23420965526558</v>
       </c>
       <c r="T4" t="n">
-        <v>0.6028653451880909</v>
+        <v>-16.14478264679504</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.05295024140513201</v>
+        <v>-16.51875293779776</v>
       </c>
       <c r="V4" t="n">
-        <v>0.08409802812744005</v>
+        <v>-7.536305029284559</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.1338069343081631</v>
+        <v>-20.97968121432941</v>
       </c>
       <c r="X4" t="n">
-        <v>0.06869266744942987</v>
+        <v>-16.3546689063688</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.0889211117885613</v>
+        <v>-24.26319529170434</v>
       </c>
       <c r="Z4" t="n">
-        <v>-0.2954891434065137</v>
+        <v>-29.41382355194741</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.0529253384358061</v>
+        <v>-31.29069855197784</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.1639024861001797</v>
+        <v>-36.49788203024799</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.3896534938395672</v>
+        <v>-53.03119749409934</v>
       </c>
     </row>
     <row r="5">
@@ -793,88 +793,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2755397597929136</v>
+        <v>-0.5429745515566462</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02020560274390648</v>
+        <v>-1.907147413067737</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1636302367015192</v>
+        <v>7.905499311170567</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2131483495799682</v>
+        <v>-11.09177154325076</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.04298345293555438</v>
+        <v>-7.26827331311563</v>
       </c>
       <c r="G5" t="n">
-        <v>0.03909994872113695</v>
+        <v>-3.315373223663929</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.4328309597348151</v>
+        <v>-13.38844145200353</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.02798213060931268</v>
+        <v>0.2039540758508949</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1732792904972661</v>
+        <v>7.914190018704072</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002107870476446408</v>
+        <v>3.255623552035985</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.2516773723386599</v>
+        <v>16.73886608065255</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.2071626542814162</v>
+        <v>12.7294817630945</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1507435573362918</v>
+        <v>-7.588763796178019</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.1862097435440715</v>
+        <v>-7.31327213910574</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.522095852917591</v>
+        <v>-4.935316698190776</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1929454570561554</v>
+        <v>-6.431944139493824</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.1394926122228837</v>
+        <v>-11.72007626584621</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.4977906295085014</v>
+        <v>-1.314255805378605</v>
       </c>
       <c r="T5" t="n">
-        <v>0.4647645797313208</v>
+        <v>-15.72796925759258</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.21909835690207</v>
+        <v>-18.32290296863097</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.05536888803305329</v>
+        <v>-5.990521356331409</v>
       </c>
       <c r="W5" t="n">
-        <v>-0.2996250138667458</v>
+        <v>-20.6133066635805</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.04829613051154613</v>
+        <v>-14.0550277387915</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.06761833012113191</v>
+        <v>-23.99766606839822</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.483464349941329</v>
+        <v>-29.32499457967619</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.1793106393523169</v>
+        <v>-30.48579605173391</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.002855933300165592</v>
+        <v>-37.78510372650722</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.5055431012590547</v>
+        <v>-53.96948521671438</v>
       </c>
     </row>
     <row r="6">
@@ -882,88 +882,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.06229364648510502</v>
+        <v>-1.073598996755198</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2155466801626512</v>
+        <v>-2.115623866512848</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2937552407794119</v>
+        <v>3.526017737593814</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4184141194386462</v>
+        <v>-11.72149363694911</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1889690937921605</v>
+        <v>-4.575912535234156</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1690059659281926</v>
+        <v>-4.521514667102897</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.1745779551957745</v>
+        <v>-12.08755308252102</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1695542585785219</v>
+        <v>-1.296319510479982</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4508209523167314</v>
+        <v>7.627759666067703</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2279225327117322</v>
+        <v>4.571844691831569</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.05028661221798543</v>
+        <v>15.32272888177511</v>
       </c>
       <c r="M6" t="n">
-        <v>0.05404436368008622</v>
+        <v>13.50073994979975</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3189828779759699</v>
+        <v>-6.822117422162766</v>
       </c>
       <c r="O6" t="n">
-        <v>0.06898158143336369</v>
+        <v>-4.953462020505739</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.3206533004735147</v>
+        <v>-3.013847306722354</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.4284768824192497</v>
+        <v>-4.974567279080247</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0806672545130581</v>
+        <v>-11.20396251754573</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2913250598176858</v>
+        <v>1.304574022894279</v>
       </c>
       <c r="T6" t="n">
-        <v>0.5898911620639612</v>
+        <v>-16.77690036287866</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.1395715762994555</v>
+        <v>-17.34588008284184</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1556043095093901</v>
+        <v>-7.314957841071942</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.1151737934116942</v>
+        <v>-21.4264139595598</v>
       </c>
       <c r="X6" t="n">
-        <v>0.1447795746394536</v>
+        <v>-16.63070443787229</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1171895678359255</v>
+        <v>-22.91160814922423</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.2815396706982</v>
+        <v>-28.35527554478023</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.05582833254581313</v>
+        <v>-30.7576901774996</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.1964147536868055</v>
+        <v>-37.09499468405851</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.3290202432615543</v>
+        <v>-55.2068264028877</v>
       </c>
     </row>
     <row r="7">
@@ -971,88 +971,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.2779561403871773</v>
+        <v>-1.087523666832824</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.07159228784993647</v>
+        <v>-2.539149916955957</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1025901219129765</v>
+        <v>6.179486134219745</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1521195926677382</v>
+        <v>-11.69205347595221</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.08722262078443582</v>
+        <v>-6.512786353641327</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.04611966894174495</v>
+        <v>-6.15082526178726</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.4859125513741203</v>
+        <v>-12.83287523592911</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.07199724798492646</v>
+        <v>0.6290464570105474</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1809844342681897</v>
+        <v>6.836757420075843</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.09490694579708314</v>
+        <v>3.310268337863547</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.3400869088143528</v>
+        <v>16.46279429234692</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.2384872608892503</v>
+        <v>14.28808018590276</v>
       </c>
       <c r="N7" t="n">
-        <v>0.07241091261954585</v>
+        <v>-6.174624918148044</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.2279828030615239</v>
+        <v>-6.193914319411046</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.5648045745600045</v>
+        <v>-4.432347038087235</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2660405306516208</v>
+        <v>-5.339031836287031</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.1510316737775788</v>
+        <v>-9.712828878304435</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.5171676742552055</v>
+        <v>0.5782101881208774</v>
       </c>
       <c r="T7" t="n">
-        <v>0.4301917257075834</v>
+        <v>-15.36616464081365</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.335172073852028</v>
+        <v>-18.78299958208659</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.1434508468947857</v>
+        <v>-7.925757249365137</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.3273933273500909</v>
+        <v>-19.89412215045123</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.1090525321125808</v>
+        <v>-15.70463466475092</v>
       </c>
       <c r="Y7" t="n">
-        <v>-0.1369160123345014</v>
+        <v>-22.10232708259301</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.5003460709219918</v>
+        <v>-30.36817266681993</v>
       </c>
       <c r="AA7" t="n">
-        <v>-0.2635203560586866</v>
+        <v>-29.5832863704983</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.01301777779876495</v>
+        <v>-37.09050088009874</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.6077496474428304</v>
+        <v>-53.34625897288411</v>
       </c>
     </row>
     <row r="8">
@@ -1060,88 +1060,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.359890009932585</v>
+        <v>-3.641622573006717</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1282594223551153</v>
+        <v>-2.12900126241522</v>
       </c>
       <c r="D8" t="n">
-        <v>0.02516427792764719</v>
+        <v>7.163279691192749</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1574837430655942</v>
+        <v>-7.135468866290093</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.09837660600790098</v>
+        <v>-7.704689008577123</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.08805141559323484</v>
+        <v>-4.194524896508128</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.5900661527504997</v>
+        <v>-14.05592443741154</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.09045421600502591</v>
+        <v>-0.3574066867107408</v>
       </c>
       <c r="J8" t="n">
-        <v>0.08848202674088915</v>
+        <v>5.925438770235912</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.09247081812640894</v>
+        <v>4.335126974127458</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.4031012081047426</v>
+        <v>12.6836183114694</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.2854065466496675</v>
+        <v>10.37611453724694</v>
       </c>
       <c r="N8" t="n">
-        <v>0.08364933486245726</v>
+        <v>-6.846003504399961</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.2672705469027565</v>
+        <v>-5.796429283940403</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.5916739239127589</v>
+        <v>-4.83798088958136</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.1141740738081203</v>
+        <v>-7.102074605198542</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1860919615309192</v>
+        <v>-11.56399954035802</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.5862356126249895</v>
+        <v>-0.6784239021190412</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2939346629280241</v>
+        <v>-14.69132981903824</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.4025883059509638</v>
+        <v>-17.35754109112679</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.1493435417272659</v>
+        <v>-9.480372106978752</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.3291004340413889</v>
+        <v>-21.90683987664676</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.1764166395256047</v>
+        <v>-15.67292248391976</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.2366000072175852</v>
+        <v>-25.55161353390026</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.5391848098154289</v>
+        <v>-30.45505905808368</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.3742258088246774</v>
+        <v>-30.50210707585311</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.1451891849314599</v>
+        <v>-35.75691886645139</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.6489950318744643</v>
+        <v>-53.27468525189303</v>
       </c>
     </row>
     <row r="9">
@@ -1149,88 +1149,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0827444524392936</v>
+        <v>-0.469008799770898</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3467144403908005</v>
+        <v>-0.1215279288577285</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4555096867575236</v>
+        <v>6.735522609015954</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5691987997457196</v>
+        <v>-8.24856719086303</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3250315387859855</v>
+        <v>-5.961402250005619</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3536940119661804</v>
+        <v>-7.029823983992267</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.0599508132505831</v>
+        <v>-14.35925005765417</v>
       </c>
       <c r="I9" t="n">
-        <v>0.323840957653984</v>
+        <v>0.4358911300878008</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5411148434132518</v>
+        <v>7.864173085910287</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3577153221877493</v>
+        <v>3.743470526606636</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1947447839416382</v>
+        <v>15.67926011973778</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2153357251536242</v>
+        <v>12.2806199563457</v>
       </c>
       <c r="N9" t="n">
-        <v>0.5434803036474283</v>
+        <v>-6.680354887084606</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1123140753950226</v>
+        <v>-4.457464054912472</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.1365015832242557</v>
+        <v>-3.225687441029581</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.6409588027356733</v>
+        <v>-6.713225499562106</v>
       </c>
       <c r="R9" t="n">
-        <v>0.2328134315198296</v>
+        <v>-12.73490312127528</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.1726716902739748</v>
+        <v>-0.5900597187203074</v>
       </c>
       <c r="T9" t="n">
-        <v>0.7782954476609634</v>
+        <v>-14.20051960605294</v>
       </c>
       <c r="U9" t="n">
-        <v>0.07437036478532805</v>
+        <v>-17.45230079500139</v>
       </c>
       <c r="V9" t="n">
-        <v>0.2538595192938972</v>
+        <v>-4.501457351254346</v>
       </c>
       <c r="W9" t="n">
-        <v>0.1200339468155964</v>
+        <v>-20.84321497597252</v>
       </c>
       <c r="X9" t="n">
-        <v>0.2861779362183506</v>
+        <v>-14.92822216379568</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.2364194357361938</v>
+        <v>-23.46918605518842</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.104382625508777</v>
+        <v>-28.76093498514265</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.1384330223923371</v>
+        <v>-31.26265421115872</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.3560702703301329</v>
+        <v>-36.39032504734379</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.1578906300931349</v>
+        <v>-52.92511420596975</v>
       </c>
     </row>
     <row r="10">
@@ -1238,88 +1238,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2836787483890625</v>
+        <v>-2.080365464378204</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.08906709416811973</v>
+        <v>-1.90707729942429</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07462899514865043</v>
+        <v>4.023061872667309</v>
       </c>
       <c r="E10" t="n">
-        <v>0.216283516176333</v>
+        <v>-10.41570178435389</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.114088582030877</v>
+        <v>-8.727219954383457</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.01047036307374299</v>
+        <v>-2.83719562236254</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.4666366472133018</v>
+        <v>-12.38814932361473</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.05343685510917437</v>
+        <v>-0.6060173421286192</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1438942422666903</v>
+        <v>5.767738540023842</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.02264848393748498</v>
+        <v>1.672794019622382</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.2803806961516316</v>
+        <v>17.91598939122799</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.262705463077208</v>
+        <v>12.67724040355363</v>
       </c>
       <c r="N10" t="n">
-        <v>0.09984532732679932</v>
+        <v>-7.292803488780454</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.2553464420088759</v>
+        <v>-6.171759807130333</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.5067107188879696</v>
+        <v>-5.84851643341989</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.2375806808466881</v>
+        <v>-6.170196315530535</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.2100645694920483</v>
+        <v>-10.59172153935027</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.5235704828516521</v>
+        <v>-1.286585587975646</v>
       </c>
       <c r="T10" t="n">
-        <v>0.3368319897091557</v>
+        <v>-17.46323388142073</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.3019395140606786</v>
+        <v>-18.25495878730424</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.1208846005027912</v>
+        <v>-6.965894922444066</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.305856117472274</v>
+        <v>-21.84572175772603</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.1019468241842721</v>
+        <v>-18.36768470713927</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.1996152931818772</v>
+        <v>-23.03688081070551</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.5267248580507302</v>
+        <v>-28.42885024273507</v>
       </c>
       <c r="AA10" t="n">
-        <v>-0.2806256683048389</v>
+        <v>-28.07001013433978</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.05567344194855323</v>
+        <v>-38.01505237345851</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.6498453985742714</v>
+        <v>-53.83160187051888</v>
       </c>
     </row>
     <row r="11">
@@ -1327,88 +1327,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1648110945095586</v>
+        <v>-0.1361167218341284</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.01773512923479471</v>
+        <v>-2.349945125598151</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1364118213025442</v>
+        <v>5.513238801517774</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2650194641677539</v>
+        <v>-11.72874705317787</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.03350994183826443</v>
+        <v>-6.274310057289685</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.002288127962883135</v>
+        <v>-4.632148106995988</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.418642194473589</v>
+        <v>-11.81772026105496</v>
       </c>
       <c r="I11" t="n">
-        <v>0.04189844966542647</v>
+        <v>-0.839997031347131</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2278253465611985</v>
+        <v>7.47240550580891</v>
       </c>
       <c r="K11" t="n">
-        <v>0.06867790256548231</v>
+        <v>2.505299535104602</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.2009777495733631</v>
+        <v>16.71846071493313</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.2232057915710196</v>
+        <v>13.17896855237374</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1506714291612104</v>
+        <v>-6.720551809843916</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.1329417650246878</v>
+        <v>-6.563113782472557</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.5168054344015153</v>
+        <v>-6.363248297528925</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.2747458715539524</v>
+        <v>-6.427359880421676</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.1315618268109876</v>
+        <v>-11.513231326504</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.4548393024804918</v>
+        <v>-1.921645304521856</v>
       </c>
       <c r="T11" t="n">
-        <v>0.4524341253459579</v>
+        <v>-14.77107448433218</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.2813225554053001</v>
+        <v>-17.23708430482464</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.02392770642619063</v>
+        <v>-6.361845134784749</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.2661123977577672</v>
+        <v>-21.49187943345967</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.04314483065823857</v>
+        <v>-16.01014149161149</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.1041058654664146</v>
+        <v>-22.63695321803819</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.4916898529197187</v>
+        <v>-30.0093366059017</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.1517411328143967</v>
+        <v>-29.07122773655565</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.05522885621054885</v>
+        <v>-38.53271419968799</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.5212367040161245</v>
+        <v>-52.6451091552</v>
       </c>
     </row>
   </sheetData>
@@ -1521,88 +1521,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4323625425424082</v>
+        <v>18.09035783948996</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2364926438739851</v>
+        <v>-7.574573752029489</v>
       </c>
       <c r="D2" t="n">
-        <v>0.31749328302199</v>
+        <v>-3.971308705849237</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2421836128725522</v>
+        <v>3.749968886309238</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2973974501500057</v>
+        <v>-1.910196971052603</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02059192379596256</v>
+        <v>-13.51254108104425</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4591218342816624</v>
+        <v>3.506309586628578</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1070439776879443</v>
+        <v>-20.79024072154307</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2100833938504235</v>
+        <v>-17.57367864959065</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.0357092802208438</v>
+        <v>-3.189376465185704</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3183499752156708</v>
+        <v>0.9753755475010712</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.0605706949949005</v>
+        <v>-5.991652528988276</v>
       </c>
       <c r="N2" t="n">
-        <v>0.346254212785457</v>
+        <v>-2.411925080305639</v>
       </c>
       <c r="O2" t="n">
-        <v>0.5345209208388559</v>
+        <v>-1.380797086968166</v>
       </c>
       <c r="P2" t="n">
-        <v>0.07498183050379688</v>
+        <v>3.243807476820508</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.2390863838447587</v>
+        <v>-4.91913646837151</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.02008927860718923</v>
+        <v>-10.80249251230266</v>
       </c>
       <c r="S2" t="n">
-        <v>0.003989872507379089</v>
+        <v>2.540598671141096</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1920184676194222</v>
+        <v>-9.568009608949712</v>
       </c>
       <c r="U2" t="n">
-        <v>0.4180005975996813</v>
+        <v>0.6872512751907638</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1322666242047839</v>
+        <v>-5.287375586005513</v>
       </c>
       <c r="W2" t="n">
-        <v>0.4607927615281203</v>
+        <v>-9.310085586312773</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04076887029481145</v>
+        <v>-5.494719952613302</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.05589327023820061</v>
+        <v>-3.197462258193638</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.07760961616726178</v>
+        <v>13.61456451492145</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.4428636562884553</v>
+        <v>-0.7684429048442256</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.1487539468539701</v>
+        <v>7.625931949875342</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.1407852464776991</v>
+        <v>-13.96191155022901</v>
       </c>
     </row>
     <row r="3">
@@ -1610,88 +1610,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.1580063773342444</v>
+        <v>18.4275624159164</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.326516239689534</v>
+        <v>-7.980532244518947</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.205234897584389</v>
+        <v>-5.048261751771806</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.3162996529743848</v>
+        <v>4.438889238237997</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2214984097419378</v>
+        <v>-3.512504317599351</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.5734167385037144</v>
+        <v>-16.70872758107307</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.03314195291498301</v>
+        <v>1.558129307951976</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.3872572882137378</v>
+        <v>-19.28215179376657</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.3101852557825238</v>
+        <v>-20.55900538763284</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.5050413998373027</v>
+        <v>-2.744776773067609</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.2091875994002373</v>
+        <v>0.8033988523865818</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.5681761101263332</v>
+        <v>-5.725335759733898</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.1679385764056638</v>
+        <v>-4.540925844589511</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0436099693410823</v>
+        <v>0.3481166177452195</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.3793631055058408</v>
+        <v>1.221004696279663</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.782951818498735</v>
+        <v>-5.62119624506836</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.476349601880269</v>
+        <v>-10.21089775750867</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.4555167779566154</v>
+        <v>1.400511705517468</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.3027750064760111</v>
+        <v>-8.007337948027942</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.04103788781291429</v>
+        <v>1.531361832826273</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.3152513431499023</v>
+        <v>-7.345168339539679</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.05260458593174117</v>
+        <v>-11.63954658748583</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.4497716297886646</v>
+        <v>-3.899057106667333</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.4873777263181943</v>
+        <v>-2.201712314616215</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.3652850880329593</v>
+        <v>15.26195019931927</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.03226838847119878</v>
+        <v>-0.5164229851871598</v>
       </c>
       <c r="AB3" t="n">
-        <v>-0.3129282462924164</v>
+        <v>4.602895639801431</v>
       </c>
       <c r="AC3" t="n">
-        <v>-0.6588024105568115</v>
+        <v>-15.58925355648864</v>
       </c>
     </row>
     <row r="4">
@@ -1699,88 +1699,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2360848525010269</v>
+        <v>18.23352649795185</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05972762498251849</v>
+        <v>-8.035318142607101</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1480978192990511</v>
+        <v>-2.858965818053119</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1083257030564238</v>
+        <v>3.470267712009265</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2083934574370783</v>
+        <v>-2.776720668844645</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.136912875968036</v>
+        <v>-14.38145822788996</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3681410915209196</v>
+        <v>3.408941575653318</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02009098907924351</v>
+        <v>-20.42744968004643</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09378600412707833</v>
+        <v>-20.35952349386834</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.1835612552155978</v>
+        <v>-5.107111300313607</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1556261506477001</v>
+        <v>-0.7447743638399709</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.132997735635336</v>
+        <v>-8.483059343605724</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2165945136996924</v>
+        <v>-4.610434900243037</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4682296329290344</v>
+        <v>-0.5397915753674927</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.02938258648495144</v>
+        <v>1.419432126036976</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.4292074231055563</v>
+        <v>-5.205415541159568</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0808796775321997</v>
+        <v>-9.791737111820172</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.1010052643540177</v>
+        <v>1.941701660103416</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1206233791043747</v>
+        <v>-8.47560736245363</v>
       </c>
       <c r="U4" t="n">
-        <v>0.3019671951080208</v>
+        <v>3.520830109519716</v>
       </c>
       <c r="V4" t="n">
-        <v>0.03187705652822176</v>
+        <v>-7.106882944097684</v>
       </c>
       <c r="W4" t="n">
-        <v>0.3240416064403014</v>
+        <v>-10.15768330591325</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.09679261914135628</v>
+        <v>-4.973940996364544</v>
       </c>
       <c r="Y4" t="n">
-        <v>-0.07942508786257224</v>
+        <v>-3.496039517431503</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.05129003621693753</v>
+        <v>14.69142479176936</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.4391150098734163</v>
+        <v>-1.388361879102415</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.01565281788076155</v>
+        <v>4.314078173670611</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.1682284475116885</v>
+        <v>-15.6641561893458</v>
       </c>
     </row>
     <row r="5">
@@ -1788,88 +1788,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1158594556242519</v>
+        <v>16.74824878055296</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.140873588514621</v>
+        <v>-8.492725661068999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09415760131450185</v>
+        <v>-1.635892768305034</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.04132648655036435</v>
+        <v>2.960242945020367</v>
       </c>
       <c r="F5" t="n">
-        <v>0.054644950545094</v>
+        <v>-2.571103187473979</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.3005536643112873</v>
+        <v>-13.92781360745312</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1967966250035018</v>
+        <v>0.1654592658020624</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.1240197991878646</v>
+        <v>-18.85186924589374</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.005357710515914493</v>
+        <v>-17.73545839215408</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.2343125042394491</v>
+        <v>-4.541625847341345</v>
       </c>
       <c r="L5" t="n">
-        <v>0.07643845146555711</v>
+        <v>0.3093604562131307</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.3033542863294209</v>
+        <v>-6.071370914845081</v>
       </c>
       <c r="N5" t="n">
-        <v>0.09468850349621058</v>
+        <v>-4.815600973864653</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2767248888341736</v>
+        <v>0.648137119660757</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1709809124928905</v>
+        <v>2.075472845400615</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.4617528954640856</v>
+        <v>-4.634159287251769</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.2170499646179997</v>
+        <v>-9.593433320518313</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.2760520869726396</v>
+        <v>3.02451871712874</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.02738224809442304</v>
+        <v>-10.43168587258605</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2156034630035929</v>
+        <v>-1.231822178536718</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.04868707069896857</v>
+        <v>-6.243332422082724</v>
       </c>
       <c r="W5" t="n">
-        <v>0.2371761543686915</v>
+        <v>-11.11698676702065</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.2386549692430298</v>
+        <v>-7.024427682695825</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.228497175257985</v>
+        <v>-3.753213486751616</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.08428078539631927</v>
+        <v>13.73796377622137</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.2335805344140996</v>
+        <v>-0.8573603035361135</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.04686731207007658</v>
+        <v>4.17797802298842</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.329322626858404</v>
+        <v>-12.89907689256381</v>
       </c>
     </row>
     <row r="6">
@@ -1877,88 +1877,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3251133806509991</v>
+        <v>18.4401846518541</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1410961399593962</v>
+        <v>-6.150587008608293</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2028440168775889</v>
+        <v>-3.924958097387672</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1938355961812475</v>
+        <v>3.766617717812798</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2057177939274193</v>
+        <v>-3.234672552232434</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1358227922043928</v>
+        <v>-15.07776567605433</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4472401471739749</v>
+        <v>3.456250992684136</v>
       </c>
       <c r="I6" t="n">
-        <v>0.04012577517924418</v>
+        <v>-20.23267781255048</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1487099610339731</v>
+        <v>-19.52335523172497</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.1002557789453868</v>
+        <v>-3.547447395729943</v>
       </c>
       <c r="L6" t="n">
-        <v>0.2043753302547796</v>
+        <v>1.765053511039139</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0862317630581359</v>
+        <v>-6.156080600940907</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3115311542847855</v>
+        <v>-2.934395947056335</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4898997969286941</v>
+        <v>-0.337270924805789</v>
       </c>
       <c r="P6" t="n">
-        <v>0.06507626422765356</v>
+        <v>1.491518503012746</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.3017937911783269</v>
+        <v>-7.108608720298049</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.04338070655427601</v>
+        <v>-9.156337668644035</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.05019571640107479</v>
+        <v>3.838896899643307</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1385817128120425</v>
+        <v>-7.581885959570799</v>
       </c>
       <c r="U6" t="n">
-        <v>0.3752406753329572</v>
+        <v>0.8524986813955251</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1159876678461407</v>
+        <v>-7.563215938437746</v>
       </c>
       <c r="W6" t="n">
-        <v>0.3615871619091586</v>
+        <v>-11.9098593723729</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.08305454473382798</v>
+        <v>-5.465884469499989</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.0005031564660129412</v>
+        <v>-3.093702025499964</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.1265779674626223</v>
+        <v>12.73787021212637</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.4616209551430031</v>
+        <v>0.3827529485764076</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.1089851926548108</v>
+        <v>4.947488522940082</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.1736168532845821</v>
+        <v>-13.04264888814803</v>
       </c>
     </row>
     <row r="7">
@@ -1966,88 +1966,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1502992789914552</v>
+        <v>18.06117833311864</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1091895846026067</v>
+        <v>-8.408198491391103</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.06387982685036597</v>
+        <v>-6.159417579528711</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.08424559243117406</v>
+        <v>2.923393891631036</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.02670482006262612</v>
+        <v>-2.783872803658633</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.3834123444381964</v>
+        <v>-14.74545104782752</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1767526646654984</v>
+        <v>1.545447635041748</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.2153040568502229</v>
+        <v>-21.01020852996496</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.08941242376873451</v>
+        <v>-19.19117798882987</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.3077053420110479</v>
+        <v>-3.501276163988181</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.01006741761798739</v>
+        <v>3.155630785915084</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.3121621838472639</v>
+        <v>-6.902757443293874</v>
       </c>
       <c r="N7" t="n">
-        <v>0.05308391921556734</v>
+        <v>-2.574972608017441</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2440520199234487</v>
+        <v>-0.2656109178575035</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.231815104110949</v>
+        <v>4.431589926570801</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.5427667538224523</v>
+        <v>-4.251344794941256</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.2790964728827383</v>
+        <v>-9.224125455733265</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.3184257595762851</v>
+        <v>2.470427075940603</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.08220807040788614</v>
+        <v>-9.895353367083001</v>
       </c>
       <c r="U7" t="n">
-        <v>0.1121713164934742</v>
+        <v>1.465018456585525</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.1369028594982685</v>
+        <v>-7.261393535840777</v>
       </c>
       <c r="W7" t="n">
-        <v>0.106898308293289</v>
+        <v>-9.873014893168939</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.2656560450320251</v>
+        <v>-5.554877043626924</v>
       </c>
       <c r="Y7" t="n">
-        <v>-0.2603349533570768</v>
+        <v>-3.700949458856035</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.09963287472265653</v>
+        <v>13.52987950596424</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.2590776361262299</v>
+        <v>-1.071404630901701</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.1386485141690856</v>
+        <v>4.59532044427843</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.4853434353977439</v>
+        <v>-13.98868896652222</v>
       </c>
     </row>
     <row r="8">
@@ -2055,88 +2055,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.01653975461887455</v>
+        <v>14.46545461348884</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2113801930475209</v>
+        <v>-8.79909200947262</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.04434229496782605</v>
+        <v>-4.180164659267599</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1225219625051831</v>
+        <v>4.522378902259005</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.09301881962769816</v>
+        <v>-3.557531608685616</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.3838447195498401</v>
+        <v>-15.35717753823863</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1051940330002439</v>
+        <v>1.292585346167598</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.2579967855087966</v>
+        <v>-23.19667014036774</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1450771271139525</v>
+        <v>-19.76720161514999</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.3605142953920428</v>
+        <v>-3.380960565534672</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.08176513372180216</v>
+        <v>0.7429976963933389</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.3370551988788137</v>
+        <v>-5.701349594812908</v>
       </c>
       <c r="N8" t="n">
-        <v>0.01317694210629541</v>
+        <v>-4.016779093079797</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1593366725649858</v>
+        <v>0.8096796638140784</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.2627560198367496</v>
+        <v>2.250026583761316</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.6122770153979928</v>
+        <v>-5.87143080077413</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.2976187969552047</v>
+        <v>-9.793690355868247</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.3739962607011009</v>
+        <v>0.7757422195845414</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.1835552661499947</v>
+        <v>-8.763227521990894</v>
       </c>
       <c r="U8" t="n">
-        <v>0.07958293954525669</v>
+        <v>1.013876613464367</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.1731977547245053</v>
+        <v>-6.580179954455257</v>
       </c>
       <c r="W8" t="n">
-        <v>0.05025856995535188</v>
+        <v>-10.8433298769826</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.2885699572418901</v>
+        <v>-5.149002375238927</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.2542981986347077</v>
+        <v>-2.88054145963446</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.2101936571187094</v>
+        <v>11.88410578825684</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1047282408054542</v>
+        <v>0.6011017056205619</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.1810859333970486</v>
+        <v>3.422149956519359</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.5011689578969256</v>
+        <v>-15.77374895441607</v>
       </c>
     </row>
     <row r="9">
@@ -2144,88 +2144,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4843028125970132</v>
+        <v>17.34309386404055</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2352772468429261</v>
+        <v>-10.1879629740546</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3845138182259883</v>
+        <v>-3.048813949778206</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2926762942539219</v>
+        <v>4.351995728710372</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3730472740766178</v>
+        <v>-1.794783157429226</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04717297117177824</v>
+        <v>-13.97176006582244</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5849083310020076</v>
+        <v>2.949519352447306</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2119660292919504</v>
+        <v>-19.32613876171793</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3330737991391661</v>
+        <v>-17.82339642374711</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0606253697476391</v>
+        <v>-3.261762399869323</v>
       </c>
       <c r="L9" t="n">
-        <v>0.3740645994926818</v>
+        <v>-0.24647128397533</v>
       </c>
       <c r="M9" t="n">
-        <v>0.05421620319885159</v>
+        <v>-6.555383926371476</v>
       </c>
       <c r="N9" t="n">
-        <v>0.3836511366237398</v>
+        <v>-5.250840221259693</v>
       </c>
       <c r="O9" t="n">
-        <v>0.6958976596673543</v>
+        <v>0.9194265532273465</v>
       </c>
       <c r="P9" t="n">
-        <v>0.1976059974876656</v>
+        <v>1.955633960221289</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.1894576861360993</v>
+        <v>-4.124096880647417</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1173252605740446</v>
+        <v>-9.585289446091629</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1325857172616811</v>
+        <v>2.594304933755851</v>
       </c>
       <c r="T9" t="n">
-        <v>0.2649219543543712</v>
+        <v>-10.75024937324942</v>
       </c>
       <c r="U9" t="n">
-        <v>0.5409465759019645</v>
+        <v>3.4572053456851</v>
       </c>
       <c r="V9" t="n">
-        <v>0.3160720698473556</v>
+        <v>-5.412579535193903</v>
       </c>
       <c r="W9" t="n">
-        <v>0.5983146359315312</v>
+        <v>-10.46583974295816</v>
       </c>
       <c r="X9" t="n">
-        <v>0.09553555527003849</v>
+        <v>-3.937830426850174</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.2372055156470285</v>
+        <v>-1.473525862779714</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.2945698736254646</v>
+        <v>15.17519763217135</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.6230100172536871</v>
+        <v>0.6701579828637394</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.2231959392615734</v>
+        <v>5.195131980509358</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.01937108581461217</v>
+        <v>-12.73183277306354</v>
       </c>
     </row>
     <row r="10">
@@ -2233,88 +2233,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.06703682325250039</v>
+        <v>18.88246445693753</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.1216793554753312</v>
+        <v>-10.53983468770544</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02678344193854455</v>
+        <v>-6.218369579543585</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.08214677255259693</v>
+        <v>4.320303276887742</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0783732190132902</v>
+        <v>-2.671644800466535</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.3827304547550826</v>
+        <v>-13.61845552953149</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1415260896560968</v>
+        <v>2.337340272206443</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.2065394505933557</v>
+        <v>-20.45544284217544</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.1023176611819251</v>
+        <v>-17.91074860348461</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.3124273688405318</v>
+        <v>-5.435375523242164</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.03286957998852962</v>
+        <v>0.2428245534378091</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.3698551665887995</v>
+        <v>-7.334362011457928</v>
       </c>
       <c r="N10" t="n">
-        <v>0.01776934934017825</v>
+        <v>-4.194095086798195</v>
       </c>
       <c r="O10" t="n">
-        <v>0.2305737171848475</v>
+        <v>0.1262741435411319</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.1849407779928753</v>
+        <v>1.924387723579986</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.5771587192820777</v>
+        <v>-3.245067060336284</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.2809683941216308</v>
+        <v>-8.415493670390351</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.2907742222526582</v>
+        <v>1.702050414269175</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.2008230613363544</v>
+        <v>-9.373913261778794</v>
       </c>
       <c r="U10" t="n">
-        <v>0.1743865219992618</v>
+        <v>1.569027089378332</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.08634777245199871</v>
+        <v>-6.070520006175636</v>
       </c>
       <c r="W10" t="n">
-        <v>0.1132123011644434</v>
+        <v>-10.03862928418067</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.2870782709265208</v>
+        <v>-4.37727945013542</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.2126467832828092</v>
+        <v>-3.373936862306573</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.1768299452553387</v>
+        <v>14.20784948955467</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.2126801543965904</v>
+        <v>-0.973573076573599</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.1084585000405304</v>
+        <v>5.044517136517763</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.4159697250773412</v>
+        <v>-14.18833798152048</v>
       </c>
     </row>
     <row r="11">
@@ -2322,88 +2322,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.16893532774505</v>
+        <v>14.39526934208785</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.08873202628727149</v>
+        <v>-6.970670747275994</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01418064930810664</v>
+        <v>-4.023757878161371</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.04922592887847112</v>
+        <v>2.745578194932317</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02685319538757758</v>
+        <v>-3.277047007142355</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.2881229621148617</v>
+        <v>-14.01941111081195</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2096790196524861</v>
+        <v>2.191424304184737</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.1419813390206049</v>
+        <v>-20.36257599291497</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.04385527231052463</v>
+        <v>-20.62332079988082</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.2784850953987107</v>
+        <v>-2.946206705165964</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.005667774715472876</v>
+        <v>-0.1914215563262407</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.3006551113644394</v>
+        <v>-6.677325763711103</v>
       </c>
       <c r="N11" t="n">
-        <v>0.06254522615911051</v>
+        <v>-4.728844610780051</v>
       </c>
       <c r="O11" t="n">
-        <v>0.2936020683534467</v>
+        <v>-0.3556223103348304</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.1211374392786692</v>
+        <v>1.477631447900896</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.4814767836105713</v>
+        <v>-5.711796545685422</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.2199511954081074</v>
+        <v>-10.09359591570766</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.1997804986056002</v>
+        <v>1.595580855035731</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.03902681529720523</v>
+        <v>-9.223945395925874</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1704383683519107</v>
+        <v>1.934153584457774</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.06823008339161313</v>
+        <v>-6.452304236101971</v>
       </c>
       <c r="W11" t="n">
-        <v>0.2162118860519115</v>
+        <v>-12.14759258267853</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.2214142194526816</v>
+        <v>-4.223342938054854</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.1237144339844321</v>
+        <v>-2.350766848609481</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.1044837672976005</v>
+        <v>12.90649797236187</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.271567823724952</v>
+        <v>-0.8837959196796081</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.1182645681048012</v>
+        <v>4.72300243636633</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.3602964380185348</v>
+        <v>-12.72557155931403</v>
       </c>
     </row>
   </sheetData>
@@ -2516,88 +2516,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.0836490153223382</v>
+        <v>-5.625236089776784</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1702754522732</v>
+        <v>-4.492804866806801</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2175293448940886</v>
+        <v>-4.713966740853254</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8681772298197454</v>
+        <v>1.203317352989799</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1855255218392848</v>
+        <v>-14.06284944644749</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1275813516851332</v>
+        <v>-12.78727537594284</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5503218754700492</v>
+        <v>2.814965286016304</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.07018684364608241</v>
+        <v>-2.53913221659873</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.07063335710341934</v>
+        <v>-8.563753893333859</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2654160219764454</v>
+        <v>1.488950011511102</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3966499175497741</v>
+        <v>-11.38646500702958</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2490075408982866</v>
+        <v>4.423955762620237</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2202495238464355</v>
+        <v>-8.128517429177702</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2817462752340703</v>
+        <v>-5.240345259732992</v>
       </c>
       <c r="P2" t="n">
-        <v>0.3717564948070879</v>
+        <v>-13.03817715404549</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.05739848125195671</v>
+        <v>-13.78024308438627</v>
       </c>
       <c r="R2" t="n">
-        <v>0.2769355823926236</v>
+        <v>-0.7503579798194071</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1497733082613833</v>
+        <v>-11.78761853554003</v>
       </c>
       <c r="T2" t="n">
-        <v>0.3174847329221144</v>
+        <v>-12.22987088733476</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1199673959434955</v>
+        <v>6.38124098023076</v>
       </c>
       <c r="V2" t="n">
-        <v>0.04232593373764701</v>
+        <v>-9.971296061096416</v>
       </c>
       <c r="W2" t="n">
-        <v>0.2698233280816511</v>
+        <v>-7.901048654200913</v>
       </c>
       <c r="X2" t="n">
-        <v>0.3859732542516097</v>
+        <v>-16.3878612140004</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.2086762686973305</v>
+        <v>-1.828921386879244</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.3295964537394078</v>
+        <v>-6.595812862720742</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.2258879346417491</v>
+        <v>-27.39268680411794</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.04304736684997726</v>
+        <v>-6.291168289940297</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.07405912276978922</v>
+        <v>-19.80186137763567</v>
       </c>
     </row>
     <row r="3">
@@ -2605,88 +2605,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.597542859273431</v>
+        <v>-6.818883773261904</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.3303937800487278</v>
+        <v>-5.372510623441075</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.7003455063937408</v>
+        <v>-2.368929407152529</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3938599150679961</v>
+        <v>0.5252353418916407</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2312200327440471</v>
+        <v>-15.00014171096014</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.4119213619378312</v>
+        <v>-11.20677851816033</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03391056893031685</v>
+        <v>3.272069460222101</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.6394609130152547</v>
+        <v>-3.390386788649379</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.5426572164610249</v>
+        <v>-9.661424112147625</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.1850416863678678</v>
+        <v>3.563205879808467</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.1197940816484936</v>
+        <v>-10.48280988227735</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.1884243782399544</v>
+        <v>4.051915199238149</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.4065230133277179</v>
+        <v>-9.114230651989303</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.2245408677091177</v>
+        <v>-6.436374722914955</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.2491517065142936</v>
+        <v>-13.2941314263707</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.5730692014895402</v>
+        <v>-13.10836807070307</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.239140984703495</v>
+        <v>-1.053363912535194</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.31343217142511</v>
+        <v>-12.18358353125703</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.159002166239661</v>
+        <v>-11.75816231033135</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.3859057392167934</v>
+        <v>3.948180534477614</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.3839895401255203</v>
+        <v>-11.24216040821767</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.2389878185390276</v>
+        <v>-6.205397729379446</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.1462325255393674</v>
+        <v>-15.35892040533156</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.2583388925119958</v>
+        <v>-3.221889975387329</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.7077926482871693</v>
+        <v>-7.58937915628077</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.7143641899443722</v>
+        <v>-26.61643965109187</v>
       </c>
       <c r="AB3" t="n">
-        <v>-0.5118035778477592</v>
+        <v>-9.798801387419182</v>
       </c>
       <c r="AC3" t="n">
-        <v>-0.6368434801035104</v>
+        <v>-18.33582224848669</v>
       </c>
     </row>
     <row r="4">
@@ -2694,88 +2694,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2273685482071319</v>
+        <v>-6.577149976098827</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1162889715736217</v>
+        <v>-4.84254589086262</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.3258674717941589</v>
+        <v>-4.126286625305527</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7315354121062806</v>
+        <v>1.426689940638771</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02369697531489623</v>
+        <v>-13.01651984368936</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05431460110441469</v>
+        <v>-9.920468128188951</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4738771060505926</v>
+        <v>2.707003519207431</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.1848885981304575</v>
+        <v>-2.281426627988874</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1731286524790598</v>
+        <v>-10.68827321018486</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2071362159482329</v>
+        <v>3.109659809836429</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2531648686860086</v>
+        <v>-7.814209627484809</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1489756518819478</v>
+        <v>3.339333410705613</v>
       </c>
       <c r="N4" t="n">
-        <v>0.05824139458790273</v>
+        <v>-7.861108158834494</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1581983054526348</v>
+        <v>-4.824517096675294</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1901299657843637</v>
+        <v>-11.46419735514247</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.1788123488246608</v>
+        <v>-13.30110365178605</v>
       </c>
       <c r="R4" t="n">
-        <v>0.163113053872437</v>
+        <v>0.1951328909401382</v>
       </c>
       <c r="S4" t="n">
-        <v>0.1121805318134987</v>
+        <v>-12.26144680907025</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2404581244536838</v>
+        <v>-11.96877888669006</v>
       </c>
       <c r="U4" t="n">
-        <v>0.05288241813284251</v>
+        <v>7.239012983944118</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.04059022842761201</v>
+        <v>-10.99581300095454</v>
       </c>
       <c r="W4" t="n">
-        <v>0.1511714595688049</v>
+        <v>-6.517114725015108</v>
       </c>
       <c r="X4" t="n">
-        <v>0.3118353783026051</v>
+        <v>-17.53393828335611</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.135300767815582</v>
+        <v>-4.565812851299319</v>
       </c>
       <c r="Z4" t="n">
-        <v>-0.3619246301502732</v>
+        <v>-6.187734418891328</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.3276866639974815</v>
+        <v>-25.40702851653849</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.1105661750638466</v>
+        <v>-8.221784165018422</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.1514537522011792</v>
+        <v>-19.53115493713051</v>
       </c>
     </row>
     <row r="5">
@@ -2783,88 +2783,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3460208671243349</v>
+        <v>-7.936111302687825</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.06483974488485796</v>
+        <v>-4.895449169464842</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4472886910021247</v>
+        <v>-3.263112850524579</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6195915488988067</v>
+        <v>1.355114777011556</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1128427286360151</v>
+        <v>-12.81354458248061</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.07829360776621039</v>
+        <v>-11.67688882982877</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3533468419810279</v>
+        <v>2.090104280098602</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.3528664167418734</v>
+        <v>-2.921948632120482</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.3029880757053983</v>
+        <v>-9.265923187073209</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0515683673314396</v>
+        <v>2.396944602740177</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1662279449471631</v>
+        <v>-7.886432883505679</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.007743174334657377</v>
+        <v>2.281685840803264</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.05722655661166236</v>
+        <v>-8.441932340827353</v>
       </c>
       <c r="O5" t="n">
-        <v>0.04087840526969778</v>
+        <v>-6.186082268700011</v>
       </c>
       <c r="P5" t="n">
-        <v>0.03101108865642922</v>
+        <v>-12.23152380444628</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.361011513432502</v>
+        <v>-12.50049947678504</v>
       </c>
       <c r="R5" t="n">
-        <v>0.05565844632793751</v>
+        <v>-0.6535831533651897</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.1241597587056887</v>
+        <v>-12.30761874478687</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0053336505554131</v>
+        <v>-12.1831014301878</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.096376553242775</v>
+        <v>3.975848884848237</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.1227584011754538</v>
+        <v>-10.61156376686587</v>
       </c>
       <c r="W5" t="n">
-        <v>0.04495812476370054</v>
+        <v>-7.658041451829229</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1392247745689945</v>
+        <v>-16.44785058316933</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.02908898666209775</v>
+        <v>-1.221050464013117</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.4717005449683173</v>
+        <v>-8.836200761572334</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.4241530776453925</v>
+        <v>-27.68346271763291</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.2596846194753147</v>
+        <v>-8.664621425219382</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.3304159753932179</v>
+        <v>-19.08343402808148</v>
       </c>
     </row>
     <row r="6">
@@ -2872,88 +2872,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1514784905003357</v>
+        <v>-7.08567176177534</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1235936977705012</v>
+        <v>-2.649540344830688</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2207318311025004</v>
+        <v>-2.255586109612517</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8342947466764884</v>
+        <v>0.725118117428257</v>
       </c>
       <c r="F6" t="n">
-        <v>0.09683992226760779</v>
+        <v>-13.21249038820341</v>
       </c>
       <c r="G6" t="n">
-        <v>0.09259903696178054</v>
+        <v>-11.66417873205729</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5130582072019726</v>
+        <v>0.8273670033958274</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.1576484347334996</v>
+        <v>-2.786073701134428</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.09881579514776531</v>
+        <v>-9.543148242840068</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2904788160350755</v>
+        <v>2.529770891546195</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3320532730103765</v>
+        <v>-10.3836400872925</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2080857930372405</v>
+        <v>4.875378230872986</v>
       </c>
       <c r="N6" t="n">
-        <v>0.09204537482553035</v>
+        <v>-9.430572262807392</v>
       </c>
       <c r="O6" t="n">
-        <v>0.2207307365656062</v>
+        <v>-5.455606548103056</v>
       </c>
       <c r="P6" t="n">
-        <v>0.2509220885769358</v>
+        <v>-10.55460815651818</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.03291636254283559</v>
+        <v>-13.44564667120729</v>
       </c>
       <c r="R6" t="n">
-        <v>0.2350820140338048</v>
+        <v>0.1601442658475829</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1107623417632019</v>
+        <v>-11.85373722064415</v>
       </c>
       <c r="T6" t="n">
-        <v>0.2992361857855237</v>
+        <v>-13.56888587427268</v>
       </c>
       <c r="U6" t="n">
-        <v>0.09441674620973246</v>
+        <v>3.317018701188685</v>
       </c>
       <c r="V6" t="n">
-        <v>0.01254716136408825</v>
+        <v>-10.21551454103358</v>
       </c>
       <c r="W6" t="n">
-        <v>0.2439885048780822</v>
+        <v>-6.379514119553577</v>
       </c>
       <c r="X6" t="n">
-        <v>0.283077771641632</v>
+        <v>-16.91442713884609</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1970830093495021</v>
+        <v>-3.436446022981291</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.3182322514334271</v>
+        <v>-6.828959019404071</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.2283092891918764</v>
+        <v>-26.0516026812103</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.05680097615126538</v>
+        <v>-7.382764177251795</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.1419545132575538</v>
+        <v>-20.49449588931284</v>
       </c>
     </row>
     <row r="7">
@@ -2961,88 +2961,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.4351872243081327</v>
+        <v>-8.615125846761462</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1097936208746585</v>
+        <v>-6.155545757761051</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.530630071568174</v>
+        <v>-4.057473078151852</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6499756656287876</v>
+        <v>2.829511413657539</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1298081352711124</v>
+        <v>-15.36436145665334</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.1601480378097979</v>
+        <v>-12.14151816072064</v>
       </c>
       <c r="H7" t="n">
-        <v>0.296892513996602</v>
+        <v>1.737221146982148</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.3459756352660875</v>
+        <v>-3.56499233540253</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.3750313451645989</v>
+        <v>-9.112759131834185</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01382652302617482</v>
+        <v>3.057691617038121</v>
       </c>
       <c r="L7" t="n">
-        <v>0.01970373644658341</v>
+        <v>-12.58360150463224</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.07136395382698049</v>
+        <v>2.700168831503466</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.2005248734194253</v>
+        <v>-7.914273274860168</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.06194186139923724</v>
+        <v>-5.062212063698671</v>
       </c>
       <c r="P7" t="n">
-        <v>0.02885857960630756</v>
+        <v>-12.21032190345417</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.3616186901766025</v>
+        <v>-13.45606897253007</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.01839407076774301</v>
+        <v>-1.161635980390625</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.1355908174013324</v>
+        <v>-12.70362659622453</v>
       </c>
       <c r="T7" t="n">
-        <v>0.05217865081030518</v>
+        <v>-14.9953192344393</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.1690567657298254</v>
+        <v>6.923646561016074</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.2270955988969068</v>
+        <v>-12.6267630920654</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.01897668020444834</v>
+        <v>-5.771769279628653</v>
       </c>
       <c r="X7" t="n">
-        <v>0.1277739233781237</v>
+        <v>-16.63329244777516</v>
       </c>
       <c r="Y7" t="n">
-        <v>-0.08058995432754447</v>
+        <v>-3.210379950150933</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.5337797581291235</v>
+        <v>-5.905990818943131</v>
       </c>
       <c r="AA7" t="n">
-        <v>-0.5498344768020442</v>
+        <v>-27.47546556318177</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.3345124719572456</v>
+        <v>-9.046575940021771</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.3748614188662277</v>
+        <v>-20.21670086955524</v>
       </c>
     </row>
     <row r="8">
@@ -3050,88 +3050,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.4619457861997067</v>
+        <v>-8.299926586843922</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1796725852208872</v>
+        <v>-6.827812898721437</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.588880939636475</v>
+        <v>-2.032454541942204</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5539493830703603</v>
+        <v>-0.2974517181959255</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2107508031693251</v>
+        <v>-12.84065354440332</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2018296373607582</v>
+        <v>-13.99021736801504</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2458907231475366</v>
+        <v>2.158945582377878</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.4520493467996762</v>
+        <v>-2.013872113900789</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.383186671870977</v>
+        <v>-9.937641874022187</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.004899137522677871</v>
+        <v>1.582005331774441</v>
       </c>
       <c r="L8" t="n">
-        <v>0.05236510810212278</v>
+        <v>-9.329658394848437</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.05019577499426056</v>
+        <v>4.333857759329925</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.2288032194425094</v>
+        <v>-8.523535336970319</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.07312775620906244</v>
+        <v>-5.934677989867392</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.07898641311078515</v>
+        <v>-11.66751092705597</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.3948400841162835</v>
+        <v>-12.87920393085149</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.01730074811095422</v>
+        <v>-0.4664457940986719</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.1531434700532965</v>
+        <v>-10.80277033875112</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.01405047096089829</v>
+        <v>-13.25958454342712</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.1676403971093086</v>
+        <v>6.225404415846988</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.2574995829571067</v>
+        <v>-9.958539160250584</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.02327644999800135</v>
+        <v>-6.249972697109444</v>
       </c>
       <c r="X8" t="n">
-        <v>0.04551280696674997</v>
+        <v>-18.52617701423971</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.1345968728394483</v>
+        <v>-2.545551244676546</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.6865792637464259</v>
+        <v>-6.318911461166802</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.5759311814496684</v>
+        <v>-27.18173510509245</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.4494863108466124</v>
+        <v>-8.717540819089944</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.4119960930953472</v>
+        <v>-19.43647621383438</v>
       </c>
     </row>
     <row r="9">
@@ -3139,88 +3139,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.01111083907072019</v>
+        <v>-5.159724254257917</v>
       </c>
       <c r="C9" t="n">
-        <v>0.274131460400054</v>
+        <v>-3.608080989648451</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.08755580967276194</v>
+        <v>-4.546301305201446</v>
       </c>
       <c r="E9" t="n">
-        <v>1.019478405225722</v>
+        <v>0.5956319669226717</v>
       </c>
       <c r="F9" t="n">
-        <v>0.213206372248405</v>
+        <v>-14.40655854851215</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2398284208792507</v>
+        <v>-11.75613910617066</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6714129736461592</v>
+        <v>2.293709898305701</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.003268082180971077</v>
+        <v>-2.019216740271562</v>
       </c>
       <c r="J9" t="n">
-        <v>0.04245851381947363</v>
+        <v>-9.293637565311618</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4248111594940613</v>
+        <v>2.565029370036655</v>
       </c>
       <c r="L9" t="n">
-        <v>0.4952273997531506</v>
+        <v>-9.210916492149646</v>
       </c>
       <c r="M9" t="n">
-        <v>0.340569455238534</v>
+        <v>4.872506153600864</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2152853171046011</v>
+        <v>-8.345321430992163</v>
       </c>
       <c r="O9" t="n">
-        <v>0.3473784458122394</v>
+        <v>-4.341359969311836</v>
       </c>
       <c r="P9" t="n">
-        <v>0.3847120294177028</v>
+        <v>-11.87797614267347</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.04313111012421422</v>
+        <v>-13.51525027468311</v>
       </c>
       <c r="R9" t="n">
-        <v>0.4129343469480671</v>
+        <v>-1.14232425020868</v>
       </c>
       <c r="S9" t="n">
-        <v>0.2475246417274225</v>
+        <v>-11.79853450039488</v>
       </c>
       <c r="T9" t="n">
-        <v>0.4247774197027724</v>
+        <v>-15.0145481397347</v>
       </c>
       <c r="U9" t="n">
-        <v>0.2171679806526836</v>
+        <v>4.987356892536513</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1733592628182073</v>
+        <v>-9.197067949227812</v>
       </c>
       <c r="W9" t="n">
-        <v>0.3621498688691457</v>
+        <v>-7.229536028097698</v>
       </c>
       <c r="X9" t="n">
-        <v>0.4916757197682774</v>
+        <v>-17.59005194518193</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.4108777459193241</v>
+        <v>-2.564118925033186</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.1460574675714831</v>
+        <v>-6.527505775908338</v>
       </c>
       <c r="AA9" t="n">
-        <v>-0.1327825894208053</v>
+        <v>-25.94319784955529</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.08308625182050619</v>
+        <v>-7.048301767423446</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.04084431949694281</v>
+        <v>-17.47778807908902</v>
       </c>
     </row>
     <row r="10">
@@ -3228,88 +3228,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.3942760650249524</v>
+        <v>-6.471966992872805</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.1571702223855627</v>
+        <v>-4.777533999153452</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.5285581129293417</v>
+        <v>-4.582481203173075</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6050178004321202</v>
+        <v>0.6312624133700635</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04754471504093481</v>
+        <v>-13.54413194673393</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.1852678404320774</v>
+        <v>-11.89163223649107</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2338021857882167</v>
+        <v>2.865124542786676</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.3589043202379852</v>
+        <v>-0.8684818442268925</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.3609660264463745</v>
+        <v>-10.23667331526461</v>
       </c>
       <c r="K10" t="n">
-        <v>0.00770789461751506</v>
+        <v>0.7410905638845309</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1130679141610289</v>
+        <v>-9.589653547399807</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.03712067457583199</v>
+        <v>3.532865117008764</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.1680370468233309</v>
+        <v>-8.306091898875096</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.07007278365242478</v>
+        <v>-5.041174295482772</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.03634846450112647</v>
+        <v>-11.56289191152655</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.3201605867180222</v>
+        <v>-14.20303666383636</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0430772136203888</v>
+        <v>0.1648068711340822</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.1784771660418387</v>
+        <v>-12.25564979648634</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.04737548619616309</v>
+        <v>-11.72788361132882</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.1838562159029136</v>
+        <v>7.453913935019592</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.2371037821160683</v>
+        <v>-11.72819620821181</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.0343426988923044</v>
+        <v>-6.940399847550059</v>
       </c>
       <c r="X10" t="n">
-        <v>0.07005687364003033</v>
+        <v>-16.48626042303003</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.05191976822351169</v>
+        <v>-2.950341180881527</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.5543266438880289</v>
+        <v>-5.496251044652269</v>
       </c>
       <c r="AA10" t="n">
-        <v>-0.589826645142436</v>
+        <v>-25.72884543653182</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.2873066896263505</v>
+        <v>-7.597157904816182</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.3746706490859285</v>
+        <v>-18.20968207724654</v>
       </c>
     </row>
     <row r="11">
@@ -3317,88 +3317,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.3305288726065693</v>
+        <v>-7.32011811125771</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.02912794369004883</v>
+        <v>-4.368631950442298</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.4635451821554591</v>
+        <v>-1.013048958529922</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6254218509896515</v>
+        <v>2.256965039268387</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0674980869467437</v>
+        <v>-13.7437638551725</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.06504043953615521</v>
+        <v>-11.90884766303352</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3437730310226751</v>
+        <v>4.280563341720634</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.3249225952896072</v>
+        <v>-2.481826171198228</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.2306978773985863</v>
+        <v>-9.783734844454637</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0740903734538591</v>
+        <v>1.589096433140175</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1306305201903141</v>
+        <v>-10.18433075460696</v>
       </c>
       <c r="M11" t="n">
-        <v>0.02961827119644289</v>
+        <v>3.419682432399803</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.1693527023404901</v>
+        <v>-8.948829860060492</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.03742064577585481</v>
+        <v>-5.410170774906486</v>
       </c>
       <c r="P11" t="n">
-        <v>0.06342422722128072</v>
+        <v>-12.94768789464042</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.3164930355685257</v>
+        <v>-13.06812452867731</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.00218851362248422</v>
+        <v>0.9350412743278582</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.09690518872737941</v>
+        <v>-12.96605832212864</v>
       </c>
       <c r="T11" t="n">
-        <v>0.07484653762343876</v>
+        <v>-12.79596643688225</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.1364754744701256</v>
+        <v>5.597263014028109</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.1460675008196613</v>
+        <v>-10.87707380483311</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.01263729198368525</v>
+        <v>-7.501051635170676</v>
       </c>
       <c r="X11" t="n">
-        <v>0.09486089216777543</v>
+        <v>-18.15398984148175</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.03392784643744556</v>
+        <v>-2.219918516582767</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.5622096821913537</v>
+        <v>-5.163208719552449</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.4423035960882278</v>
+        <v>-25.80346850010205</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.3039991621997749</v>
+        <v>-7.785552887824117</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.3005383269119257</v>
+        <v>-17.48884074992373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected emissions update, tested for historical data and various future data parameters
</commit_message>
<xml_diff>
--- a/Data/intermediate.xlsx
+++ b/Data/intermediate.xlsx
@@ -526,88 +526,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-3.062472067885806</v>
+        <v>2.203256752069693</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.238964260942972</v>
+        <v>-2.915147586742647</v>
       </c>
       <c r="D2" t="n">
-        <v>7.437373840288144</v>
+        <v>-3.660142648263641</v>
       </c>
       <c r="E2" t="n">
-        <v>-10.72152501685048</v>
+        <v>-5.627657280467734</v>
       </c>
       <c r="F2" t="n">
-        <v>-6.291011590403967</v>
+        <v>-3.759456289974312</v>
       </c>
       <c r="G2" t="n">
-        <v>-5.122548905943133</v>
+        <v>3.457793147082079</v>
       </c>
       <c r="H2" t="n">
-        <v>-12.09360305353633</v>
+        <v>-2.151884861079954</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.194374853749748</v>
+        <v>-0.08139502643800833</v>
       </c>
       <c r="J2" t="n">
-        <v>5.588484447958806</v>
+        <v>-3.65614698063467</v>
       </c>
       <c r="K2" t="n">
-        <v>2.942436717004137</v>
+        <v>-3.092599224656857</v>
       </c>
       <c r="L2" t="n">
-        <v>16.97104816942395</v>
+        <v>-4.789174734805638</v>
       </c>
       <c r="M2" t="n">
-        <v>14.66687257116591</v>
+        <v>-4.32385018326091</v>
       </c>
       <c r="N2" t="n">
-        <v>-5.279801303487293</v>
+        <v>-6.563543568839558</v>
       </c>
       <c r="O2" t="n">
-        <v>-2.027855489921127</v>
+        <v>-4.947148139797709</v>
       </c>
       <c r="P2" t="n">
-        <v>-6.020561393380905</v>
+        <v>-5.410340650569359</v>
       </c>
       <c r="Q2" t="n">
-        <v>-7.19228927023893</v>
+        <v>-5.779042343796273</v>
       </c>
       <c r="R2" t="n">
-        <v>-10.88254097223103</v>
+        <v>-10.29566691701302</v>
       </c>
       <c r="S2" t="n">
-        <v>-1.91471115892682</v>
+        <v>-9.437867291806139</v>
       </c>
       <c r="T2" t="n">
-        <v>-13.10694981157039</v>
+        <v>-11.73230453567659</v>
       </c>
       <c r="U2" t="n">
-        <v>-17.32416129087358</v>
+        <v>-8.80485939379988</v>
       </c>
       <c r="V2" t="n">
-        <v>-6.89214987764487</v>
+        <v>-10.27294460356858</v>
       </c>
       <c r="W2" t="n">
-        <v>-21.53375914133988</v>
+        <v>-11.8913566109667</v>
       </c>
       <c r="X2" t="n">
-        <v>-15.59812707021529</v>
+        <v>-12.39654096035627</v>
       </c>
       <c r="Y2" t="n">
-        <v>-23.40566861543854</v>
+        <v>-13.69387899498244</v>
       </c>
       <c r="Z2" t="n">
-        <v>-30.63856331673106</v>
+        <v>-22.96036864186023</v>
       </c>
       <c r="AA2" t="n">
-        <v>-30.35127888996791</v>
+        <v>-21.36830209179941</v>
       </c>
       <c r="AB2" t="n">
-        <v>-37.94820144614945</v>
+        <v>-32.74570025339889</v>
       </c>
       <c r="AC2" t="n">
-        <v>-53.50836577097834</v>
+        <v>-57.70849630944869</v>
       </c>
     </row>
     <row r="3">
@@ -615,88 +615,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.139485085637585</v>
+        <v>-1.881483636539404</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.241979489516393</v>
+        <v>-7.610894813088846</v>
       </c>
       <c r="D3" t="n">
-        <v>5.59988776736893</v>
+        <v>-7.529855965082808</v>
       </c>
       <c r="E3" t="n">
-        <v>-10.20867042735266</v>
+        <v>-8.040674335274598</v>
       </c>
       <c r="F3" t="n">
-        <v>-5.327468593538963</v>
+        <v>-7.931021727948621</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.685846710856667</v>
+        <v>-4.882400256709</v>
       </c>
       <c r="H3" t="n">
-        <v>-12.10355983859855</v>
+        <v>-6.578456229286526</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4370724523983638</v>
+        <v>-5.498367406501969</v>
       </c>
       <c r="J3" t="n">
-        <v>6.602389756637396</v>
+        <v>-7.663183278783197</v>
       </c>
       <c r="K3" t="n">
-        <v>3.73543412644946</v>
+        <v>-5.396457385667087</v>
       </c>
       <c r="L3" t="n">
-        <v>14.68014145885492</v>
+        <v>-11.05498653466389</v>
       </c>
       <c r="M3" t="n">
-        <v>11.86278066764788</v>
+        <v>-8.280524944280138</v>
       </c>
       <c r="N3" t="n">
-        <v>-8.006074568606715</v>
+        <v>-10.87376220365612</v>
       </c>
       <c r="O3" t="n">
-        <v>-4.177002472873207</v>
+        <v>-7.887282319054789</v>
       </c>
       <c r="P3" t="n">
-        <v>-5.132740790948361</v>
+        <v>-9.319158251965057</v>
       </c>
       <c r="Q3" t="n">
-        <v>-5.061576974475349</v>
+        <v>-8.013638761938655</v>
       </c>
       <c r="R3" t="n">
-        <v>-10.13486565098249</v>
+        <v>-15.48131407677113</v>
       </c>
       <c r="S3" t="n">
-        <v>-1.994121656626827</v>
+        <v>-13.11741151899361</v>
       </c>
       <c r="T3" t="n">
-        <v>-14.97482099342375</v>
+        <v>-15.22228286513356</v>
       </c>
       <c r="U3" t="n">
-        <v>-17.25606074705173</v>
+        <v>-12.25803535755876</v>
       </c>
       <c r="V3" t="n">
-        <v>-6.01774991476924</v>
+        <v>-14.59559105636559</v>
       </c>
       <c r="W3" t="n">
-        <v>-21.98781703417996</v>
+        <v>-14.83550628264717</v>
       </c>
       <c r="X3" t="n">
-        <v>-14.28049012570534</v>
+        <v>-16.6513914847616</v>
       </c>
       <c r="Y3" t="n">
-        <v>-24.60085862736441</v>
+        <v>-19.36401392885483</v>
       </c>
       <c r="Z3" t="n">
-        <v>-29.77937129340319</v>
+        <v>-27.58237606423543</v>
       </c>
       <c r="AA3" t="n">
-        <v>-30.99139082150541</v>
+        <v>-27.56433428728441</v>
       </c>
       <c r="AB3" t="n">
-        <v>-36.71630962320474</v>
+        <v>-36.76700297901852</v>
       </c>
       <c r="AC3" t="n">
-        <v>-54.51464059041903</v>
+        <v>-64.75300442263308</v>
       </c>
     </row>
     <row r="4">
@@ -704,88 +704,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4467285704480823</v>
+        <v>0.7953684310351807</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.168513231793739</v>
+        <v>-3.95518560632639</v>
       </c>
       <c r="D4" t="n">
-        <v>7.697884648782734</v>
+        <v>-3.834810490073308</v>
       </c>
       <c r="E4" t="n">
-        <v>-11.45940576018544</v>
+        <v>-4.095594264574564</v>
       </c>
       <c r="F4" t="n">
-        <v>-7.420421936007324</v>
+        <v>-2.072252697127052</v>
       </c>
       <c r="G4" t="n">
-        <v>-4.555631857672106</v>
+        <v>1.670466167149034</v>
       </c>
       <c r="H4" t="n">
-        <v>-11.49305199086962</v>
+        <v>-1.657361479381778</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.5261801105283777</v>
+        <v>-2.908289143196434</v>
       </c>
       <c r="J4" t="n">
-        <v>6.537566657249014</v>
+        <v>-1.83561055369456</v>
       </c>
       <c r="K4" t="n">
-        <v>3.856865919024551</v>
+        <v>-2.054297467932693</v>
       </c>
       <c r="L4" t="n">
-        <v>15.27426585997895</v>
+        <v>-6.832052111065551</v>
       </c>
       <c r="M4" t="n">
-        <v>13.30410813477789</v>
+        <v>-3.682437617249104</v>
       </c>
       <c r="N4" t="n">
-        <v>-6.82700796225998</v>
+        <v>-7.322462774972543</v>
       </c>
       <c r="O4" t="n">
-        <v>-5.75984944657945</v>
+        <v>-4.299926846572474</v>
       </c>
       <c r="P4" t="n">
-        <v>-4.370530604408938</v>
+        <v>-5.659622431925891</v>
       </c>
       <c r="Q4" t="n">
-        <v>-6.163529070313156</v>
+        <v>-7.562249599549294</v>
       </c>
       <c r="R4" t="n">
-        <v>-11.39575175159627</v>
+        <v>-12.1942411244396</v>
       </c>
       <c r="S4" t="n">
-        <v>-1.23420965526558</v>
+        <v>-9.660928597468297</v>
       </c>
       <c r="T4" t="n">
-        <v>-16.14478264679504</v>
+        <v>-12.53064772218563</v>
       </c>
       <c r="U4" t="n">
-        <v>-16.51875293779776</v>
+        <v>-9.818043177620867</v>
       </c>
       <c r="V4" t="n">
-        <v>-7.536305029284559</v>
+        <v>-11.00606694940653</v>
       </c>
       <c r="W4" t="n">
-        <v>-20.97968121432941</v>
+        <v>-11.73646190531282</v>
       </c>
       <c r="X4" t="n">
-        <v>-16.3546689063688</v>
+        <v>-14.60158795273038</v>
       </c>
       <c r="Y4" t="n">
-        <v>-24.26319529170434</v>
+        <v>-14.33850458860851</v>
       </c>
       <c r="Z4" t="n">
-        <v>-29.41382355194741</v>
+        <v>-24.78367772925949</v>
       </c>
       <c r="AA4" t="n">
-        <v>-31.29069855197784</v>
+        <v>-21.1141749815219</v>
       </c>
       <c r="AB4" t="n">
-        <v>-36.49788203024799</v>
+        <v>-34.1079995451833</v>
       </c>
       <c r="AC4" t="n">
-        <v>-53.03119749409934</v>
+        <v>-58.20102472861575</v>
       </c>
     </row>
     <row r="5">
@@ -793,88 +793,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.5429745515566462</v>
+        <v>0.9442875544672349</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.907147413067737</v>
+        <v>-4.32879138192052</v>
       </c>
       <c r="D5" t="n">
-        <v>7.905499311170567</v>
+        <v>-6.295316875160136</v>
       </c>
       <c r="E5" t="n">
-        <v>-11.09177154325076</v>
+        <v>-4.858044154532653</v>
       </c>
       <c r="F5" t="n">
-        <v>-7.26827331311563</v>
+        <v>-5.919374760540562</v>
       </c>
       <c r="G5" t="n">
-        <v>-3.315373223663929</v>
+        <v>-0.4853489344750486</v>
       </c>
       <c r="H5" t="n">
-        <v>-13.38844145200353</v>
+        <v>-5.912970544198999</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2039540758508949</v>
+        <v>-3.974345334776983</v>
       </c>
       <c r="J5" t="n">
-        <v>7.914190018704072</v>
+        <v>-6.124049291914567</v>
       </c>
       <c r="K5" t="n">
-        <v>3.255623552035985</v>
+        <v>-4.028606783320361</v>
       </c>
       <c r="L5" t="n">
-        <v>16.73886608065255</v>
+        <v>-7.108447751729591</v>
       </c>
       <c r="M5" t="n">
-        <v>12.7294817630945</v>
+        <v>-6.711656811327776</v>
       </c>
       <c r="N5" t="n">
-        <v>-7.588763796178019</v>
+        <v>-7.863059456945824</v>
       </c>
       <c r="O5" t="n">
-        <v>-7.31327213910574</v>
+        <v>-6.961979516399829</v>
       </c>
       <c r="P5" t="n">
-        <v>-4.935316698190776</v>
+        <v>-7.92524629157768</v>
       </c>
       <c r="Q5" t="n">
-        <v>-6.431944139493824</v>
+        <v>-8.514691497949892</v>
       </c>
       <c r="R5" t="n">
-        <v>-11.72007626584621</v>
+        <v>-12.13520499982537</v>
       </c>
       <c r="S5" t="n">
-        <v>-1.314255805378605</v>
+        <v>-11.42893577036436</v>
       </c>
       <c r="T5" t="n">
-        <v>-15.72796925759258</v>
+        <v>-13.90026640299797</v>
       </c>
       <c r="U5" t="n">
-        <v>-18.32290296863097</v>
+        <v>-9.408802151321726</v>
       </c>
       <c r="V5" t="n">
-        <v>-5.990521356331409</v>
+        <v>-13.98175040463344</v>
       </c>
       <c r="W5" t="n">
-        <v>-20.6133066635805</v>
+        <v>-13.25359540148225</v>
       </c>
       <c r="X5" t="n">
-        <v>-14.0550277387915</v>
+        <v>-15.04194871916292</v>
       </c>
       <c r="Y5" t="n">
-        <v>-23.99766606839822</v>
+        <v>-17.53561349713091</v>
       </c>
       <c r="Z5" t="n">
-        <v>-29.32499457967619</v>
+        <v>-27.07955578331005</v>
       </c>
       <c r="AA5" t="n">
-        <v>-30.48579605173391</v>
+        <v>-25.43829475158022</v>
       </c>
       <c r="AB5" t="n">
-        <v>-37.78510372650722</v>
+        <v>-35.36851546598874</v>
       </c>
       <c r="AC5" t="n">
-        <v>-53.96948521671438</v>
+        <v>-60.37071762353019</v>
       </c>
     </row>
     <row r="6">
@@ -882,88 +882,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.073598996755198</v>
+        <v>0.4989234413804855</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.115623866512848</v>
+        <v>-4.72682516897868</v>
       </c>
       <c r="D6" t="n">
-        <v>3.526017737593814</v>
+        <v>-4.11915039764253</v>
       </c>
       <c r="E6" t="n">
-        <v>-11.72149363694911</v>
+        <v>-4.146657334951867</v>
       </c>
       <c r="F6" t="n">
-        <v>-4.575912535234156</v>
+        <v>-2.855825727560295</v>
       </c>
       <c r="G6" t="n">
-        <v>-4.521514667102897</v>
+        <v>0.4112854032744053</v>
       </c>
       <c r="H6" t="n">
-        <v>-12.08755308252102</v>
+        <v>-1.789193881255226</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.296319510479982</v>
+        <v>-3.610227415955889</v>
       </c>
       <c r="J6" t="n">
-        <v>7.627759666067703</v>
+        <v>-4.280319401019038</v>
       </c>
       <c r="K6" t="n">
-        <v>4.571844691831569</v>
+        <v>-0.7683269453788366</v>
       </c>
       <c r="L6" t="n">
-        <v>15.32272888177511</v>
+        <v>-5.429506179676224</v>
       </c>
       <c r="M6" t="n">
-        <v>13.50073994979975</v>
+        <v>-3.474159082076488</v>
       </c>
       <c r="N6" t="n">
-        <v>-6.822117422162766</v>
+        <v>-5.574496445657659</v>
       </c>
       <c r="O6" t="n">
-        <v>-4.953462020505739</v>
+        <v>-2.62039647647817</v>
       </c>
       <c r="P6" t="n">
-        <v>-3.013847306722354</v>
+        <v>-4.835961795275614</v>
       </c>
       <c r="Q6" t="n">
-        <v>-4.974567279080247</v>
+        <v>-5.089149202307958</v>
       </c>
       <c r="R6" t="n">
-        <v>-11.20396251754573</v>
+        <v>-8.974356110814046</v>
       </c>
       <c r="S6" t="n">
-        <v>1.304574022894279</v>
+        <v>-7.419526956099681</v>
       </c>
       <c r="T6" t="n">
-        <v>-16.77690036287866</v>
+        <v>-12.30138079326382</v>
       </c>
       <c r="U6" t="n">
-        <v>-17.34588008284184</v>
+        <v>-6.672105161730501</v>
       </c>
       <c r="V6" t="n">
-        <v>-7.314957841071942</v>
+        <v>-13.73176459404712</v>
       </c>
       <c r="W6" t="n">
-        <v>-21.4264139595598</v>
+        <v>-13.28911674802127</v>
       </c>
       <c r="X6" t="n">
-        <v>-16.63070443787229</v>
+        <v>-12.55128271845177</v>
       </c>
       <c r="Y6" t="n">
-        <v>-22.91160814922423</v>
+        <v>-13.56248038126602</v>
       </c>
       <c r="Z6" t="n">
-        <v>-28.35527554478023</v>
+        <v>-24.56034366366385</v>
       </c>
       <c r="AA6" t="n">
-        <v>-30.7576901774996</v>
+        <v>-23.66822743222455</v>
       </c>
       <c r="AB6" t="n">
-        <v>-37.09499468405851</v>
+        <v>-31.54318367530349</v>
       </c>
       <c r="AC6" t="n">
-        <v>-55.2068264028877</v>
+        <v>-59.19228956777507</v>
       </c>
     </row>
     <row r="7">
@@ -971,88 +971,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.087523666832824</v>
+        <v>-2.294807694406027</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.539149916955957</v>
+        <v>-7.546663788411537</v>
       </c>
       <c r="D7" t="n">
-        <v>6.179486134219745</v>
+        <v>-6.982084156116814</v>
       </c>
       <c r="E7" t="n">
-        <v>-11.69205347595221</v>
+        <v>-4.123906149344998</v>
       </c>
       <c r="F7" t="n">
-        <v>-6.512786353641327</v>
+        <v>-5.990423572688631</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.15082526178726</v>
+        <v>-2.333674320411922</v>
       </c>
       <c r="H7" t="n">
-        <v>-12.83287523592911</v>
+        <v>-3.41467200611289</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6290464570105474</v>
+        <v>-3.650166964255903</v>
       </c>
       <c r="J7" t="n">
-        <v>6.836757420075843</v>
+        <v>-5.862792941231871</v>
       </c>
       <c r="K7" t="n">
-        <v>3.310268337863547</v>
+        <v>-4.993616062798331</v>
       </c>
       <c r="L7" t="n">
-        <v>16.46279429234692</v>
+        <v>-8.40191133935207</v>
       </c>
       <c r="M7" t="n">
-        <v>14.28808018590276</v>
+        <v>-6.620169115085226</v>
       </c>
       <c r="N7" t="n">
-        <v>-6.174624918148044</v>
+        <v>-7.776390799101457</v>
       </c>
       <c r="O7" t="n">
-        <v>-6.193914319411046</v>
+        <v>-6.890070653246162</v>
       </c>
       <c r="P7" t="n">
-        <v>-4.432347038087235</v>
+        <v>-7.776689040046603</v>
       </c>
       <c r="Q7" t="n">
-        <v>-5.339031836287031</v>
+        <v>-7.186613228492441</v>
       </c>
       <c r="R7" t="n">
-        <v>-9.712828878304435</v>
+        <v>-11.46787664099678</v>
       </c>
       <c r="S7" t="n">
-        <v>0.5782101881208774</v>
+        <v>-11.62815950769745</v>
       </c>
       <c r="T7" t="n">
-        <v>-15.36616464081365</v>
+        <v>-13.0988408981005</v>
       </c>
       <c r="U7" t="n">
-        <v>-18.78299958208659</v>
+        <v>-11.22395362794025</v>
       </c>
       <c r="V7" t="n">
-        <v>-7.925757249365137</v>
+        <v>-12.26369417461324</v>
       </c>
       <c r="W7" t="n">
-        <v>-19.89412215045123</v>
+        <v>-14.69174554211075</v>
       </c>
       <c r="X7" t="n">
-        <v>-15.70463466475092</v>
+        <v>-15.32529109338185</v>
       </c>
       <c r="Y7" t="n">
-        <v>-22.10232708259301</v>
+        <v>-18.26211719753348</v>
       </c>
       <c r="Z7" t="n">
-        <v>-30.36817266681993</v>
+        <v>-25.39428508331583</v>
       </c>
       <c r="AA7" t="n">
-        <v>-29.5832863704983</v>
+        <v>-25.86757835300908</v>
       </c>
       <c r="AB7" t="n">
-        <v>-37.09050088009874</v>
+        <v>-36.14309128917374</v>
       </c>
       <c r="AC7" t="n">
-        <v>-53.34625897288411</v>
+        <v>-60.52867622333567</v>
       </c>
     </row>
     <row r="8">
@@ -1060,88 +1060,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.641622573006717</v>
+        <v>-2.024835429105408</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.12900126241522</v>
+        <v>-6.540190397102974</v>
       </c>
       <c r="D8" t="n">
-        <v>7.163279691192749</v>
+        <v>-6.732385428531448</v>
       </c>
       <c r="E8" t="n">
-        <v>-7.135468866290093</v>
+        <v>-7.212665057998301</v>
       </c>
       <c r="F8" t="n">
-        <v>-7.704689008577123</v>
+        <v>-4.975485376161116</v>
       </c>
       <c r="G8" t="n">
-        <v>-4.194524896508128</v>
+        <v>-2.311026035374536</v>
       </c>
       <c r="H8" t="n">
-        <v>-14.05592443741154</v>
+        <v>-6.308129058493849</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.3574066867107408</v>
+        <v>-4.926094697181014</v>
       </c>
       <c r="J8" t="n">
-        <v>5.925438770235912</v>
+        <v>-7.375321619822163</v>
       </c>
       <c r="K8" t="n">
-        <v>4.335126974127458</v>
+        <v>-6.683008241116678</v>
       </c>
       <c r="L8" t="n">
-        <v>12.6836183114694</v>
+        <v>-8.706392676362491</v>
       </c>
       <c r="M8" t="n">
-        <v>10.37611453724694</v>
+        <v>-5.672905146848614</v>
       </c>
       <c r="N8" t="n">
-        <v>-6.846003504399961</v>
+        <v>-11.02136340087631</v>
       </c>
       <c r="O8" t="n">
-        <v>-5.796429283940403</v>
+        <v>-5.29758382773346</v>
       </c>
       <c r="P8" t="n">
-        <v>-4.83798088958136</v>
+        <v>-9.583070269509054</v>
       </c>
       <c r="Q8" t="n">
-        <v>-7.102074605198542</v>
+        <v>-9.824528098103189</v>
       </c>
       <c r="R8" t="n">
-        <v>-11.56399954035802</v>
+        <v>-13.17642804268808</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.6784239021190412</v>
+        <v>-12.41494082192739</v>
       </c>
       <c r="T8" t="n">
-        <v>-14.69132981903824</v>
+        <v>-14.24890486095475</v>
       </c>
       <c r="U8" t="n">
-        <v>-17.35754109112679</v>
+        <v>-8.632913934583662</v>
       </c>
       <c r="V8" t="n">
-        <v>-9.480372106978752</v>
+        <v>-13.86328696749337</v>
       </c>
       <c r="W8" t="n">
-        <v>-21.90683987664676</v>
+        <v>-12.96674166146745</v>
       </c>
       <c r="X8" t="n">
-        <v>-15.67292248391976</v>
+        <v>-14.91582036810826</v>
       </c>
       <c r="Y8" t="n">
-        <v>-25.55161353390026</v>
+        <v>-18.78478674667726</v>
       </c>
       <c r="Z8" t="n">
-        <v>-30.45505905808368</v>
+        <v>-26.54650013277378</v>
       </c>
       <c r="AA8" t="n">
-        <v>-30.50210707585311</v>
+        <v>-26.10415856187034</v>
       </c>
       <c r="AB8" t="n">
-        <v>-35.75691886645139</v>
+        <v>-36.82820112678417</v>
       </c>
       <c r="AC8" t="n">
-        <v>-53.27468525189303</v>
+        <v>-61.0851259327351</v>
       </c>
     </row>
     <row r="9">
@@ -1149,88 +1149,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.469008799770898</v>
+        <v>1.888915345369813</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1215279288577285</v>
+        <v>-1.814724410018849</v>
       </c>
       <c r="D9" t="n">
-        <v>6.735522609015954</v>
+        <v>-0.04613429769095967</v>
       </c>
       <c r="E9" t="n">
-        <v>-8.24856719086303</v>
+        <v>-5.262475771921713</v>
       </c>
       <c r="F9" t="n">
-        <v>-5.961402250005619</v>
+        <v>-0.3158840407642288</v>
       </c>
       <c r="G9" t="n">
-        <v>-7.029823983992267</v>
+        <v>1.790553463542927</v>
       </c>
       <c r="H9" t="n">
-        <v>-14.35925005765417</v>
+        <v>-0.4751389910029726</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4358911300878008</v>
+        <v>-0.09260290178227049</v>
       </c>
       <c r="J9" t="n">
-        <v>7.864173085910287</v>
+        <v>-1.090014993697799</v>
       </c>
       <c r="K9" t="n">
-        <v>3.743470526606636</v>
+        <v>0.2201118890005671</v>
       </c>
       <c r="L9" t="n">
-        <v>15.67926011973778</v>
+        <v>-4.159502025095445</v>
       </c>
       <c r="M9" t="n">
-        <v>12.2806199563457</v>
+        <v>-1.223938197675252</v>
       </c>
       <c r="N9" t="n">
-        <v>-6.680354887084606</v>
+        <v>-4.646886882458485</v>
       </c>
       <c r="O9" t="n">
-        <v>-4.457464054912472</v>
+        <v>-3.434997638079896</v>
       </c>
       <c r="P9" t="n">
-        <v>-3.225687441029581</v>
+        <v>-3.420484680036818</v>
       </c>
       <c r="Q9" t="n">
-        <v>-6.713225499562106</v>
+        <v>-4.533470595113121</v>
       </c>
       <c r="R9" t="n">
-        <v>-12.73490312127528</v>
+        <v>-8.939639275725511</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.5900597187203074</v>
+        <v>-9.990165138775854</v>
       </c>
       <c r="T9" t="n">
-        <v>-14.20051960605294</v>
+        <v>-8.736730876077186</v>
       </c>
       <c r="U9" t="n">
-        <v>-17.45230079500139</v>
+        <v>-6.652507715051908</v>
       </c>
       <c r="V9" t="n">
-        <v>-4.501457351254346</v>
+        <v>-10.0868993419846</v>
       </c>
       <c r="W9" t="n">
-        <v>-20.84321497597252</v>
+        <v>-11.1534415820112</v>
       </c>
       <c r="X9" t="n">
-        <v>-14.92822216379568</v>
+        <v>-10.3183432912204</v>
       </c>
       <c r="Y9" t="n">
-        <v>-23.46918605518842</v>
+        <v>-12.47106515441497</v>
       </c>
       <c r="Z9" t="n">
-        <v>-28.76093498514265</v>
+        <v>-21.9299559389906</v>
       </c>
       <c r="AA9" t="n">
-        <v>-31.26265421115872</v>
+        <v>-21.5646936706212</v>
       </c>
       <c r="AB9" t="n">
-        <v>-36.39032504734379</v>
+        <v>-31.90093255372198</v>
       </c>
       <c r="AC9" t="n">
-        <v>-52.92511420596975</v>
+        <v>-54.949358731065</v>
       </c>
     </row>
     <row r="10">
@@ -1238,88 +1238,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.080365464378204</v>
+        <v>-1.263728627304542</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.90707729942429</v>
+        <v>-5.825251801485225</v>
       </c>
       <c r="D10" t="n">
-        <v>4.023061872667309</v>
+        <v>-5.849769125306823</v>
       </c>
       <c r="E10" t="n">
-        <v>-10.41570178435389</v>
+        <v>-7.259487258608887</v>
       </c>
       <c r="F10" t="n">
-        <v>-8.727219954383457</v>
+        <v>-5.819354771964166</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.83719562236254</v>
+        <v>-0.8926958034422805</v>
       </c>
       <c r="H10" t="n">
-        <v>-12.38814932361473</v>
+        <v>-3.869878302408033</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.6060173421286192</v>
+        <v>-3.351700648739033</v>
       </c>
       <c r="J10" t="n">
-        <v>5.767738540023842</v>
+        <v>-6.992023399408396</v>
       </c>
       <c r="K10" t="n">
-        <v>1.672794019622382</v>
+        <v>-4.934651414357422</v>
       </c>
       <c r="L10" t="n">
-        <v>17.91598939122799</v>
+        <v>-8.26594737318746</v>
       </c>
       <c r="M10" t="n">
-        <v>12.67724040355363</v>
+        <v>-4.773692581083308</v>
       </c>
       <c r="N10" t="n">
-        <v>-7.292803488780454</v>
+        <v>-7.709983142389076</v>
       </c>
       <c r="O10" t="n">
-        <v>-6.171759807130333</v>
+        <v>-6.902519239547972</v>
       </c>
       <c r="P10" t="n">
-        <v>-5.84851643341989</v>
+        <v>-7.968867320338195</v>
       </c>
       <c r="Q10" t="n">
-        <v>-6.170196315530535</v>
+        <v>-8.674215500591178</v>
       </c>
       <c r="R10" t="n">
-        <v>-10.59172153935027</v>
+        <v>-14.059878252038</v>
       </c>
       <c r="S10" t="n">
-        <v>-1.286585587975646</v>
+        <v>-10.61778145035866</v>
       </c>
       <c r="T10" t="n">
-        <v>-17.46323388142073</v>
+        <v>-15.66133615876454</v>
       </c>
       <c r="U10" t="n">
-        <v>-18.25495878730424</v>
+        <v>-10.43582322671984</v>
       </c>
       <c r="V10" t="n">
-        <v>-6.965894922444066</v>
+        <v>-15.61692608595417</v>
       </c>
       <c r="W10" t="n">
-        <v>-21.84572175772603</v>
+        <v>-13.43586772655391</v>
       </c>
       <c r="X10" t="n">
-        <v>-18.36768470713927</v>
+        <v>-15.22959850136501</v>
       </c>
       <c r="Y10" t="n">
-        <v>-23.03688081070551</v>
+        <v>-16.98189786677914</v>
       </c>
       <c r="Z10" t="n">
-        <v>-28.42885024273507</v>
+        <v>-25.94465602227765</v>
       </c>
       <c r="AA10" t="n">
-        <v>-28.07001013433978</v>
+        <v>-26.78884536405297</v>
       </c>
       <c r="AB10" t="n">
-        <v>-38.01505237345851</v>
+        <v>-36.11939055969883</v>
       </c>
       <c r="AC10" t="n">
-        <v>-53.83160187051888</v>
+        <v>-61.18583849904258</v>
       </c>
     </row>
     <row r="11">
@@ -1327,88 +1327,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1361167218341284</v>
+        <v>-1.693018527669403</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.349945125598151</v>
+        <v>-6.691224027106706</v>
       </c>
       <c r="D11" t="n">
-        <v>5.513238801517774</v>
+        <v>-6.693076253709986</v>
       </c>
       <c r="E11" t="n">
-        <v>-11.72874705317787</v>
+        <v>-5.938186596566551</v>
       </c>
       <c r="F11" t="n">
-        <v>-6.274310057289685</v>
+        <v>-3.610318501720269</v>
       </c>
       <c r="G11" t="n">
-        <v>-4.632148106995988</v>
+        <v>-0.241759051957267</v>
       </c>
       <c r="H11" t="n">
-        <v>-11.81772026105496</v>
+        <v>-4.313422973084021</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.839997031347131</v>
+        <v>-3.839537321802083</v>
       </c>
       <c r="J11" t="n">
-        <v>7.47240550580891</v>
+        <v>-5.967152930014751</v>
       </c>
       <c r="K11" t="n">
-        <v>2.505299535104602</v>
+        <v>-5.146775322726474</v>
       </c>
       <c r="L11" t="n">
-        <v>16.71846071493313</v>
+        <v>-8.333860754992445</v>
       </c>
       <c r="M11" t="n">
-        <v>13.17896855237374</v>
+        <v>-4.846700551034296</v>
       </c>
       <c r="N11" t="n">
-        <v>-6.720551809843916</v>
+        <v>-8.784877608770985</v>
       </c>
       <c r="O11" t="n">
-        <v>-6.563113782472557</v>
+        <v>-5.181870881613721</v>
       </c>
       <c r="P11" t="n">
-        <v>-6.363248297528925</v>
+        <v>-7.906628283397611</v>
       </c>
       <c r="Q11" t="n">
-        <v>-6.427359880421676</v>
+        <v>-6.989313813575601</v>
       </c>
       <c r="R11" t="n">
-        <v>-11.513231326504</v>
+        <v>-11.02721178281118</v>
       </c>
       <c r="S11" t="n">
-        <v>-1.921645304521856</v>
+        <v>-12.50961211585008</v>
       </c>
       <c r="T11" t="n">
-        <v>-14.77107448433218</v>
+        <v>-13.61901973642837</v>
       </c>
       <c r="U11" t="n">
-        <v>-17.23708430482464</v>
+        <v>-10.50760837374294</v>
       </c>
       <c r="V11" t="n">
-        <v>-6.361845134784749</v>
+        <v>-14.46019000329179</v>
       </c>
       <c r="W11" t="n">
-        <v>-21.49187943345967</v>
+        <v>-14.80208620390368</v>
       </c>
       <c r="X11" t="n">
-        <v>-16.01014149161149</v>
+        <v>-13.71932100086302</v>
       </c>
       <c r="Y11" t="n">
-        <v>-22.63695321803819</v>
+        <v>-17.37120807843441</v>
       </c>
       <c r="Z11" t="n">
-        <v>-30.0093366059017</v>
+        <v>-26.40248661778353</v>
       </c>
       <c r="AA11" t="n">
-        <v>-29.07122773655565</v>
+        <v>-24.9096549581789</v>
       </c>
       <c r="AB11" t="n">
-        <v>-38.53271419968799</v>
+        <v>-36.29111481592779</v>
       </c>
       <c r="AC11" t="n">
-        <v>-52.6451091552</v>
+        <v>-61.62050791790782</v>
       </c>
     </row>
   </sheetData>
@@ -1521,88 +1521,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>18.09035783948996</v>
+        <v>0.4917582512556288</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.574573752029489</v>
+        <v>-2.959717985808141</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.971308705849237</v>
+        <v>2.387988719353929</v>
       </c>
       <c r="E2" t="n">
-        <v>3.749968886309238</v>
+        <v>1.845828554486171</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.910196971052603</v>
+        <v>-4.502091833101876</v>
       </c>
       <c r="G2" t="n">
-        <v>-13.51254108104425</v>
+        <v>-1.6131918533991</v>
       </c>
       <c r="H2" t="n">
-        <v>3.506309586628578</v>
+        <v>-1.952149672721519</v>
       </c>
       <c r="I2" t="n">
-        <v>-20.79024072154307</v>
+        <v>5.344785187546942</v>
       </c>
       <c r="J2" t="n">
-        <v>-17.57367864959065</v>
+        <v>5.609846825493651</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.189376465185704</v>
+        <v>2.14797831322402</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9753755475010712</v>
+        <v>2.808267819688757</v>
       </c>
       <c r="M2" t="n">
-        <v>-5.991652528988276</v>
+        <v>-1.107294336184879</v>
       </c>
       <c r="N2" t="n">
-        <v>-2.411925080305639</v>
+        <v>-2.993589592808061</v>
       </c>
       <c r="O2" t="n">
-        <v>-1.380797086968166</v>
+        <v>-2.329286826683694</v>
       </c>
       <c r="P2" t="n">
-        <v>3.243807476820508</v>
+        <v>-0.4407077548697069</v>
       </c>
       <c r="Q2" t="n">
-        <v>-4.91913646837151</v>
+        <v>-2.42716408179106</v>
       </c>
       <c r="R2" t="n">
-        <v>-10.80249251230266</v>
+        <v>1.401645482825969</v>
       </c>
       <c r="S2" t="n">
-        <v>2.540598671141096</v>
+        <v>-5.365168477586463</v>
       </c>
       <c r="T2" t="n">
-        <v>-9.568009608949712</v>
+        <v>2.211911339261191</v>
       </c>
       <c r="U2" t="n">
-        <v>0.6872512751907638</v>
+        <v>-3.016672431096848</v>
       </c>
       <c r="V2" t="n">
-        <v>-5.287375586005513</v>
+        <v>-4.6988882027504</v>
       </c>
       <c r="W2" t="n">
-        <v>-9.310085586312773</v>
+        <v>-2.933176116765403</v>
       </c>
       <c r="X2" t="n">
-        <v>-5.494719952613302</v>
+        <v>-5.432895246737232</v>
       </c>
       <c r="Y2" t="n">
-        <v>-3.197462258193638</v>
+        <v>-0.1225713137370676</v>
       </c>
       <c r="Z2" t="n">
-        <v>13.61456451492145</v>
+        <v>-6.151130510123215</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.7684429048442256</v>
+        <v>-3.955631387964204</v>
       </c>
       <c r="AB2" t="n">
-        <v>7.625931949875342</v>
+        <v>-2.801755406745296</v>
       </c>
       <c r="AC2" t="n">
-        <v>-13.96191155022901</v>
+        <v>-0.6694118815303289</v>
       </c>
     </row>
     <row r="3">
@@ -1610,88 +1610,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>18.4275624159164</v>
+        <v>-4.095640568593942</v>
       </c>
       <c r="C3" t="n">
-        <v>-7.980532244518947</v>
+        <v>-7.575646792765325</v>
       </c>
       <c r="D3" t="n">
-        <v>-5.048261751771806</v>
+        <v>-3.098135104784025</v>
       </c>
       <c r="E3" t="n">
-        <v>4.438889238237997</v>
+        <v>-3.256966048885553</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.512504317599351</v>
+        <v>-8.489353287726043</v>
       </c>
       <c r="G3" t="n">
-        <v>-16.70872758107307</v>
+        <v>-7.219113364686571</v>
       </c>
       <c r="H3" t="n">
-        <v>1.558129307951976</v>
+        <v>-7.983950367469896</v>
       </c>
       <c r="I3" t="n">
-        <v>-19.28215179376657</v>
+        <v>-1.369563466793604</v>
       </c>
       <c r="J3" t="n">
-        <v>-20.55900538763284</v>
+        <v>-0.4152581154811124</v>
       </c>
       <c r="K3" t="n">
-        <v>-2.744776773067609</v>
+        <v>-6.385798210858574</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8033988523865818</v>
+        <v>-0.2483977503771619</v>
       </c>
       <c r="M3" t="n">
-        <v>-5.725335759733898</v>
+        <v>-4.784264565790122</v>
       </c>
       <c r="N3" t="n">
-        <v>-4.540925844589511</v>
+        <v>-8.102915085648966</v>
       </c>
       <c r="O3" t="n">
-        <v>0.3481166177452195</v>
+        <v>-7.252564724283189</v>
       </c>
       <c r="P3" t="n">
-        <v>1.221004696279663</v>
+        <v>-4.01109771108565</v>
       </c>
       <c r="Q3" t="n">
-        <v>-5.62119624506836</v>
+        <v>-8.653012842012942</v>
       </c>
       <c r="R3" t="n">
-        <v>-10.21089775750867</v>
+        <v>-4.369195672471357</v>
       </c>
       <c r="S3" t="n">
-        <v>1.400511705517468</v>
+        <v>-11.71410567764538</v>
       </c>
       <c r="T3" t="n">
-        <v>-8.007337948027942</v>
+        <v>-2.077026206501396</v>
       </c>
       <c r="U3" t="n">
-        <v>1.531361832826273</v>
+        <v>-7.821996395400034</v>
       </c>
       <c r="V3" t="n">
-        <v>-7.345168339539679</v>
+        <v>-9.933323177703119</v>
       </c>
       <c r="W3" t="n">
-        <v>-11.63954658748583</v>
+        <v>-8.700210650493849</v>
       </c>
       <c r="X3" t="n">
-        <v>-3.899057106667333</v>
+        <v>-11.00272203360808</v>
       </c>
       <c r="Y3" t="n">
-        <v>-2.201712314616215</v>
+        <v>-5.897195685543796</v>
       </c>
       <c r="Z3" t="n">
-        <v>15.26195019931927</v>
+        <v>-12.33463104076379</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.5164229851871598</v>
+        <v>-8.732106951771959</v>
       </c>
       <c r="AB3" t="n">
-        <v>4.602895639801431</v>
+        <v>-8.386997721263665</v>
       </c>
       <c r="AC3" t="n">
-        <v>-15.58925355648864</v>
+        <v>-5.669033607612114</v>
       </c>
     </row>
     <row r="4">
@@ -1699,88 +1699,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>18.23352649795185</v>
+        <v>-2.052948834403503</v>
       </c>
       <c r="C4" t="n">
-        <v>-8.035318142607101</v>
+        <v>-6.075162623094208</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.858965818053119</v>
+        <v>0.127780376193122</v>
       </c>
       <c r="E4" t="n">
-        <v>3.470267712009265</v>
+        <v>0.6617674801120046</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.776720668844645</v>
+        <v>-4.671050460282114</v>
       </c>
       <c r="G4" t="n">
-        <v>-14.38145822788996</v>
+        <v>-3.370477579261629</v>
       </c>
       <c r="H4" t="n">
-        <v>3.408941575653318</v>
+        <v>-1.74866280309149</v>
       </c>
       <c r="I4" t="n">
-        <v>-20.42744968004643</v>
+        <v>3.403942046019032</v>
       </c>
       <c r="J4" t="n">
-        <v>-20.35952349386834</v>
+        <v>3.559400435815274</v>
       </c>
       <c r="K4" t="n">
-        <v>-5.107111300313607</v>
+        <v>-0.3934350614195658</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.7447743638399709</v>
+        <v>1.848271856821371</v>
       </c>
       <c r="M4" t="n">
-        <v>-8.483059343605724</v>
+        <v>-1.791723102315412</v>
       </c>
       <c r="N4" t="n">
-        <v>-4.610434900243037</v>
+        <v>-2.756217499830806</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.5397915753674927</v>
+        <v>-2.282193530544329</v>
       </c>
       <c r="P4" t="n">
-        <v>1.419432126036976</v>
+        <v>-1.562711416659242</v>
       </c>
       <c r="Q4" t="n">
-        <v>-5.205415541159568</v>
+        <v>-5.016920683575912</v>
       </c>
       <c r="R4" t="n">
-        <v>-9.791737111820172</v>
+        <v>-1.434161862828359</v>
       </c>
       <c r="S4" t="n">
-        <v>1.941701660103416</v>
+        <v>-7.366115956388446</v>
       </c>
       <c r="T4" t="n">
-        <v>-8.47560736245363</v>
+        <v>2.00228641189864</v>
       </c>
       <c r="U4" t="n">
-        <v>3.520830109519716</v>
+        <v>-4.670874360603381</v>
       </c>
       <c r="V4" t="n">
-        <v>-7.106882944097684</v>
+        <v>-5.125702488692555</v>
       </c>
       <c r="W4" t="n">
-        <v>-10.15768330591325</v>
+        <v>-3.053644760314656</v>
       </c>
       <c r="X4" t="n">
-        <v>-4.973940996364544</v>
+        <v>-5.712114201875075</v>
       </c>
       <c r="Y4" t="n">
-        <v>-3.496039517431503</v>
+        <v>-0.9223260441544241</v>
       </c>
       <c r="Z4" t="n">
-        <v>14.69142479176936</v>
+        <v>-8.241657104121298</v>
       </c>
       <c r="AA4" t="n">
-        <v>-1.388361879102415</v>
+        <v>-5.065921441536243</v>
       </c>
       <c r="AB4" t="n">
-        <v>4.314078173670611</v>
+        <v>-5.169515604708063</v>
       </c>
       <c r="AC4" t="n">
-        <v>-15.6641561893458</v>
+        <v>-0.9336992321905404</v>
       </c>
     </row>
     <row r="5">
@@ -1788,88 +1788,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>16.74824878055296</v>
+        <v>-1.174033340006362</v>
       </c>
       <c r="C5" t="n">
-        <v>-8.492725661068999</v>
+        <v>-3.688481227473984</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.635892768305034</v>
+        <v>-2.538902791554903</v>
       </c>
       <c r="E5" t="n">
-        <v>2.960242945020367</v>
+        <v>-1.696489707723484</v>
       </c>
       <c r="F5" t="n">
-        <v>-2.571103187473979</v>
+        <v>-6.01696512759136</v>
       </c>
       <c r="G5" t="n">
-        <v>-13.92781360745312</v>
+        <v>-5.366030980056644</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1654592658020624</v>
+        <v>-5.29411341515751</v>
       </c>
       <c r="I5" t="n">
-        <v>-18.85186924589374</v>
+        <v>2.659417280774077</v>
       </c>
       <c r="J5" t="n">
-        <v>-17.73545839215408</v>
+        <v>1.347202974463557</v>
       </c>
       <c r="K5" t="n">
-        <v>-4.541625847341345</v>
+        <v>-1.347155340269099</v>
       </c>
       <c r="L5" t="n">
-        <v>0.3093604562131307</v>
+        <v>-0.2693136180314641</v>
       </c>
       <c r="M5" t="n">
-        <v>-6.071370914845081</v>
+        <v>-2.607267524055779</v>
       </c>
       <c r="N5" t="n">
-        <v>-4.815600973864653</v>
+        <v>-5.186609815790632</v>
       </c>
       <c r="O5" t="n">
-        <v>0.648137119660757</v>
+        <v>-6.137336998777203</v>
       </c>
       <c r="P5" t="n">
-        <v>2.075472845400615</v>
+        <v>-0.8161989857089593</v>
       </c>
       <c r="Q5" t="n">
-        <v>-4.634159287251769</v>
+        <v>-5.737629479667218</v>
       </c>
       <c r="R5" t="n">
-        <v>-9.593433320518313</v>
+        <v>-2.219859090578889</v>
       </c>
       <c r="S5" t="n">
-        <v>3.02451871712874</v>
+        <v>-7.67366129674391</v>
       </c>
       <c r="T5" t="n">
-        <v>-10.43168587258605</v>
+        <v>0.2518619436150629</v>
       </c>
       <c r="U5" t="n">
-        <v>-1.231822178536718</v>
+        <v>-4.460728774141926</v>
       </c>
       <c r="V5" t="n">
-        <v>-6.243332422082724</v>
+        <v>-8.890726976779979</v>
       </c>
       <c r="W5" t="n">
-        <v>-11.11698676702065</v>
+        <v>-6.017905914702954</v>
       </c>
       <c r="X5" t="n">
-        <v>-7.024427682695825</v>
+        <v>-6.595175764148705</v>
       </c>
       <c r="Y5" t="n">
-        <v>-3.753213486751616</v>
+        <v>-1.956286616815378</v>
       </c>
       <c r="Z5" t="n">
-        <v>13.73796377622137</v>
+        <v>-9.555561328293841</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.8573603035361135</v>
+        <v>-6.634191122382017</v>
       </c>
       <c r="AB5" t="n">
-        <v>4.17797802298842</v>
+        <v>-7.982494735583884</v>
       </c>
       <c r="AC5" t="n">
-        <v>-12.89907689256381</v>
+        <v>-2.900855680143348</v>
       </c>
     </row>
     <row r="6">
@@ -1877,88 +1877,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>18.4401846518541</v>
+        <v>0.4683299132077314</v>
       </c>
       <c r="C6" t="n">
-        <v>-6.150587008608293</v>
+        <v>-3.151189683488103</v>
       </c>
       <c r="D6" t="n">
-        <v>-3.924958097387672</v>
+        <v>1.993095467518601</v>
       </c>
       <c r="E6" t="n">
-        <v>3.766617717812798</v>
+        <v>1.967641343959416</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.234672552232434</v>
+        <v>-5.810249663947443</v>
       </c>
       <c r="G6" t="n">
-        <v>-15.07776567605433</v>
+        <v>-3.89400144013814</v>
       </c>
       <c r="H6" t="n">
-        <v>3.456250992684136</v>
+        <v>-2.633359213206711</v>
       </c>
       <c r="I6" t="n">
-        <v>-20.23267781255048</v>
+        <v>3.621102886878688</v>
       </c>
       <c r="J6" t="n">
-        <v>-19.52335523172497</v>
+        <v>4.826653512521098</v>
       </c>
       <c r="K6" t="n">
-        <v>-3.547447395729943</v>
+        <v>0.2785647415433309</v>
       </c>
       <c r="L6" t="n">
-        <v>1.765053511039139</v>
+        <v>5.426513348954369</v>
       </c>
       <c r="M6" t="n">
-        <v>-6.156080600940907</v>
+        <v>-1.258992020779643</v>
       </c>
       <c r="N6" t="n">
-        <v>-2.934395947056335</v>
+        <v>-4.696988852796188</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.337270924805789</v>
+        <v>-6.649920924719382</v>
       </c>
       <c r="P6" t="n">
-        <v>1.491518503012746</v>
+        <v>0.90462590098412</v>
       </c>
       <c r="Q6" t="n">
-        <v>-7.108608720298049</v>
+        <v>-3.747442024131419</v>
       </c>
       <c r="R6" t="n">
-        <v>-9.156337668644035</v>
+        <v>1.167596770552644</v>
       </c>
       <c r="S6" t="n">
-        <v>3.838896899643307</v>
+        <v>-5.700473351068956</v>
       </c>
       <c r="T6" t="n">
-        <v>-7.581885959570799</v>
+        <v>3.707032800708575</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8524986813955251</v>
+        <v>-1.166850646729945</v>
       </c>
       <c r="V6" t="n">
-        <v>-7.563215938437746</v>
+        <v>-4.853371777422474</v>
       </c>
       <c r="W6" t="n">
-        <v>-11.9098593723729</v>
+        <v>-2.756233678319231</v>
       </c>
       <c r="X6" t="n">
-        <v>-5.465884469499989</v>
+        <v>-1.846325856985123</v>
       </c>
       <c r="Y6" t="n">
-        <v>-3.093702025499964</v>
+        <v>-2.049913512606953</v>
       </c>
       <c r="Z6" t="n">
-        <v>12.73787021212637</v>
+        <v>-6.822136772544708</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.3827529485764076</v>
+        <v>-4.537102851954559</v>
       </c>
       <c r="AB6" t="n">
-        <v>4.947488522940082</v>
+        <v>-3.845915617003623</v>
       </c>
       <c r="AC6" t="n">
-        <v>-13.04264888814803</v>
+        <v>-2.959013717010996</v>
       </c>
     </row>
     <row r="7">
@@ -1966,88 +1966,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>18.06117833311864</v>
+        <v>-3.364582431218789</v>
       </c>
       <c r="C7" t="n">
-        <v>-8.408198491391103</v>
+        <v>-5.365074799214037</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.159417579528711</v>
+        <v>-2.251646666721208</v>
       </c>
       <c r="E7" t="n">
-        <v>2.923393891631036</v>
+        <v>-0.3712906616832337</v>
       </c>
       <c r="F7" t="n">
-        <v>-2.783872803658633</v>
+        <v>-6.195861075786995</v>
       </c>
       <c r="G7" t="n">
-        <v>-14.74545104782752</v>
+        <v>-5.323470309610887</v>
       </c>
       <c r="H7" t="n">
-        <v>1.545447635041748</v>
+        <v>-5.464993774120474</v>
       </c>
       <c r="I7" t="n">
-        <v>-21.01020852996496</v>
+        <v>0.744277775470084</v>
       </c>
       <c r="J7" t="n">
-        <v>-19.19117798882987</v>
+        <v>1.876313548577223</v>
       </c>
       <c r="K7" t="n">
-        <v>-3.501276163988181</v>
+        <v>-3.691751757443634</v>
       </c>
       <c r="L7" t="n">
-        <v>3.155630785915084</v>
+        <v>0.2189978260785557</v>
       </c>
       <c r="M7" t="n">
-        <v>-6.902757443293874</v>
+        <v>-5.178884295615966</v>
       </c>
       <c r="N7" t="n">
-        <v>-2.574972608017441</v>
+        <v>-5.640932627454033</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.2656109178575035</v>
+        <v>-6.826137920366616</v>
       </c>
       <c r="P7" t="n">
-        <v>4.431589926570801</v>
+        <v>-2.848134178028599</v>
       </c>
       <c r="Q7" t="n">
-        <v>-4.251344794941256</v>
+        <v>-5.826668785744792</v>
       </c>
       <c r="R7" t="n">
-        <v>-9.224125455733265</v>
+        <v>-0.9912499525140346</v>
       </c>
       <c r="S7" t="n">
-        <v>2.470427075940603</v>
+        <v>-8.424242434813214</v>
       </c>
       <c r="T7" t="n">
-        <v>-9.895353367083001</v>
+        <v>0.7032485832593904</v>
       </c>
       <c r="U7" t="n">
-        <v>1.465018456585525</v>
+        <v>-4.781484338996088</v>
       </c>
       <c r="V7" t="n">
-        <v>-7.261393535840777</v>
+        <v>-7.674722865299287</v>
       </c>
       <c r="W7" t="n">
-        <v>-9.873014893168939</v>
+        <v>-6.299893078623837</v>
       </c>
       <c r="X7" t="n">
-        <v>-5.554877043626924</v>
+        <v>-7.793060266505037</v>
       </c>
       <c r="Y7" t="n">
-        <v>-3.700949458856035</v>
+        <v>-3.006497557325553</v>
       </c>
       <c r="Z7" t="n">
-        <v>13.52987950596424</v>
+        <v>-10.44138074068182</v>
       </c>
       <c r="AA7" t="n">
-        <v>-1.071404630901701</v>
+        <v>-5.426406458900496</v>
       </c>
       <c r="AB7" t="n">
-        <v>4.59532044427843</v>
+        <v>-8.116127393969599</v>
       </c>
       <c r="AC7" t="n">
-        <v>-13.98868896652222</v>
+        <v>-2.649513293292382</v>
       </c>
     </row>
     <row r="8">
@@ -2055,88 +2055,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>14.46545461348884</v>
+        <v>-3.151928855012915</v>
       </c>
       <c r="C8" t="n">
-        <v>-8.79909200947262</v>
+        <v>-6.712168170167446</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.180164659267599</v>
+        <v>-1.939505007477458</v>
       </c>
       <c r="E8" t="n">
-        <v>4.522378902259005</v>
+        <v>-1.973500984068051</v>
       </c>
       <c r="F8" t="n">
-        <v>-3.557531608685616</v>
+        <v>-8.55453910652844</v>
       </c>
       <c r="G8" t="n">
-        <v>-15.35717753823863</v>
+        <v>-5.340705304355114</v>
       </c>
       <c r="H8" t="n">
-        <v>1.292585346167598</v>
+        <v>-5.751725889451284</v>
       </c>
       <c r="I8" t="n">
-        <v>-23.19667014036774</v>
+        <v>-0.2951434199068377</v>
       </c>
       <c r="J8" t="n">
-        <v>-19.76720161514999</v>
+        <v>2.155639943072104</v>
       </c>
       <c r="K8" t="n">
-        <v>-3.380960565534672</v>
+        <v>-4.777627846130311</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7429976963933389</v>
+        <v>-0.4381315294280279</v>
       </c>
       <c r="M8" t="n">
-        <v>-5.701349594812908</v>
+        <v>-3.068535045654614</v>
       </c>
       <c r="N8" t="n">
-        <v>-4.016779093079797</v>
+        <v>-6.194831164878726</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8096796638140784</v>
+        <v>-4.826068548369197</v>
       </c>
       <c r="P8" t="n">
-        <v>2.250026583761316</v>
+        <v>-3.335220534160649</v>
       </c>
       <c r="Q8" t="n">
-        <v>-5.87143080077413</v>
+        <v>-6.392210266356443</v>
       </c>
       <c r="R8" t="n">
-        <v>-9.793690355868247</v>
+        <v>-4.472700731445444</v>
       </c>
       <c r="S8" t="n">
-        <v>0.7757422195845414</v>
+        <v>-10.19737072423963</v>
       </c>
       <c r="T8" t="n">
-        <v>-8.763227521990894</v>
+        <v>0.4363259740397512</v>
       </c>
       <c r="U8" t="n">
-        <v>1.013876613464367</v>
+        <v>-6.25692392523174</v>
       </c>
       <c r="V8" t="n">
-        <v>-6.580179954455257</v>
+        <v>-9.142923664611034</v>
       </c>
       <c r="W8" t="n">
-        <v>-10.8433298769826</v>
+        <v>-5.756023599520257</v>
       </c>
       <c r="X8" t="n">
-        <v>-5.149002375238927</v>
+        <v>-6.556907206943179</v>
       </c>
       <c r="Y8" t="n">
-        <v>-2.88054145963446</v>
+        <v>-4.545511640807442</v>
       </c>
       <c r="Z8" t="n">
-        <v>11.88410578825684</v>
+        <v>-9.765283025942765</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.6011017056205619</v>
+        <v>-8.920434811837552</v>
       </c>
       <c r="AB8" t="n">
-        <v>3.422149956519359</v>
+        <v>-6.150568038110202</v>
       </c>
       <c r="AC8" t="n">
-        <v>-15.77374895441607</v>
+        <v>-5.237999960502909</v>
       </c>
     </row>
     <row r="9">
@@ -2144,88 +2144,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>17.34309386404055</v>
+        <v>3.294036055565201</v>
       </c>
       <c r="C9" t="n">
-        <v>-10.1879629740546</v>
+        <v>-4.03544236651368</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.048813949778206</v>
+        <v>2.887108148939694</v>
       </c>
       <c r="E9" t="n">
-        <v>4.351995728710372</v>
+        <v>0.8349422396149982</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.794783157429226</v>
+        <v>-2.678743982927048</v>
       </c>
       <c r="G9" t="n">
-        <v>-13.97176006582244</v>
+        <v>-1.283663988995016</v>
       </c>
       <c r="H9" t="n">
-        <v>2.949519352447306</v>
+        <v>-2.360589818967857</v>
       </c>
       <c r="I9" t="n">
-        <v>-19.32613876171793</v>
+        <v>5.506072891581881</v>
       </c>
       <c r="J9" t="n">
-        <v>-17.82339642374711</v>
+        <v>6.270010181094366</v>
       </c>
       <c r="K9" t="n">
-        <v>-3.261762399869323</v>
+        <v>0.8265834545038613</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.24647128397533</v>
+        <v>4.466762987505165</v>
       </c>
       <c r="M9" t="n">
-        <v>-6.555383926371476</v>
+        <v>0.08699924037136542</v>
       </c>
       <c r="N9" t="n">
-        <v>-5.250840221259693</v>
+        <v>-1.41840326662469</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9194265532273465</v>
+        <v>-0.3261443576926659</v>
       </c>
       <c r="P9" t="n">
-        <v>1.955633960221289</v>
+        <v>0.1262952755579858</v>
       </c>
       <c r="Q9" t="n">
-        <v>-4.124096880647417</v>
+        <v>-1.454038725977885</v>
       </c>
       <c r="R9" t="n">
-        <v>-9.585289446091629</v>
+        <v>1.585602337049582</v>
       </c>
       <c r="S9" t="n">
-        <v>2.594304933755851</v>
+        <v>-4.078409997820755</v>
       </c>
       <c r="T9" t="n">
-        <v>-10.75024937324942</v>
+        <v>3.722052844033621</v>
       </c>
       <c r="U9" t="n">
-        <v>3.4572053456851</v>
+        <v>-0.9053400810041508</v>
       </c>
       <c r="V9" t="n">
-        <v>-5.412579535193903</v>
+        <v>-4.051051373324423</v>
       </c>
       <c r="W9" t="n">
-        <v>-10.46583974295816</v>
+        <v>-1.154515731908194</v>
       </c>
       <c r="X9" t="n">
-        <v>-3.937830426850174</v>
+        <v>-3.049138132097052</v>
       </c>
       <c r="Y9" t="n">
-        <v>-1.473525862779714</v>
+        <v>0.7082186751469424</v>
       </c>
       <c r="Z9" t="n">
-        <v>15.17519763217135</v>
+        <v>-4.431813274623834</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.6701579828637394</v>
+        <v>-3.340264898982113</v>
       </c>
       <c r="AB9" t="n">
-        <v>5.195131980509358</v>
+        <v>-2.374692917244388</v>
       </c>
       <c r="AC9" t="n">
-        <v>-12.73183277306354</v>
+        <v>-0.4293236260848747</v>
       </c>
     </row>
     <row r="10">
@@ -2233,88 +2233,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>18.88246445693753</v>
+        <v>-0.725297013619782</v>
       </c>
       <c r="C10" t="n">
-        <v>-10.53983468770544</v>
+        <v>-7.399430661741725</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.218369579543585</v>
+        <v>-1.665218982159704</v>
       </c>
       <c r="E10" t="n">
-        <v>4.320303276887742</v>
+        <v>-1.822543998315759</v>
       </c>
       <c r="F10" t="n">
-        <v>-2.671644800466535</v>
+        <v>-6.630894962721269</v>
       </c>
       <c r="G10" t="n">
-        <v>-13.61845552953149</v>
+        <v>-6.594332402743688</v>
       </c>
       <c r="H10" t="n">
-        <v>2.337340272206443</v>
+        <v>-6.941292067383948</v>
       </c>
       <c r="I10" t="n">
-        <v>-20.45544284217544</v>
+        <v>1.494776028795632</v>
       </c>
       <c r="J10" t="n">
-        <v>-17.91074860348461</v>
+        <v>2.760364574123642</v>
       </c>
       <c r="K10" t="n">
-        <v>-5.435375523242164</v>
+        <v>-1.433876776190391</v>
       </c>
       <c r="L10" t="n">
-        <v>0.2428245534378091</v>
+        <v>-0.4197669463957685</v>
       </c>
       <c r="M10" t="n">
-        <v>-7.334362011457928</v>
+        <v>-3.404381288330781</v>
       </c>
       <c r="N10" t="n">
-        <v>-4.194095086798195</v>
+        <v>-6.019830491810713</v>
       </c>
       <c r="O10" t="n">
-        <v>0.1262741435411319</v>
+        <v>-5.514133026952914</v>
       </c>
       <c r="P10" t="n">
-        <v>1.924387723579986</v>
+        <v>-3.519758916737507</v>
       </c>
       <c r="Q10" t="n">
-        <v>-3.245067060336284</v>
+        <v>-5.871276859825762</v>
       </c>
       <c r="R10" t="n">
-        <v>-8.415493670390351</v>
+        <v>-0.8416680767292708</v>
       </c>
       <c r="S10" t="n">
-        <v>1.702050414269175</v>
+        <v>-7.294988249217768</v>
       </c>
       <c r="T10" t="n">
-        <v>-9.373913261778794</v>
+        <v>0.6046493393941939</v>
       </c>
       <c r="U10" t="n">
-        <v>1.569027089378332</v>
+        <v>-5.023561797487723</v>
       </c>
       <c r="V10" t="n">
-        <v>-6.070520006175636</v>
+        <v>-7.155287482795969</v>
       </c>
       <c r="W10" t="n">
-        <v>-10.03862928418067</v>
+        <v>-8.290605270723443</v>
       </c>
       <c r="X10" t="n">
-        <v>-4.37727945013542</v>
+        <v>-6.683563278380445</v>
       </c>
       <c r="Y10" t="n">
-        <v>-3.373936862306573</v>
+        <v>-5.239108832892147</v>
       </c>
       <c r="Z10" t="n">
-        <v>14.20784948955467</v>
+        <v>-8.23768116089933</v>
       </c>
       <c r="AA10" t="n">
-        <v>-0.973573076573599</v>
+        <v>-5.689109214518346</v>
       </c>
       <c r="AB10" t="n">
-        <v>5.044517136517763</v>
+        <v>-5.736658490743015</v>
       </c>
       <c r="AC10" t="n">
-        <v>-14.18833798152048</v>
+        <v>-4.380497780280019</v>
       </c>
     </row>
     <row r="11">
@@ -2322,88 +2322,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>14.39526934208785</v>
+        <v>-3.601479636925513</v>
       </c>
       <c r="C11" t="n">
-        <v>-6.970670747275994</v>
+        <v>-3.724157481580981</v>
       </c>
       <c r="D11" t="n">
-        <v>-4.023757878161371</v>
+        <v>-1.696326747531093</v>
       </c>
       <c r="E11" t="n">
-        <v>2.745578194932317</v>
+        <v>-3.099282033884496</v>
       </c>
       <c r="F11" t="n">
-        <v>-3.277047007142355</v>
+        <v>-7.248501734385076</v>
       </c>
       <c r="G11" t="n">
-        <v>-14.01941111081195</v>
+        <v>-4.925649236810915</v>
       </c>
       <c r="H11" t="n">
-        <v>2.191424304184737</v>
+        <v>-7.091917474263788</v>
       </c>
       <c r="I11" t="n">
-        <v>-20.36257599291497</v>
+        <v>3.219100756492281</v>
       </c>
       <c r="J11" t="n">
-        <v>-20.62332079988082</v>
+        <v>0.8483566578949082</v>
       </c>
       <c r="K11" t="n">
-        <v>-2.946206705165964</v>
+        <v>-4.13415356830274</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.1914215563262407</v>
+        <v>0.3248323156686816</v>
       </c>
       <c r="M11" t="n">
-        <v>-6.677325763711103</v>
+        <v>-2.073059512804826</v>
       </c>
       <c r="N11" t="n">
-        <v>-4.728844610780051</v>
+        <v>-4.880883402141144</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.3556223103348304</v>
+        <v>-6.38643072016721</v>
       </c>
       <c r="P11" t="n">
-        <v>1.477631447900896</v>
+        <v>-2.556152152859179</v>
       </c>
       <c r="Q11" t="n">
-        <v>-5.711796545685422</v>
+        <v>-5.535600573067315</v>
       </c>
       <c r="R11" t="n">
-        <v>-10.09359591570766</v>
+        <v>-0.3246452611715669</v>
       </c>
       <c r="S11" t="n">
-        <v>1.595580855035731</v>
+        <v>-8.181687225033309</v>
       </c>
       <c r="T11" t="n">
-        <v>-9.223945395925874</v>
+        <v>0.7635704509762169</v>
       </c>
       <c r="U11" t="n">
-        <v>1.934153584457774</v>
+        <v>-4.810424512911117</v>
       </c>
       <c r="V11" t="n">
-        <v>-6.452304236101971</v>
+        <v>-6.960356767389039</v>
       </c>
       <c r="W11" t="n">
-        <v>-12.14759258267853</v>
+        <v>-6.086088554031262</v>
       </c>
       <c r="X11" t="n">
-        <v>-4.223342938054854</v>
+        <v>-7.189900749072761</v>
       </c>
       <c r="Y11" t="n">
-        <v>-2.350766848609481</v>
+        <v>-4.345189628026935</v>
       </c>
       <c r="Z11" t="n">
-        <v>12.90649797236187</v>
+        <v>-8.713029219376653</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.8837959196796081</v>
+        <v>-6.921023741428662</v>
       </c>
       <c r="AB11" t="n">
-        <v>4.72300243636633</v>
+        <v>-5.589694479656585</v>
       </c>
       <c r="AC11" t="n">
-        <v>-12.72557155931403</v>
+        <v>-3.472248717910272</v>
       </c>
     </row>
   </sheetData>
@@ -2516,88 +2516,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-5.625236089776784</v>
+        <v>-0.2192360798642401</v>
       </c>
       <c r="C2" t="n">
-        <v>-4.492804866806801</v>
+        <v>3.932829207289005</v>
       </c>
       <c r="D2" t="n">
-        <v>-4.713966740853254</v>
+        <v>-0.5497069068155274</v>
       </c>
       <c r="E2" t="n">
-        <v>1.203317352989799</v>
+        <v>-0.3688396474673852</v>
       </c>
       <c r="F2" t="n">
-        <v>-14.06284944644749</v>
+        <v>-3.315153807549311</v>
       </c>
       <c r="G2" t="n">
-        <v>-12.78727537594284</v>
+        <v>-3.850868759059056</v>
       </c>
       <c r="H2" t="n">
-        <v>2.814965286016304</v>
+        <v>-4.19932036599381</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.53913221659873</v>
+        <v>-1.8840779232556</v>
       </c>
       <c r="J2" t="n">
-        <v>-8.563753893333859</v>
+        <v>-0.3644486126276298</v>
       </c>
       <c r="K2" t="n">
-        <v>1.488950011511102</v>
+        <v>0.7920757472293483</v>
       </c>
       <c r="L2" t="n">
-        <v>-11.38646500702958</v>
+        <v>-3.338293812148726</v>
       </c>
       <c r="M2" t="n">
-        <v>4.423955762620237</v>
+        <v>-5.779200440115058</v>
       </c>
       <c r="N2" t="n">
-        <v>-8.128517429177702</v>
+        <v>-2.084545132723243</v>
       </c>
       <c r="O2" t="n">
-        <v>-5.240345259732992</v>
+        <v>-4.944836424646981</v>
       </c>
       <c r="P2" t="n">
-        <v>-13.03817715404549</v>
+        <v>-1.787918613131159</v>
       </c>
       <c r="Q2" t="n">
-        <v>-13.78024308438627</v>
+        <v>1.433325943204848</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.7503579798194071</v>
+        <v>-2.409601001138493</v>
       </c>
       <c r="S2" t="n">
-        <v>-11.78761853554003</v>
+        <v>-1.833102456807632</v>
       </c>
       <c r="T2" t="n">
-        <v>-12.22987088733476</v>
+        <v>-5.279972693434644</v>
       </c>
       <c r="U2" t="n">
-        <v>6.38124098023076</v>
+        <v>-1.606754036742478</v>
       </c>
       <c r="V2" t="n">
-        <v>-9.971296061096416</v>
+        <v>-3.073784580791491</v>
       </c>
       <c r="W2" t="n">
-        <v>-7.901048654200913</v>
+        <v>-0.8225710767341248</v>
       </c>
       <c r="X2" t="n">
-        <v>-16.3878612140004</v>
+        <v>-2.739185998660152</v>
       </c>
       <c r="Y2" t="n">
-        <v>-1.828921386879244</v>
+        <v>-3.64781884626753</v>
       </c>
       <c r="Z2" t="n">
-        <v>-6.595812862720742</v>
+        <v>-6.904062910307508</v>
       </c>
       <c r="AA2" t="n">
-        <v>-27.39268680411794</v>
+        <v>-13.11511786421644</v>
       </c>
       <c r="AB2" t="n">
-        <v>-6.291168289940297</v>
+        <v>-12.19734349013965</v>
       </c>
       <c r="AC2" t="n">
-        <v>-19.80186137763567</v>
+        <v>-26.77351080235648</v>
       </c>
     </row>
     <row r="3">
@@ -2605,88 +2605,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-6.818883773261904</v>
+        <v>-4.488234091521339</v>
       </c>
       <c r="C3" t="n">
-        <v>-5.372510623441075</v>
+        <v>0.9339154178312921</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.368929407152529</v>
+        <v>-4.91070662986446</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5252353418916407</v>
+        <v>-4.870848464669735</v>
       </c>
       <c r="F3" t="n">
-        <v>-15.00014171096014</v>
+        <v>-7.190109679316423</v>
       </c>
       <c r="G3" t="n">
-        <v>-11.20677851816033</v>
+        <v>-8.787236897861955</v>
       </c>
       <c r="H3" t="n">
-        <v>3.272069460222101</v>
+        <v>-11.38112766444931</v>
       </c>
       <c r="I3" t="n">
-        <v>-3.390386788649379</v>
+        <v>-6.480512682866273</v>
       </c>
       <c r="J3" t="n">
-        <v>-9.661424112147625</v>
+        <v>-4.997010370269642</v>
       </c>
       <c r="K3" t="n">
-        <v>3.563205879808467</v>
+        <v>-4.785361840741272</v>
       </c>
       <c r="L3" t="n">
-        <v>-10.48280988227735</v>
+        <v>-8.563848579015117</v>
       </c>
       <c r="M3" t="n">
-        <v>4.051915199238149</v>
+        <v>-11.48972087050335</v>
       </c>
       <c r="N3" t="n">
-        <v>-9.114230651989303</v>
+        <v>-6.605096512894963</v>
       </c>
       <c r="O3" t="n">
-        <v>-6.436374722914955</v>
+        <v>-6.796962517912295</v>
       </c>
       <c r="P3" t="n">
-        <v>-13.2941314263707</v>
+        <v>-8.391116120410548</v>
       </c>
       <c r="Q3" t="n">
-        <v>-13.10836807070307</v>
+        <v>-5.087295131984782</v>
       </c>
       <c r="R3" t="n">
-        <v>-1.053363912535194</v>
+        <v>-6.747174498243846</v>
       </c>
       <c r="S3" t="n">
-        <v>-12.18358353125703</v>
+        <v>-7.537533357603952</v>
       </c>
       <c r="T3" t="n">
-        <v>-11.75816231033135</v>
+        <v>-10.62296631719891</v>
       </c>
       <c r="U3" t="n">
-        <v>3.948180534477614</v>
+        <v>-6.671499566544768</v>
       </c>
       <c r="V3" t="n">
-        <v>-11.24216040821767</v>
+        <v>-8.191181385388584</v>
       </c>
       <c r="W3" t="n">
-        <v>-6.205397729379446</v>
+        <v>-7.862039044823195</v>
       </c>
       <c r="X3" t="n">
-        <v>-15.35892040533156</v>
+        <v>-6.056807672408887</v>
       </c>
       <c r="Y3" t="n">
-        <v>-3.221889975387329</v>
+        <v>-10.61578322207663</v>
       </c>
       <c r="Z3" t="n">
-        <v>-7.58937915628077</v>
+        <v>-10.07794347628271</v>
       </c>
       <c r="AA3" t="n">
-        <v>-26.61643965109187</v>
+        <v>-18.12394404799697</v>
       </c>
       <c r="AB3" t="n">
-        <v>-9.798801387419182</v>
+        <v>-18.03838776936672</v>
       </c>
       <c r="AC3" t="n">
-        <v>-18.33582224848669</v>
+        <v>-29.99186591685859</v>
       </c>
     </row>
     <row r="4">
@@ -2694,88 +2694,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-6.577149976098827</v>
+        <v>0.8884027924239324</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.84254589086262</v>
+        <v>3.094157592811216</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.126286625305527</v>
+        <v>-1.731124630146192</v>
       </c>
       <c r="E4" t="n">
-        <v>1.426689940638771</v>
+        <v>-0.1667799561675105</v>
       </c>
       <c r="F4" t="n">
-        <v>-13.01651984368936</v>
+        <v>-4.198143015164398</v>
       </c>
       <c r="G4" t="n">
-        <v>-9.920468128188951</v>
+        <v>-6.789096264620001</v>
       </c>
       <c r="H4" t="n">
-        <v>2.707003519207431</v>
+        <v>-2.890938398931994</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.281426627988874</v>
+        <v>-2.399985638104661</v>
       </c>
       <c r="J4" t="n">
-        <v>-10.68827321018486</v>
+        <v>0.1718709096857269</v>
       </c>
       <c r="K4" t="n">
-        <v>3.109659809836429</v>
+        <v>-0.5836572902495778</v>
       </c>
       <c r="L4" t="n">
-        <v>-7.814209627484809</v>
+        <v>-4.974185944031365</v>
       </c>
       <c r="M4" t="n">
-        <v>3.339333410705613</v>
+        <v>-8.398400501097933</v>
       </c>
       <c r="N4" t="n">
-        <v>-7.861108158834494</v>
+        <v>-3.752713624733567</v>
       </c>
       <c r="O4" t="n">
-        <v>-4.824517096675294</v>
+        <v>-3.551037719549174</v>
       </c>
       <c r="P4" t="n">
-        <v>-11.46419735514247</v>
+        <v>-1.994631289746989</v>
       </c>
       <c r="Q4" t="n">
-        <v>-13.30110365178605</v>
+        <v>0.2868211069140063</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1951328909401382</v>
+        <v>-1.993688388556705</v>
       </c>
       <c r="S4" t="n">
-        <v>-12.26144680907025</v>
+        <v>-4.481105334496869</v>
       </c>
       <c r="T4" t="n">
-        <v>-11.96877888669006</v>
+        <v>-7.391729438522151</v>
       </c>
       <c r="U4" t="n">
-        <v>7.239012983944118</v>
+        <v>-1.446513957212687</v>
       </c>
       <c r="V4" t="n">
-        <v>-10.99581300095454</v>
+        <v>-3.544553176232637</v>
       </c>
       <c r="W4" t="n">
-        <v>-6.517114725015108</v>
+        <v>-3.486902211223833</v>
       </c>
       <c r="X4" t="n">
-        <v>-17.53393828335611</v>
+        <v>-2.352193530868212</v>
       </c>
       <c r="Y4" t="n">
-        <v>-4.565812851299319</v>
+        <v>-6.463080794596896</v>
       </c>
       <c r="Z4" t="n">
-        <v>-6.187734418891328</v>
+        <v>-6.817761357164551</v>
       </c>
       <c r="AA4" t="n">
-        <v>-25.40702851653849</v>
+        <v>-14.6541137446198</v>
       </c>
       <c r="AB4" t="n">
-        <v>-8.221784165018422</v>
+        <v>-13.78455156276005</v>
       </c>
       <c r="AC4" t="n">
-        <v>-19.53115493713051</v>
+        <v>-24.7093680593986</v>
       </c>
     </row>
     <row r="5">
@@ -2783,88 +2783,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-7.936111302687825</v>
+        <v>-1.037232961635761</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.895449169464842</v>
+        <v>1.498204538189374</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.263112850524579</v>
+        <v>-1.57304656248288</v>
       </c>
       <c r="E5" t="n">
-        <v>1.355114777011556</v>
+        <v>-0.7662261628781515</v>
       </c>
       <c r="F5" t="n">
-        <v>-12.81354458248061</v>
+        <v>-7.958019404157573</v>
       </c>
       <c r="G5" t="n">
-        <v>-11.67688882982877</v>
+        <v>-7.328858568074191</v>
       </c>
       <c r="H5" t="n">
-        <v>2.090104280098602</v>
+        <v>-7.49095144434194</v>
       </c>
       <c r="I5" t="n">
-        <v>-2.921948632120482</v>
+        <v>-5.538477767960431</v>
       </c>
       <c r="J5" t="n">
-        <v>-9.265923187073209</v>
+        <v>-2.079440786600828</v>
       </c>
       <c r="K5" t="n">
-        <v>2.396944602740177</v>
+        <v>-1.095781272762849</v>
       </c>
       <c r="L5" t="n">
-        <v>-7.886432883505679</v>
+        <v>-4.580864851266332</v>
       </c>
       <c r="M5" t="n">
-        <v>2.281685840803264</v>
+        <v>-10.11524399592979</v>
       </c>
       <c r="N5" t="n">
-        <v>-8.441932340827353</v>
+        <v>-3.424050486577362</v>
       </c>
       <c r="O5" t="n">
-        <v>-6.186082268700011</v>
+        <v>-7.406950457591426</v>
       </c>
       <c r="P5" t="n">
-        <v>-12.23152380444628</v>
+        <v>-4.807863627142798</v>
       </c>
       <c r="Q5" t="n">
-        <v>-12.50049947678504</v>
+        <v>-3.104856758257314</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.6535831533651897</v>
+        <v>-3.531187525354487</v>
       </c>
       <c r="S5" t="n">
-        <v>-12.30761874478687</v>
+        <v>-3.161285610915692</v>
       </c>
       <c r="T5" t="n">
-        <v>-12.1831014301878</v>
+        <v>-9.758337188923399</v>
       </c>
       <c r="U5" t="n">
-        <v>3.975848884848237</v>
+        <v>-1.921037151353009</v>
       </c>
       <c r="V5" t="n">
-        <v>-10.61156376686587</v>
+        <v>-5.587218360518044</v>
       </c>
       <c r="W5" t="n">
-        <v>-7.658041451829229</v>
+        <v>-5.829926035968189</v>
       </c>
       <c r="X5" t="n">
-        <v>-16.44785058316933</v>
+        <v>-3.105121635137797</v>
       </c>
       <c r="Y5" t="n">
-        <v>-1.221050464013117</v>
+        <v>-8.583134664853862</v>
       </c>
       <c r="Z5" t="n">
-        <v>-8.836200761572334</v>
+        <v>-8.56640528861355</v>
       </c>
       <c r="AA5" t="n">
-        <v>-27.68346271763291</v>
+        <v>-16.03787911358906</v>
       </c>
       <c r="AB5" t="n">
-        <v>-8.664621425219382</v>
+        <v>-12.45074434123308</v>
       </c>
       <c r="AC5" t="n">
-        <v>-19.08343402808148</v>
+        <v>-28.26911494309371</v>
       </c>
     </row>
     <row r="6">
@@ -2872,88 +2872,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-7.08567176177534</v>
+        <v>-0.6034087560317271</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.649540344830688</v>
+        <v>3.608772351893525</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.255586109612517</v>
+        <v>-1.587877247904891</v>
       </c>
       <c r="E6" t="n">
-        <v>0.725118117428257</v>
+        <v>0.5328880856347098</v>
       </c>
       <c r="F6" t="n">
-        <v>-13.21249038820341</v>
+        <v>-5.266820642874016</v>
       </c>
       <c r="G6" t="n">
-        <v>-11.66417873205729</v>
+        <v>-4.233105935655685</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8273670033958274</v>
+        <v>-4.923560195624421</v>
       </c>
       <c r="I6" t="n">
-        <v>-2.786073701134428</v>
+        <v>-1.788851658672323</v>
       </c>
       <c r="J6" t="n">
-        <v>-9.543148242840068</v>
+        <v>1.549468797036089</v>
       </c>
       <c r="K6" t="n">
-        <v>2.529770891546195</v>
+        <v>-0.8435752911074741</v>
       </c>
       <c r="L6" t="n">
-        <v>-10.3836400872925</v>
+        <v>-4.030379559876737</v>
       </c>
       <c r="M6" t="n">
-        <v>4.875378230872986</v>
+        <v>-5.448280178912725</v>
       </c>
       <c r="N6" t="n">
-        <v>-9.430572262807392</v>
+        <v>-0.97354529949793</v>
       </c>
       <c r="O6" t="n">
-        <v>-5.455606548103056</v>
+        <v>-3.525291279374967</v>
       </c>
       <c r="P6" t="n">
-        <v>-10.55460815651818</v>
+        <v>-0.776391393425492</v>
       </c>
       <c r="Q6" t="n">
-        <v>-13.44564667120729</v>
+        <v>1.365520101088945</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1601442658475829</v>
+        <v>-0.6101121198049158</v>
       </c>
       <c r="S6" t="n">
-        <v>-11.85373722064415</v>
+        <v>-1.45787135006529</v>
       </c>
       <c r="T6" t="n">
-        <v>-13.56888587427268</v>
+        <v>-6.766277295167809</v>
       </c>
       <c r="U6" t="n">
-        <v>3.317018701188685</v>
+        <v>-0.7842643825244875</v>
       </c>
       <c r="V6" t="n">
-        <v>-10.21551454103358</v>
+        <v>-5.199802727947398</v>
       </c>
       <c r="W6" t="n">
-        <v>-6.379514119553577</v>
+        <v>-2.454565653844468</v>
       </c>
       <c r="X6" t="n">
-        <v>-16.91442713884609</v>
+        <v>-0.9141262114064901</v>
       </c>
       <c r="Y6" t="n">
-        <v>-3.436446022981291</v>
+        <v>-4.177194629668987</v>
       </c>
       <c r="Z6" t="n">
-        <v>-6.828959019404071</v>
+        <v>-6.776632629782704</v>
       </c>
       <c r="AA6" t="n">
-        <v>-26.0516026812103</v>
+        <v>-15.32328572484093</v>
       </c>
       <c r="AB6" t="n">
-        <v>-7.382764177251795</v>
+        <v>-11.07144868839621</v>
       </c>
       <c r="AC6" t="n">
-        <v>-20.49449588931284</v>
+        <v>-24.99009975284665</v>
       </c>
     </row>
     <row r="7">
@@ -2961,88 +2961,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-8.615125846761462</v>
+        <v>-0.7797687191348519</v>
       </c>
       <c r="C7" t="n">
-        <v>-6.155545757761051</v>
+        <v>1.106334910732926</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.057473078151852</v>
+        <v>-2.742807381729604</v>
       </c>
       <c r="E7" t="n">
-        <v>2.829511413657539</v>
+        <v>-2.172274040444718</v>
       </c>
       <c r="F7" t="n">
-        <v>-15.36436145665334</v>
+        <v>-6.788913905299843</v>
       </c>
       <c r="G7" t="n">
-        <v>-12.14151816072064</v>
+        <v>-6.451501018197147</v>
       </c>
       <c r="H7" t="n">
-        <v>1.737221146982148</v>
+        <v>-6.848694357175392</v>
       </c>
       <c r="I7" t="n">
-        <v>-3.56499233540253</v>
+        <v>-4.568478152164185</v>
       </c>
       <c r="J7" t="n">
-        <v>-9.112759131834185</v>
+        <v>-2.420810783583923</v>
       </c>
       <c r="K7" t="n">
-        <v>3.057691617038121</v>
+        <v>-1.211215949903835</v>
       </c>
       <c r="L7" t="n">
-        <v>-12.58360150463224</v>
+        <v>-7.04504626075967</v>
       </c>
       <c r="M7" t="n">
-        <v>2.700168831503466</v>
+        <v>-8.985282189256296</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.914273274860168</v>
+        <v>-4.309646323802127</v>
       </c>
       <c r="O7" t="n">
-        <v>-5.062212063698671</v>
+        <v>-5.733333714847717</v>
       </c>
       <c r="P7" t="n">
-        <v>-12.21032190345417</v>
+        <v>-3.649857681957848</v>
       </c>
       <c r="Q7" t="n">
-        <v>-13.45606897253007</v>
+        <v>-2.398966627333301</v>
       </c>
       <c r="R7" t="n">
-        <v>-1.161635980390625</v>
+        <v>-3.71105062168416</v>
       </c>
       <c r="S7" t="n">
-        <v>-12.70362659622453</v>
+        <v>-3.281995397817633</v>
       </c>
       <c r="T7" t="n">
-        <v>-14.9953192344393</v>
+        <v>-9.051621248072951</v>
       </c>
       <c r="U7" t="n">
-        <v>6.923646561016074</v>
+        <v>-2.110602738547324</v>
       </c>
       <c r="V7" t="n">
-        <v>-12.6267630920654</v>
+        <v>-5.258446576359384</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.771769279628653</v>
+        <v>-5.775776825046653</v>
       </c>
       <c r="X7" t="n">
-        <v>-16.63329244777516</v>
+        <v>-4.45923251081748</v>
       </c>
       <c r="Y7" t="n">
-        <v>-3.210379950150933</v>
+        <v>-7.921096470270614</v>
       </c>
       <c r="Z7" t="n">
-        <v>-5.905990818943131</v>
+        <v>-8.232438927948863</v>
       </c>
       <c r="AA7" t="n">
-        <v>-27.47546556318177</v>
+        <v>-16.01684205806386</v>
       </c>
       <c r="AB7" t="n">
-        <v>-9.046575940021771</v>
+        <v>-13.87592365556315</v>
       </c>
       <c r="AC7" t="n">
-        <v>-20.21670086955524</v>
+        <v>-29.24522953562117</v>
       </c>
     </row>
     <row r="8">
@@ -3050,88 +3050,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.299926586843922</v>
+        <v>-3.497336815771669</v>
       </c>
       <c r="C8" t="n">
-        <v>-6.827812898721437</v>
+        <v>-0.4239202831708275</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.032454541942204</v>
+        <v>-1.915619286817837</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2974517181959255</v>
+        <v>-2.808758189121256</v>
       </c>
       <c r="F8" t="n">
-        <v>-12.84065354440332</v>
+        <v>-8.859571336999316</v>
       </c>
       <c r="G8" t="n">
-        <v>-13.99021736801504</v>
+        <v>-7.497996013633128</v>
       </c>
       <c r="H8" t="n">
-        <v>2.158945582377878</v>
+        <v>-8.638247214112791</v>
       </c>
       <c r="I8" t="n">
-        <v>-2.013872113900789</v>
+        <v>-5.826058566477866</v>
       </c>
       <c r="J8" t="n">
-        <v>-9.937641874022187</v>
+        <v>-3.351854447657033</v>
       </c>
       <c r="K8" t="n">
-        <v>1.582005331774441</v>
+        <v>-3.520943813695574</v>
       </c>
       <c r="L8" t="n">
-        <v>-9.329658394848437</v>
+        <v>-7.298203767088231</v>
       </c>
       <c r="M8" t="n">
-        <v>4.333857759329925</v>
+        <v>-10.11405260438208</v>
       </c>
       <c r="N8" t="n">
-        <v>-8.523535336970319</v>
+        <v>-4.650484887787235</v>
       </c>
       <c r="O8" t="n">
-        <v>-5.934677989867392</v>
+        <v>-8.198477053385536</v>
       </c>
       <c r="P8" t="n">
-        <v>-11.66751092705597</v>
+        <v>-4.131974037610242</v>
       </c>
       <c r="Q8" t="n">
-        <v>-12.87920393085149</v>
+        <v>-3.799895232953336</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.4664457940986719</v>
+        <v>-5.56535431268846</v>
       </c>
       <c r="S8" t="n">
-        <v>-10.80277033875112</v>
+        <v>-3.323443410330103</v>
       </c>
       <c r="T8" t="n">
-        <v>-13.25958454342712</v>
+        <v>-10.68541104799367</v>
       </c>
       <c r="U8" t="n">
-        <v>6.225404415846988</v>
+        <v>-3.685594501379578</v>
       </c>
       <c r="V8" t="n">
-        <v>-9.958539160250584</v>
+        <v>-6.683597180356361</v>
       </c>
       <c r="W8" t="n">
-        <v>-6.249972697109444</v>
+        <v>-5.552075227323503</v>
       </c>
       <c r="X8" t="n">
-        <v>-18.52617701423971</v>
+        <v>-4.680844823062698</v>
       </c>
       <c r="Y8" t="n">
-        <v>-2.545551244676546</v>
+        <v>-9.09638942610278</v>
       </c>
       <c r="Z8" t="n">
-        <v>-6.318911461166802</v>
+        <v>-9.61643843507588</v>
       </c>
       <c r="AA8" t="n">
-        <v>-27.18173510509245</v>
+        <v>-17.24362768393093</v>
       </c>
       <c r="AB8" t="n">
-        <v>-8.717540819089944</v>
+        <v>-15.52905326032036</v>
       </c>
       <c r="AC8" t="n">
-        <v>-19.43647621383438</v>
+        <v>-27.96833972160688</v>
       </c>
     </row>
     <row r="9">
@@ -3139,88 +3139,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.159724254257917</v>
+        <v>2.321501256468058</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.608080989648451</v>
+        <v>5.69916095847807</v>
       </c>
       <c r="D9" t="n">
-        <v>-4.546301305201446</v>
+        <v>2.583575356621776</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5956319669226717</v>
+        <v>-0.1740157010920926</v>
       </c>
       <c r="F9" t="n">
-        <v>-14.40655854851215</v>
+        <v>-4.776107512678346</v>
       </c>
       <c r="G9" t="n">
-        <v>-11.75613910617066</v>
+        <v>-4.155097487360514</v>
       </c>
       <c r="H9" t="n">
-        <v>2.293709898305701</v>
+        <v>-2.137165300884776</v>
       </c>
       <c r="I9" t="n">
-        <v>-2.019216740271562</v>
+        <v>-0.5747391816900782</v>
       </c>
       <c r="J9" t="n">
-        <v>-9.293637565311618</v>
+        <v>1.334646507418773</v>
       </c>
       <c r="K9" t="n">
-        <v>2.565029370036655</v>
+        <v>2.042390564867019</v>
       </c>
       <c r="L9" t="n">
-        <v>-9.210916492149646</v>
+        <v>-3.925979211153975</v>
       </c>
       <c r="M9" t="n">
-        <v>4.872506153600864</v>
+        <v>-2.592985237143178</v>
       </c>
       <c r="N9" t="n">
-        <v>-8.345321430992163</v>
+        <v>1.752773815858947</v>
       </c>
       <c r="O9" t="n">
-        <v>-4.341359969311836</v>
+        <v>-3.460114593620195</v>
       </c>
       <c r="P9" t="n">
-        <v>-11.87797614267347</v>
+        <v>1.356270484092342</v>
       </c>
       <c r="Q9" t="n">
-        <v>-13.51525027468311</v>
+        <v>1.970256309676699</v>
       </c>
       <c r="R9" t="n">
-        <v>-1.14232425020868</v>
+        <v>-0.6189053137788862</v>
       </c>
       <c r="S9" t="n">
-        <v>-11.79853450039488</v>
+        <v>0.7373017505634403</v>
       </c>
       <c r="T9" t="n">
-        <v>-15.0145481397347</v>
+        <v>-4.478120751656885</v>
       </c>
       <c r="U9" t="n">
-        <v>4.987356892536513</v>
+        <v>1.484942009588107</v>
       </c>
       <c r="V9" t="n">
-        <v>-9.197067949227812</v>
+        <v>-3.210674440675641</v>
       </c>
       <c r="W9" t="n">
-        <v>-7.229536028097698</v>
+        <v>-2.91737069566406</v>
       </c>
       <c r="X9" t="n">
-        <v>-17.59005194518193</v>
+        <v>0.3413780882800248</v>
       </c>
       <c r="Y9" t="n">
-        <v>-2.564118925033186</v>
+        <v>-3.571726143339256</v>
       </c>
       <c r="Z9" t="n">
-        <v>-6.527505775908338</v>
+        <v>-5.29260045955489</v>
       </c>
       <c r="AA9" t="n">
-        <v>-25.94319784955529</v>
+        <v>-13.9698963679016</v>
       </c>
       <c r="AB9" t="n">
-        <v>-7.048301767423446</v>
+        <v>-11.01101969231705</v>
       </c>
       <c r="AC9" t="n">
-        <v>-17.47778807908902</v>
+        <v>-25.51130512839035</v>
       </c>
     </row>
     <row r="10">
@@ -3228,88 +3228,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.471966992872805</v>
+        <v>-2.18429866034467</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.777533999153452</v>
+        <v>1.224837972978936</v>
       </c>
       <c r="D10" t="n">
-        <v>-4.582481203173075</v>
+        <v>-0.3874946663050038</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6312624133700635</v>
+        <v>-3.282424587745585</v>
       </c>
       <c r="F10" t="n">
-        <v>-13.54413194673393</v>
+        <v>-6.418524223660762</v>
       </c>
       <c r="G10" t="n">
-        <v>-11.89163223649107</v>
+        <v>-7.472617432156625</v>
       </c>
       <c r="H10" t="n">
-        <v>2.865124542786676</v>
+        <v>-8.727713269742953</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.8684818442268925</v>
+        <v>-4.648658900744808</v>
       </c>
       <c r="J10" t="n">
-        <v>-10.23667331526461</v>
+        <v>-2.453924450183163</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7410905638845309</v>
+        <v>-2.32272792044179</v>
       </c>
       <c r="L10" t="n">
-        <v>-9.589653547399807</v>
+        <v>-8.719745017539868</v>
       </c>
       <c r="M10" t="n">
-        <v>3.532865117008764</v>
+        <v>-9.819081881922797</v>
       </c>
       <c r="N10" t="n">
-        <v>-8.306091898875096</v>
+        <v>-5.793573051843848</v>
       </c>
       <c r="O10" t="n">
-        <v>-5.041174295482772</v>
+        <v>-6.973256633338111</v>
       </c>
       <c r="P10" t="n">
-        <v>-11.56289191152655</v>
+        <v>-3.490294642903228</v>
       </c>
       <c r="Q10" t="n">
-        <v>-14.20303666383636</v>
+        <v>-3.027931083028234</v>
       </c>
       <c r="R10" t="n">
-        <v>0.1648068711340822</v>
+        <v>-4.738397547942506</v>
       </c>
       <c r="S10" t="n">
-        <v>-12.25564979648634</v>
+        <v>-4.502578436887663</v>
       </c>
       <c r="T10" t="n">
-        <v>-11.72788361132882</v>
+        <v>-8.835670671407389</v>
       </c>
       <c r="U10" t="n">
-        <v>7.453913935019592</v>
+        <v>-4.586270557802048</v>
       </c>
       <c r="V10" t="n">
-        <v>-11.72819620821181</v>
+        <v>-5.188276568780406</v>
       </c>
       <c r="W10" t="n">
-        <v>-6.940399847550059</v>
+        <v>-5.471715499594805</v>
       </c>
       <c r="X10" t="n">
-        <v>-16.48626042303003</v>
+        <v>-3.216295149262013</v>
       </c>
       <c r="Y10" t="n">
-        <v>-2.950341180881527</v>
+        <v>-8.23692341309609</v>
       </c>
       <c r="Z10" t="n">
-        <v>-5.496251044652269</v>
+        <v>-6.56580015135967</v>
       </c>
       <c r="AA10" t="n">
-        <v>-25.72884543653182</v>
+        <v>-16.64282593384941</v>
       </c>
       <c r="AB10" t="n">
-        <v>-7.597157904816182</v>
+        <v>-14.93569811352126</v>
       </c>
       <c r="AC10" t="n">
-        <v>-18.20968207724654</v>
+        <v>-27.65758951528124</v>
       </c>
     </row>
     <row r="11">
@@ -3317,88 +3317,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-7.32011811125771</v>
+        <v>-1.427574238537269</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.368631950442298</v>
+        <v>1.834311427721602</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.013048958529922</v>
+        <v>-2.20908447411592</v>
       </c>
       <c r="E11" t="n">
-        <v>2.256965039268387</v>
+        <v>-1.876431349391078</v>
       </c>
       <c r="F11" t="n">
-        <v>-13.7437638551725</v>
+        <v>-6.274967331157087</v>
       </c>
       <c r="G11" t="n">
-        <v>-11.90884766303352</v>
+        <v>-6.292649487229951</v>
       </c>
       <c r="H11" t="n">
-        <v>4.280563341720634</v>
+        <v>-7.023530873417693</v>
       </c>
       <c r="I11" t="n">
-        <v>-2.481826171198228</v>
+        <v>-2.835144882608922</v>
       </c>
       <c r="J11" t="n">
-        <v>-9.783734844454637</v>
+        <v>-0.3773303055323507</v>
       </c>
       <c r="K11" t="n">
-        <v>1.589096433140175</v>
+        <v>-3.085385939272279</v>
       </c>
       <c r="L11" t="n">
-        <v>-10.18433075460696</v>
+        <v>-6.622315321303926</v>
       </c>
       <c r="M11" t="n">
-        <v>3.419682432399803</v>
+        <v>-8.903854797820317</v>
       </c>
       <c r="N11" t="n">
-        <v>-8.948829860060492</v>
+        <v>-3.131205046106939</v>
       </c>
       <c r="O11" t="n">
-        <v>-5.410170774906486</v>
+        <v>-5.881692863159792</v>
       </c>
       <c r="P11" t="n">
-        <v>-12.94768789464042</v>
+        <v>-3.044897046998348</v>
       </c>
       <c r="Q11" t="n">
-        <v>-13.06812452867731</v>
+        <v>-1.35365637659571</v>
       </c>
       <c r="R11" t="n">
-        <v>0.9350412743278582</v>
+        <v>-2.972124630295163</v>
       </c>
       <c r="S11" t="n">
-        <v>-12.96605832212864</v>
+        <v>-2.921828440919924</v>
       </c>
       <c r="T11" t="n">
-        <v>-12.79596643688225</v>
+        <v>-8.346154121525259</v>
       </c>
       <c r="U11" t="n">
-        <v>5.597263014028109</v>
+        <v>-1.777682462215355</v>
       </c>
       <c r="V11" t="n">
-        <v>-10.87707380483311</v>
+        <v>-5.124824071675583</v>
       </c>
       <c r="W11" t="n">
-        <v>-7.501051635170676</v>
+        <v>-3.733242597350861</v>
       </c>
       <c r="X11" t="n">
-        <v>-18.15398984148175</v>
+        <v>-3.494789141003109</v>
       </c>
       <c r="Y11" t="n">
-        <v>-2.219918516582767</v>
+        <v>-8.941951593334956</v>
       </c>
       <c r="Z11" t="n">
-        <v>-5.163208719552449</v>
+        <v>-7.579562262884042</v>
       </c>
       <c r="AA11" t="n">
-        <v>-25.80346850010205</v>
+        <v>-15.68790848862102</v>
       </c>
       <c r="AB11" t="n">
-        <v>-7.785552887824117</v>
+        <v>-13.90828500375036</v>
       </c>
       <c r="AC11" t="n">
-        <v>-17.48884074992373</v>
+        <v>-27.0040873750091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorganized graphs, launched simulations with new parameters
</commit_message>
<xml_diff>
--- a/Data/intermediate.xlsx
+++ b/Data/intermediate.xlsx
@@ -526,88 +526,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.203256752069693</v>
+        <v>-4.37591544257347</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.915147586742647</v>
+        <v>-7.5092474554787</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.660142648263641</v>
+        <v>-10.6775589220017</v>
       </c>
       <c r="E2" t="n">
-        <v>-5.627657280467734</v>
+        <v>0.8047639845420127</v>
       </c>
       <c r="F2" t="n">
-        <v>-3.759456289974312</v>
+        <v>-25.94493367425536</v>
       </c>
       <c r="G2" t="n">
-        <v>3.457793147082079</v>
+        <v>4.712077593405253</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.151884861079954</v>
+        <v>-8.858828769114027</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.08139502643800833</v>
+        <v>-8.761903243228208</v>
       </c>
       <c r="J2" t="n">
-        <v>-3.65614698063467</v>
+        <v>-9.309517779741665</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.092599224656857</v>
+        <v>-16.13152142690379</v>
       </c>
       <c r="L2" t="n">
-        <v>-4.789174734805638</v>
+        <v>11.4773704467009</v>
       </c>
       <c r="M2" t="n">
-        <v>-4.32385018326091</v>
+        <v>18.17000083693042</v>
       </c>
       <c r="N2" t="n">
-        <v>-6.563543568839558</v>
+        <v>-20.00891666409281</v>
       </c>
       <c r="O2" t="n">
-        <v>-4.947148139797709</v>
+        <v>4.476413056415514</v>
       </c>
       <c r="P2" t="n">
-        <v>-5.410340650569359</v>
+        <v>-9.098167601125553</v>
       </c>
       <c r="Q2" t="n">
-        <v>-5.779042343796273</v>
+        <v>-36.01736496307453</v>
       </c>
       <c r="R2" t="n">
-        <v>-10.29566691701302</v>
+        <v>-21.47533216878614</v>
       </c>
       <c r="S2" t="n">
-        <v>-9.437867291806139</v>
+        <v>-10.45804644929309</v>
       </c>
       <c r="T2" t="n">
-        <v>-11.73230453567659</v>
+        <v>-16.01245750865135</v>
       </c>
       <c r="U2" t="n">
-        <v>-8.80485939379988</v>
+        <v>0.7813625545734695</v>
       </c>
       <c r="V2" t="n">
-        <v>-10.27294460356858</v>
+        <v>-26.62515184771175</v>
       </c>
       <c r="W2" t="n">
-        <v>-11.8913566109667</v>
+        <v>-15.52034828190498</v>
       </c>
       <c r="X2" t="n">
-        <v>-12.39654096035627</v>
+        <v>-0.5020175502479347</v>
       </c>
       <c r="Y2" t="n">
-        <v>-13.69387899498244</v>
+        <v>-12.85078204446999</v>
       </c>
       <c r="Z2" t="n">
-        <v>-22.96036864186023</v>
+        <v>-18.15836164984467</v>
       </c>
       <c r="AA2" t="n">
-        <v>-21.36830209179941</v>
+        <v>-32.39532213677237</v>
       </c>
       <c r="AB2" t="n">
-        <v>-32.74570025339889</v>
+        <v>-34.07759786032231</v>
       </c>
       <c r="AC2" t="n">
-        <v>-57.70849630944869</v>
+        <v>-57.6812284706039</v>
       </c>
     </row>
     <row r="3">
@@ -615,88 +615,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.881483636539404</v>
+        <v>-4.063010489990986</v>
       </c>
       <c r="C3" t="n">
-        <v>-7.610894813088846</v>
+        <v>-14.58972326207568</v>
       </c>
       <c r="D3" t="n">
-        <v>-7.529855965082808</v>
+        <v>-4.33509712439794</v>
       </c>
       <c r="E3" t="n">
-        <v>-8.040674335274598</v>
+        <v>-16.61498428529804</v>
       </c>
       <c r="F3" t="n">
-        <v>-7.931021727948621</v>
+        <v>-1.033556914543943</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.882400256709</v>
+        <v>-8.553711421441452</v>
       </c>
       <c r="H3" t="n">
-        <v>-6.578456229286526</v>
+        <v>-8.893636849855813</v>
       </c>
       <c r="I3" t="n">
-        <v>-5.498367406501969</v>
+        <v>-20.03468273796431</v>
       </c>
       <c r="J3" t="n">
-        <v>-7.663183278783197</v>
+        <v>-12.96211843727084</v>
       </c>
       <c r="K3" t="n">
-        <v>-5.396457385667087</v>
+        <v>-7.373708908702452</v>
       </c>
       <c r="L3" t="n">
-        <v>-11.05498653466389</v>
+        <v>-6.541550494639615</v>
       </c>
       <c r="M3" t="n">
-        <v>-8.280524944280138</v>
+        <v>0.8117726577368547</v>
       </c>
       <c r="N3" t="n">
-        <v>-10.87376220365612</v>
+        <v>-14.45042625462476</v>
       </c>
       <c r="O3" t="n">
-        <v>-7.887282319054789</v>
+        <v>0.3073484110631561</v>
       </c>
       <c r="P3" t="n">
-        <v>-9.319158251965057</v>
+        <v>6.5292622775694</v>
       </c>
       <c r="Q3" t="n">
-        <v>-8.013638761938655</v>
+        <v>-24.88975093632032</v>
       </c>
       <c r="R3" t="n">
-        <v>-15.48131407677113</v>
+        <v>2.099808890607038</v>
       </c>
       <c r="S3" t="n">
-        <v>-13.11741151899361</v>
+        <v>-15.86453964635165</v>
       </c>
       <c r="T3" t="n">
-        <v>-15.22228286513356</v>
+        <v>-6.532304355495157</v>
       </c>
       <c r="U3" t="n">
-        <v>-12.25803535755876</v>
+        <v>9.644747568714397</v>
       </c>
       <c r="V3" t="n">
-        <v>-14.59559105636559</v>
+        <v>-25.35123354601576</v>
       </c>
       <c r="W3" t="n">
-        <v>-14.83550628264717</v>
+        <v>-21.13599954500621</v>
       </c>
       <c r="X3" t="n">
-        <v>-16.6513914847616</v>
+        <v>-7.019099586132585</v>
       </c>
       <c r="Y3" t="n">
-        <v>-19.36401392885483</v>
+        <v>-15.7846468738178</v>
       </c>
       <c r="Z3" t="n">
-        <v>-27.58237606423543</v>
+        <v>-21.48307123688756</v>
       </c>
       <c r="AA3" t="n">
-        <v>-27.56433428728441</v>
+        <v>-27.14350978935121</v>
       </c>
       <c r="AB3" t="n">
-        <v>-36.76700297901852</v>
+        <v>-50.28035575625257</v>
       </c>
       <c r="AC3" t="n">
-        <v>-64.75300442263308</v>
+        <v>-61.17809135906398</v>
       </c>
     </row>
     <row r="4">
@@ -704,88 +704,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7953684310351807</v>
+        <v>-8.480295553239328</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.95518560632639</v>
+        <v>-2.92896102930693</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.834810490073308</v>
+        <v>-12.64462357470505</v>
       </c>
       <c r="E4" t="n">
-        <v>-4.095594264574564</v>
+        <v>16.15567612381698</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.072252697127052</v>
+        <v>-11.98326467407366</v>
       </c>
       <c r="G4" t="n">
-        <v>1.670466167149034</v>
+        <v>-11.81537870629669</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.657361479381778</v>
+        <v>8.858438959390604</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.908289143196434</v>
+        <v>-19.02617518715093</v>
       </c>
       <c r="J4" t="n">
-        <v>-1.83561055369456</v>
+        <v>2.349010856270377</v>
       </c>
       <c r="K4" t="n">
-        <v>-2.054297467932693</v>
+        <v>9.19041089342587</v>
       </c>
       <c r="L4" t="n">
-        <v>-6.832052111065551</v>
+        <v>3.029128311970418</v>
       </c>
       <c r="M4" t="n">
-        <v>-3.682437617249104</v>
+        <v>10.06670575705137</v>
       </c>
       <c r="N4" t="n">
-        <v>-7.322462774972543</v>
+        <v>7.096687042644453</v>
       </c>
       <c r="O4" t="n">
-        <v>-4.299926846572474</v>
+        <v>0.544051541062994</v>
       </c>
       <c r="P4" t="n">
-        <v>-5.659622431925891</v>
+        <v>7.792403652397224</v>
       </c>
       <c r="Q4" t="n">
-        <v>-7.562249599549294</v>
+        <v>-6.716750778266237</v>
       </c>
       <c r="R4" t="n">
-        <v>-12.1942411244396</v>
+        <v>-10.56547620930952</v>
       </c>
       <c r="S4" t="n">
-        <v>-9.660928597468297</v>
+        <v>-13.76918406124377</v>
       </c>
       <c r="T4" t="n">
-        <v>-12.53064772218563</v>
+        <v>6.883864650183005</v>
       </c>
       <c r="U4" t="n">
-        <v>-9.818043177620867</v>
+        <v>-15.90336389134866</v>
       </c>
       <c r="V4" t="n">
-        <v>-11.00606694940653</v>
+        <v>-10.49625149105573</v>
       </c>
       <c r="W4" t="n">
-        <v>-11.73646190531282</v>
+        <v>1.683100753678101</v>
       </c>
       <c r="X4" t="n">
-        <v>-14.60158795273038</v>
+        <v>-20.49927566315812</v>
       </c>
       <c r="Y4" t="n">
-        <v>-14.33850458860851</v>
+        <v>-19.10121772574955</v>
       </c>
       <c r="Z4" t="n">
-        <v>-24.78367772925949</v>
+        <v>-23.01106231801046</v>
       </c>
       <c r="AA4" t="n">
-        <v>-21.1141749815219</v>
+        <v>-37.71254339838866</v>
       </c>
       <c r="AB4" t="n">
-        <v>-34.1079995451833</v>
+        <v>-30.43881386098379</v>
       </c>
       <c r="AC4" t="n">
-        <v>-58.20102472861575</v>
+        <v>-72.27396180730634</v>
       </c>
     </row>
     <row r="5">
@@ -793,88 +793,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9442875544672349</v>
+        <v>-6.514432803468567</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.32879138192052</v>
+        <v>-6.03029964765697</v>
       </c>
       <c r="D5" t="n">
-        <v>-6.295316875160136</v>
+        <v>-3.203884008147706</v>
       </c>
       <c r="E5" t="n">
-        <v>-4.858044154532653</v>
+        <v>5.271493969412774</v>
       </c>
       <c r="F5" t="n">
-        <v>-5.919374760540562</v>
+        <v>-11.35423320469122</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.4853489344750486</v>
+        <v>-0.1906325831874849</v>
       </c>
       <c r="H5" t="n">
-        <v>-5.912970544198999</v>
+        <v>16.61733239844433</v>
       </c>
       <c r="I5" t="n">
-        <v>-3.974345334776983</v>
+        <v>6.092366318221879</v>
       </c>
       <c r="J5" t="n">
-        <v>-6.124049291914567</v>
+        <v>13.29259879633245</v>
       </c>
       <c r="K5" t="n">
-        <v>-4.028606783320361</v>
+        <v>4.265814979213212</v>
       </c>
       <c r="L5" t="n">
-        <v>-7.108447751729591</v>
+        <v>-1.200491553542308</v>
       </c>
       <c r="M5" t="n">
-        <v>-6.711656811327776</v>
+        <v>11.24216929016774</v>
       </c>
       <c r="N5" t="n">
-        <v>-7.863059456945824</v>
+        <v>-21.29987182580024</v>
       </c>
       <c r="O5" t="n">
-        <v>-6.961979516399829</v>
+        <v>-11.45574796621661</v>
       </c>
       <c r="P5" t="n">
-        <v>-7.92524629157768</v>
+        <v>12.35680904889786</v>
       </c>
       <c r="Q5" t="n">
-        <v>-8.514691497949892</v>
+        <v>-6.625120376681697</v>
       </c>
       <c r="R5" t="n">
-        <v>-12.13520499982537</v>
+        <v>-9.897871270323863</v>
       </c>
       <c r="S5" t="n">
-        <v>-11.42893577036436</v>
+        <v>-8.295285168413102</v>
       </c>
       <c r="T5" t="n">
-        <v>-13.90026640299797</v>
+        <v>-20.14937447522136</v>
       </c>
       <c r="U5" t="n">
-        <v>-9.408802151321726</v>
+        <v>-2.891619169236591</v>
       </c>
       <c r="V5" t="n">
-        <v>-13.98175040463344</v>
+        <v>-28.88858880236882</v>
       </c>
       <c r="W5" t="n">
-        <v>-13.25359540148225</v>
+        <v>-8.612915827974213</v>
       </c>
       <c r="X5" t="n">
-        <v>-15.04194871916292</v>
+        <v>-15.75866497703221</v>
       </c>
       <c r="Y5" t="n">
-        <v>-17.53561349713091</v>
+        <v>-19.43376117543467</v>
       </c>
       <c r="Z5" t="n">
-        <v>-27.07955578331005</v>
+        <v>-36.01968923130091</v>
       </c>
       <c r="AA5" t="n">
-        <v>-25.43829475158022</v>
+        <v>-40.62279518827542</v>
       </c>
       <c r="AB5" t="n">
-        <v>-35.36851546598874</v>
+        <v>-46.42335489417393</v>
       </c>
       <c r="AC5" t="n">
-        <v>-60.37071762353019</v>
+        <v>-67.16519021547086</v>
       </c>
     </row>
     <row r="6">
@@ -882,88 +882,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4989234413804855</v>
+        <v>10.58583409348475</v>
       </c>
       <c r="C6" t="n">
-        <v>-4.72682516897868</v>
+        <v>-3.813020252595602</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.11915039764253</v>
+        <v>1.38204868618796</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.146657334951867</v>
+        <v>-0.3556670601226912</v>
       </c>
       <c r="F6" t="n">
-        <v>-2.855825727560295</v>
+        <v>0.8761676410622545</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4112854032744053</v>
+        <v>-7.603800524141286</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.789193881255226</v>
+        <v>-24.95302445806139</v>
       </c>
       <c r="I6" t="n">
-        <v>-3.610227415955889</v>
+        <v>-12.61560441472351</v>
       </c>
       <c r="J6" t="n">
-        <v>-4.280319401019038</v>
+        <v>-7.023304154540126</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.7683269453788366</v>
+        <v>10.61850521068024</v>
       </c>
       <c r="L6" t="n">
-        <v>-5.429506179676224</v>
+        <v>-8.948597453863627</v>
       </c>
       <c r="M6" t="n">
-        <v>-3.474159082076488</v>
+        <v>-1.012251091251839</v>
       </c>
       <c r="N6" t="n">
-        <v>-5.574496445657659</v>
+        <v>-13.80168817539048</v>
       </c>
       <c r="O6" t="n">
-        <v>-2.62039647647817</v>
+        <v>-1.27526077772191</v>
       </c>
       <c r="P6" t="n">
-        <v>-4.835961795275614</v>
+        <v>4.236960576359035</v>
       </c>
       <c r="Q6" t="n">
-        <v>-5.089149202307958</v>
+        <v>-9.068325612685737</v>
       </c>
       <c r="R6" t="n">
-        <v>-8.974356110814046</v>
+        <v>-19.82039512375609</v>
       </c>
       <c r="S6" t="n">
-        <v>-7.419526956099681</v>
+        <v>-8.372214487470018</v>
       </c>
       <c r="T6" t="n">
-        <v>-12.30138079326382</v>
+        <v>0.8860997667161801</v>
       </c>
       <c r="U6" t="n">
-        <v>-6.672105161730501</v>
+        <v>7.507043707401792</v>
       </c>
       <c r="V6" t="n">
-        <v>-13.73176459404712</v>
+        <v>-15.93467410195335</v>
       </c>
       <c r="W6" t="n">
-        <v>-13.28911674802127</v>
+        <v>10.90430728606896</v>
       </c>
       <c r="X6" t="n">
-        <v>-12.55128271845177</v>
+        <v>-20.85554751773277</v>
       </c>
       <c r="Y6" t="n">
-        <v>-13.56248038126602</v>
+        <v>-23.80932198369081</v>
       </c>
       <c r="Z6" t="n">
-        <v>-24.56034366366385</v>
+        <v>-8.900998484560759</v>
       </c>
       <c r="AA6" t="n">
-        <v>-23.66822743222455</v>
+        <v>-33.76229991865128</v>
       </c>
       <c r="AB6" t="n">
-        <v>-31.54318367530349</v>
+        <v>-27.62015160288553</v>
       </c>
       <c r="AC6" t="n">
-        <v>-59.19228956777507</v>
+        <v>-40.68782081676954</v>
       </c>
     </row>
     <row r="7">
@@ -971,88 +971,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.294807694406027</v>
+        <v>-13.50912164734515</v>
       </c>
       <c r="C7" t="n">
-        <v>-7.546663788411537</v>
+        <v>2.742686468307664</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.982084156116814</v>
+        <v>-21.02855482354231</v>
       </c>
       <c r="E7" t="n">
-        <v>-4.123906149344998</v>
+        <v>-3.269777592439826</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.990423572688631</v>
+        <v>-21.09100152941513</v>
       </c>
       <c r="G7" t="n">
-        <v>-2.333674320411922</v>
+        <v>8.203620266184315</v>
       </c>
       <c r="H7" t="n">
-        <v>-3.41467200611289</v>
+        <v>2.191978974877195</v>
       </c>
       <c r="I7" t="n">
-        <v>-3.650166964255903</v>
+        <v>0.8275864364836529</v>
       </c>
       <c r="J7" t="n">
-        <v>-5.862792941231871</v>
+        <v>-10.31885591180059</v>
       </c>
       <c r="K7" t="n">
-        <v>-4.993616062798331</v>
+        <v>-8.657778478643923</v>
       </c>
       <c r="L7" t="n">
-        <v>-8.40191133935207</v>
+        <v>-3.112986162740213</v>
       </c>
       <c r="M7" t="n">
-        <v>-6.620169115085226</v>
+        <v>-14.53852278144884</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.776390799101457</v>
+        <v>-14.57623623588075</v>
       </c>
       <c r="O7" t="n">
-        <v>-6.890070653246162</v>
+        <v>-10.84601140055648</v>
       </c>
       <c r="P7" t="n">
-        <v>-7.776689040046603</v>
+        <v>-8.809656663413886</v>
       </c>
       <c r="Q7" t="n">
-        <v>-7.186613228492441</v>
+        <v>-3.789717818090438</v>
       </c>
       <c r="R7" t="n">
-        <v>-11.46787664099678</v>
+        <v>-30.82405352970963</v>
       </c>
       <c r="S7" t="n">
-        <v>-11.62815950769745</v>
+        <v>-5.334509474949088</v>
       </c>
       <c r="T7" t="n">
-        <v>-13.0988408981005</v>
+        <v>-11.44686908682296</v>
       </c>
       <c r="U7" t="n">
-        <v>-11.22395362794025</v>
+        <v>-4.224021093043688</v>
       </c>
       <c r="V7" t="n">
-        <v>-12.26369417461324</v>
+        <v>-9.868984942385104</v>
       </c>
       <c r="W7" t="n">
-        <v>-14.69174554211075</v>
+        <v>-2.172540265266409</v>
       </c>
       <c r="X7" t="n">
-        <v>-15.32529109338185</v>
+        <v>-12.84491459467034</v>
       </c>
       <c r="Y7" t="n">
-        <v>-18.26211719753348</v>
+        <v>-21.60957075188134</v>
       </c>
       <c r="Z7" t="n">
-        <v>-25.39428508331583</v>
+        <v>-24.30194808925436</v>
       </c>
       <c r="AA7" t="n">
-        <v>-25.86757835300908</v>
+        <v>-20.95779663091692</v>
       </c>
       <c r="AB7" t="n">
-        <v>-36.14309128917374</v>
+        <v>-32.31744176244015</v>
       </c>
       <c r="AC7" t="n">
-        <v>-60.52867622333567</v>
+        <v>-49.38574241686479</v>
       </c>
     </row>
     <row r="8">
@@ -1060,88 +1060,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.024835429105408</v>
+        <v>-21.74579774609886</v>
       </c>
       <c r="C8" t="n">
-        <v>-6.540190397102974</v>
+        <v>-16.66140304492159</v>
       </c>
       <c r="D8" t="n">
-        <v>-6.732385428531448</v>
+        <v>-8.463095333944704</v>
       </c>
       <c r="E8" t="n">
-        <v>-7.212665057998301</v>
+        <v>-27.00053580668978</v>
       </c>
       <c r="F8" t="n">
-        <v>-4.975485376161116</v>
+        <v>-7.272145494635935</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.311026035374536</v>
+        <v>1.720325511493761</v>
       </c>
       <c r="H8" t="n">
-        <v>-6.308129058493849</v>
+        <v>-10.53671531190081</v>
       </c>
       <c r="I8" t="n">
-        <v>-4.926094697181014</v>
+        <v>3.088387972016882</v>
       </c>
       <c r="J8" t="n">
-        <v>-7.375321619822163</v>
+        <v>-5.648815570560104</v>
       </c>
       <c r="K8" t="n">
-        <v>-6.683008241116678</v>
+        <v>-0.5118187192190504</v>
       </c>
       <c r="L8" t="n">
-        <v>-8.706392676362491</v>
+        <v>-27.69311034929306</v>
       </c>
       <c r="M8" t="n">
-        <v>-5.672905146848614</v>
+        <v>1.812100420334327</v>
       </c>
       <c r="N8" t="n">
-        <v>-11.02136340087631</v>
+        <v>-20.21292428513679</v>
       </c>
       <c r="O8" t="n">
-        <v>-5.29758382773346</v>
+        <v>-31.83788255582397</v>
       </c>
       <c r="P8" t="n">
-        <v>-9.583070269509054</v>
+        <v>-6.596491684253561</v>
       </c>
       <c r="Q8" t="n">
-        <v>-9.824528098103189</v>
+        <v>0.3246477018886385</v>
       </c>
       <c r="R8" t="n">
-        <v>-13.17642804268808</v>
+        <v>-15.15752119745722</v>
       </c>
       <c r="S8" t="n">
-        <v>-12.41494082192739</v>
+        <v>-3.429996753950915</v>
       </c>
       <c r="T8" t="n">
-        <v>-14.24890486095475</v>
+        <v>-14.74403305597108</v>
       </c>
       <c r="U8" t="n">
-        <v>-8.632913934583662</v>
+        <v>-10.99564347329052</v>
       </c>
       <c r="V8" t="n">
-        <v>-13.86328696749337</v>
+        <v>-24.449778853974</v>
       </c>
       <c r="W8" t="n">
-        <v>-12.96674166146745</v>
+        <v>-18.64797930701799</v>
       </c>
       <c r="X8" t="n">
-        <v>-14.91582036810826</v>
+        <v>-31.77945370848727</v>
       </c>
       <c r="Y8" t="n">
-        <v>-18.78478674667726</v>
+        <v>-29.18440779283829</v>
       </c>
       <c r="Z8" t="n">
-        <v>-26.54650013277378</v>
+        <v>-1.318337237077987</v>
       </c>
       <c r="AA8" t="n">
-        <v>-26.10415856187034</v>
+        <v>-33.42827029575906</v>
       </c>
       <c r="AB8" t="n">
-        <v>-36.82820112678417</v>
+        <v>-27.85723368103619</v>
       </c>
       <c r="AC8" t="n">
-        <v>-61.0851259327351</v>
+        <v>-52.81369881654733</v>
       </c>
     </row>
     <row r="9">
@@ -1149,88 +1149,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.888915345369813</v>
+        <v>2.596773594175547</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.814724410018849</v>
+        <v>5.379898603605952</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.04613429769095967</v>
+        <v>20.44671816392555</v>
       </c>
       <c r="E9" t="n">
-        <v>-5.262475771921713</v>
+        <v>-14.55783700058184</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.3158840407642288</v>
+        <v>-10.36873564921872</v>
       </c>
       <c r="G9" t="n">
-        <v>1.790553463542927</v>
+        <v>4.517563803014924</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.4751389910029726</v>
+        <v>-4.816679300868488</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.09260290178227049</v>
+        <v>13.98308318949527</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.090014993697799</v>
+        <v>-14.62803372186307</v>
       </c>
       <c r="K9" t="n">
-        <v>0.2201118890005671</v>
+        <v>9.502966938102897</v>
       </c>
       <c r="L9" t="n">
-        <v>-4.159502025095445</v>
+        <v>-6.007936796419272</v>
       </c>
       <c r="M9" t="n">
-        <v>-1.223938197675252</v>
+        <v>7.001057196308612</v>
       </c>
       <c r="N9" t="n">
-        <v>-4.646886882458485</v>
+        <v>-5.921539543420183</v>
       </c>
       <c r="O9" t="n">
-        <v>-3.434997638079896</v>
+        <v>-20.63732225348218</v>
       </c>
       <c r="P9" t="n">
-        <v>-3.420484680036818</v>
+        <v>-12.07213413740535</v>
       </c>
       <c r="Q9" t="n">
-        <v>-4.533470595113121</v>
+        <v>17.62201255184491</v>
       </c>
       <c r="R9" t="n">
-        <v>-8.939639275725511</v>
+        <v>3.856698151289178</v>
       </c>
       <c r="S9" t="n">
-        <v>-9.990165138775854</v>
+        <v>-14.31335348880412</v>
       </c>
       <c r="T9" t="n">
-        <v>-8.736730876077186</v>
+        <v>-15.75987092263796</v>
       </c>
       <c r="U9" t="n">
-        <v>-6.652507715051908</v>
+        <v>-6.469454658889955</v>
       </c>
       <c r="V9" t="n">
-        <v>-10.0868993419846</v>
+        <v>1.447613092556734</v>
       </c>
       <c r="W9" t="n">
-        <v>-11.1534415820112</v>
+        <v>-30.57798287353074</v>
       </c>
       <c r="X9" t="n">
-        <v>-10.3183432912204</v>
+        <v>-12.79368794761072</v>
       </c>
       <c r="Y9" t="n">
-        <v>-12.47106515441497</v>
+        <v>-25.7857790821601</v>
       </c>
       <c r="Z9" t="n">
-        <v>-21.9299559389906</v>
+        <v>-34.96312404761855</v>
       </c>
       <c r="AA9" t="n">
-        <v>-21.5646936706212</v>
+        <v>-22.19671755981662</v>
       </c>
       <c r="AB9" t="n">
-        <v>-31.90093255372198</v>
+        <v>-40.22438644770011</v>
       </c>
       <c r="AC9" t="n">
-        <v>-54.949358731065</v>
+        <v>-60.69967746103092</v>
       </c>
     </row>
     <row r="10">
@@ -1238,88 +1238,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.263728627304542</v>
+        <v>-10.91708287244365</v>
       </c>
       <c r="C10" t="n">
-        <v>-5.825251801485225</v>
+        <v>-13.43363550177162</v>
       </c>
       <c r="D10" t="n">
-        <v>-5.849769125306823</v>
+        <v>-2.629801609906425</v>
       </c>
       <c r="E10" t="n">
-        <v>-7.259487258608887</v>
+        <v>16.65608577528276</v>
       </c>
       <c r="F10" t="n">
-        <v>-5.819354771964166</v>
+        <v>-12.66860246768684</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.8926958034422805</v>
+        <v>-12.75563055005234</v>
       </c>
       <c r="H10" t="n">
-        <v>-3.869878302408033</v>
+        <v>-5.365146776386793</v>
       </c>
       <c r="I10" t="n">
-        <v>-3.351700648739033</v>
+        <v>14.48308914207417</v>
       </c>
       <c r="J10" t="n">
-        <v>-6.992023399408396</v>
+        <v>-14.62154342483526</v>
       </c>
       <c r="K10" t="n">
-        <v>-4.934651414357422</v>
+        <v>-18.92452028896291</v>
       </c>
       <c r="L10" t="n">
-        <v>-8.26594737318746</v>
+        <v>-3.886024555525826</v>
       </c>
       <c r="M10" t="n">
-        <v>-4.773692581083308</v>
+        <v>6.17018561991532</v>
       </c>
       <c r="N10" t="n">
-        <v>-7.709983142389076</v>
+        <v>19.34085352294499</v>
       </c>
       <c r="O10" t="n">
-        <v>-6.902519239547972</v>
+        <v>-21.16665124422441</v>
       </c>
       <c r="P10" t="n">
-        <v>-7.968867320338195</v>
+        <v>0.2796491528482701</v>
       </c>
       <c r="Q10" t="n">
-        <v>-8.674215500591178</v>
+        <v>-14.80517159254043</v>
       </c>
       <c r="R10" t="n">
-        <v>-14.059878252038</v>
+        <v>10.36458046664092</v>
       </c>
       <c r="S10" t="n">
-        <v>-10.61778145035866</v>
+        <v>-15.98245042028558</v>
       </c>
       <c r="T10" t="n">
-        <v>-15.66133615876454</v>
+        <v>-28.84901982645899</v>
       </c>
       <c r="U10" t="n">
-        <v>-10.43582322671984</v>
+        <v>-5.858264975682322</v>
       </c>
       <c r="V10" t="n">
-        <v>-15.61692608595417</v>
+        <v>-10.59607057114103</v>
       </c>
       <c r="W10" t="n">
-        <v>-13.43586772655391</v>
+        <v>-14.19691473768326</v>
       </c>
       <c r="X10" t="n">
-        <v>-15.22959850136501</v>
+        <v>-24.59244362525473</v>
       </c>
       <c r="Y10" t="n">
-        <v>-16.98189786677914</v>
+        <v>-32.50160311751056</v>
       </c>
       <c r="Z10" t="n">
-        <v>-25.94465602227765</v>
+        <v>-23.7708578843086</v>
       </c>
       <c r="AA10" t="n">
-        <v>-26.78884536405297</v>
+        <v>-25.30730275392791</v>
       </c>
       <c r="AB10" t="n">
-        <v>-36.11939055969883</v>
+        <v>-35.79605981899367</v>
       </c>
       <c r="AC10" t="n">
-        <v>-61.18583849904258</v>
+        <v>-52.35480746120744</v>
       </c>
     </row>
     <row r="11">
@@ -1327,88 +1327,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.693018527669403</v>
+        <v>-7.438279216612668</v>
       </c>
       <c r="C11" t="n">
-        <v>-6.691224027106706</v>
+        <v>-15.57534266806742</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.693076253709986</v>
+        <v>-15.84403293409424</v>
       </c>
       <c r="E11" t="n">
-        <v>-5.938186596566551</v>
+        <v>-6.395560689778394</v>
       </c>
       <c r="F11" t="n">
-        <v>-3.610318501720269</v>
+        <v>-13.45025334629554</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.241759051957267</v>
+        <v>-7.192563180471688</v>
       </c>
       <c r="H11" t="n">
-        <v>-4.313422973084021</v>
+        <v>-1.786060692122788</v>
       </c>
       <c r="I11" t="n">
-        <v>-3.839537321802083</v>
+        <v>-6.115630983832726</v>
       </c>
       <c r="J11" t="n">
-        <v>-5.967152930014751</v>
+        <v>5.974395419075162</v>
       </c>
       <c r="K11" t="n">
-        <v>-5.146775322726474</v>
+        <v>0.2551007902877345</v>
       </c>
       <c r="L11" t="n">
-        <v>-8.333860754992445</v>
+        <v>-3.857617771833592</v>
       </c>
       <c r="M11" t="n">
-        <v>-4.846700551034296</v>
+        <v>13.39888581348286</v>
       </c>
       <c r="N11" t="n">
-        <v>-8.784877608770985</v>
+        <v>-17.29652414679305</v>
       </c>
       <c r="O11" t="n">
-        <v>-5.181870881613721</v>
+        <v>-8.248244939274135</v>
       </c>
       <c r="P11" t="n">
-        <v>-7.906628283397611</v>
+        <v>-10.73928019881163</v>
       </c>
       <c r="Q11" t="n">
-        <v>-6.989313813575601</v>
+        <v>-7.811845471884364</v>
       </c>
       <c r="R11" t="n">
-        <v>-11.02721178281118</v>
+        <v>0.5232552771941368</v>
       </c>
       <c r="S11" t="n">
-        <v>-12.50961211585008</v>
+        <v>-6.339811832216146</v>
       </c>
       <c r="T11" t="n">
-        <v>-13.61901973642837</v>
+        <v>-3.921304934591928</v>
       </c>
       <c r="U11" t="n">
-        <v>-10.50760837374294</v>
+        <v>-1.289565758957272</v>
       </c>
       <c r="V11" t="n">
-        <v>-14.46019000329179</v>
+        <v>-1.359823021296673</v>
       </c>
       <c r="W11" t="n">
-        <v>-14.80208620390368</v>
+        <v>-13.47856713210816</v>
       </c>
       <c r="X11" t="n">
-        <v>-13.71932100086302</v>
+        <v>-13.13646435321342</v>
       </c>
       <c r="Y11" t="n">
-        <v>-17.37120807843441</v>
+        <v>-34.1076081222966</v>
       </c>
       <c r="Z11" t="n">
-        <v>-26.40248661778353</v>
+        <v>-16.81324086423653</v>
       </c>
       <c r="AA11" t="n">
-        <v>-24.9096549581789</v>
+        <v>-22.76399274279718</v>
       </c>
       <c r="AB11" t="n">
-        <v>-36.29111481592779</v>
+        <v>-30.82755430005296</v>
       </c>
       <c r="AC11" t="n">
-        <v>-61.62050791790782</v>
+        <v>-56.46165494482593</v>
       </c>
     </row>
   </sheetData>
@@ -1521,88 +1521,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4917582512556288</v>
+        <v>1.172052827782203</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.959717985808141</v>
+        <v>-3.674239514764215</v>
       </c>
       <c r="D2" t="n">
-        <v>2.387988719353929</v>
+        <v>9.230211477795908</v>
       </c>
       <c r="E2" t="n">
-        <v>1.845828554486171</v>
+        <v>8.391353905848883</v>
       </c>
       <c r="F2" t="n">
-        <v>-4.502091833101876</v>
+        <v>1.420214415521063</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.6131918533991</v>
+        <v>-17.78135057820563</v>
       </c>
       <c r="H2" t="n">
-        <v>-1.952149672721519</v>
+        <v>1.35555889739316</v>
       </c>
       <c r="I2" t="n">
-        <v>5.344785187546942</v>
+        <v>-9.420699302424801</v>
       </c>
       <c r="J2" t="n">
-        <v>5.609846825493651</v>
+        <v>-1.521874756177716</v>
       </c>
       <c r="K2" t="n">
-        <v>2.14797831322402</v>
+        <v>-4.288209367836984</v>
       </c>
       <c r="L2" t="n">
-        <v>2.808267819688757</v>
+        <v>5.881083591827855</v>
       </c>
       <c r="M2" t="n">
-        <v>-1.107294336184879</v>
+        <v>-3.940134067118988</v>
       </c>
       <c r="N2" t="n">
-        <v>-2.993589592808061</v>
+        <v>8.29212387821878</v>
       </c>
       <c r="O2" t="n">
-        <v>-2.329286826683694</v>
+        <v>4.647742389256814</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.4407077548697069</v>
+        <v>31.67549457351596</v>
       </c>
       <c r="Q2" t="n">
-        <v>-2.42716408179106</v>
+        <v>-3.157243490686982</v>
       </c>
       <c r="R2" t="n">
-        <v>1.401645482825969</v>
+        <v>-0.8554140405675237</v>
       </c>
       <c r="S2" t="n">
-        <v>-5.365168477586463</v>
+        <v>3.487180593396078</v>
       </c>
       <c r="T2" t="n">
-        <v>2.211911339261191</v>
+        <v>-9.33366002243206</v>
       </c>
       <c r="U2" t="n">
-        <v>-3.016672431096848</v>
+        <v>-2.877685234021543</v>
       </c>
       <c r="V2" t="n">
-        <v>-4.6988882027504</v>
+        <v>5.023193999845203</v>
       </c>
       <c r="W2" t="n">
-        <v>-2.933176116765403</v>
+        <v>-16.94335248371687</v>
       </c>
       <c r="X2" t="n">
-        <v>-5.432895246737232</v>
+        <v>-15.9275501834807</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.1225713137370676</v>
+        <v>5.578681963972844</v>
       </c>
       <c r="Z2" t="n">
-        <v>-6.151130510123215</v>
+        <v>-7.163841325317901</v>
       </c>
       <c r="AA2" t="n">
-        <v>-3.955631387964204</v>
+        <v>-14.1083254406283</v>
       </c>
       <c r="AB2" t="n">
-        <v>-2.801755406745296</v>
+        <v>-7.312932864920183</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.6694118815303289</v>
+        <v>-4.869424213048415</v>
       </c>
     </row>
     <row r="3">
@@ -1610,88 +1610,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-4.095640568593942</v>
+        <v>-0.2711978450583876</v>
       </c>
       <c r="C3" t="n">
-        <v>-7.575646792765325</v>
+        <v>5.782068509114335</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.098135104784025</v>
+        <v>-22.79759651781352</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.256966048885553</v>
+        <v>-10.1142992142409</v>
       </c>
       <c r="F3" t="n">
-        <v>-8.489353287726043</v>
+        <v>-13.90412239175617</v>
       </c>
       <c r="G3" t="n">
-        <v>-7.219113364686571</v>
+        <v>-12.29609346028762</v>
       </c>
       <c r="H3" t="n">
-        <v>-7.983950367469896</v>
+        <v>-18.68230122739583</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.369563466793604</v>
+        <v>-8.204210351252447</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.4152581154811124</v>
+        <v>-8.955508387658559</v>
       </c>
       <c r="K3" t="n">
-        <v>-6.385798210858574</v>
+        <v>-2.597572777081974</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.2483977503771619</v>
+        <v>8.433556386321923</v>
       </c>
       <c r="M3" t="n">
-        <v>-4.784264565790122</v>
+        <v>7.395550828650586</v>
       </c>
       <c r="N3" t="n">
-        <v>-8.102915085648966</v>
+        <v>-20.4486835971118</v>
       </c>
       <c r="O3" t="n">
-        <v>-7.252564724283189</v>
+        <v>-5.220465495851476</v>
       </c>
       <c r="P3" t="n">
-        <v>-4.01109771108565</v>
+        <v>-15.94230880726302</v>
       </c>
       <c r="Q3" t="n">
-        <v>-8.653012842012942</v>
+        <v>-22.60172143529551</v>
       </c>
       <c r="R3" t="n">
-        <v>-4.369195672471357</v>
+        <v>10.41754143523284</v>
       </c>
       <c r="S3" t="n">
-        <v>-11.71410567764538</v>
+        <v>-13.41587956276643</v>
       </c>
       <c r="T3" t="n">
-        <v>-2.077026206501396</v>
+        <v>-18.97599535320375</v>
       </c>
       <c r="U3" t="n">
-        <v>-7.821996395400034</v>
+        <v>23.27792071788025</v>
       </c>
       <c r="V3" t="n">
-        <v>-9.933323177703119</v>
+        <v>2.162399182685979</v>
       </c>
       <c r="W3" t="n">
-        <v>-8.700210650493849</v>
+        <v>4.002488632455426</v>
       </c>
       <c r="X3" t="n">
-        <v>-11.00272203360808</v>
+        <v>0.151221073887263</v>
       </c>
       <c r="Y3" t="n">
-        <v>-5.897195685543796</v>
+        <v>7.90381324545683</v>
       </c>
       <c r="Z3" t="n">
-        <v>-12.33463104076379</v>
+        <v>-12.35283355612831</v>
       </c>
       <c r="AA3" t="n">
-        <v>-8.732106951771959</v>
+        <v>-6.580300712313051</v>
       </c>
       <c r="AB3" t="n">
-        <v>-8.386997721263665</v>
+        <v>-2.447200808198393</v>
       </c>
       <c r="AC3" t="n">
-        <v>-5.669033607612114</v>
+        <v>-20.03917596007695</v>
       </c>
     </row>
     <row r="4">
@@ -1699,88 +1699,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.052948834403503</v>
+        <v>6.650664101859102</v>
       </c>
       <c r="C4" t="n">
-        <v>-6.075162623094208</v>
+        <v>4.076919366636142</v>
       </c>
       <c r="D4" t="n">
-        <v>0.127780376193122</v>
+        <v>-2.997678503444531</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6617674801120046</v>
+        <v>16.26727439537065</v>
       </c>
       <c r="F4" t="n">
-        <v>-4.671050460282114</v>
+        <v>-6.097601829750767</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.370477579261629</v>
+        <v>5.271944894311501</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.74866280309149</v>
+        <v>12.08844386476253</v>
       </c>
       <c r="I4" t="n">
-        <v>3.403942046019032</v>
+        <v>5.09278737077323</v>
       </c>
       <c r="J4" t="n">
-        <v>3.559400435815274</v>
+        <v>-0.1430472864025039</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.3934350614195658</v>
+        <v>4.362995175143578</v>
       </c>
       <c r="L4" t="n">
-        <v>1.848271856821371</v>
+        <v>-2.32672068768579</v>
       </c>
       <c r="M4" t="n">
-        <v>-1.791723102315412</v>
+        <v>-0.2184415262802164</v>
       </c>
       <c r="N4" t="n">
-        <v>-2.756217499830806</v>
+        <v>-10.79448668590727</v>
       </c>
       <c r="O4" t="n">
-        <v>-2.282193530544329</v>
+        <v>-8.376869410176342</v>
       </c>
       <c r="P4" t="n">
-        <v>-1.562711416659242</v>
+        <v>-4.21170665847609</v>
       </c>
       <c r="Q4" t="n">
-        <v>-5.016920683575912</v>
+        <v>3.986073171958389</v>
       </c>
       <c r="R4" t="n">
-        <v>-1.434161862828359</v>
+        <v>-10.12670115101325</v>
       </c>
       <c r="S4" t="n">
-        <v>-7.366115956388446</v>
+        <v>-13.42571283757013</v>
       </c>
       <c r="T4" t="n">
-        <v>2.00228641189864</v>
+        <v>-8.669741518657286</v>
       </c>
       <c r="U4" t="n">
-        <v>-4.670874360603381</v>
+        <v>-11.45315938717332</v>
       </c>
       <c r="V4" t="n">
-        <v>-5.125702488692555</v>
+        <v>-25.69143254894173</v>
       </c>
       <c r="W4" t="n">
-        <v>-3.053644760314656</v>
+        <v>-8.201658587415928</v>
       </c>
       <c r="X4" t="n">
-        <v>-5.712114201875075</v>
+        <v>5.117105522678567</v>
       </c>
       <c r="Y4" t="n">
-        <v>-0.9223260441544241</v>
+        <v>4.702209281265961</v>
       </c>
       <c r="Z4" t="n">
-        <v>-8.241657104121298</v>
+        <v>-9.364580267616407</v>
       </c>
       <c r="AA4" t="n">
-        <v>-5.065921441536243</v>
+        <v>4.472078255486279</v>
       </c>
       <c r="AB4" t="n">
-        <v>-5.169515604708063</v>
+        <v>-17.51896094098132</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.9336992321905404</v>
+        <v>14.62062055063519</v>
       </c>
     </row>
     <row r="5">
@@ -1788,88 +1788,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.174033340006362</v>
+        <v>7.249801312035705</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.688481227473984</v>
+        <v>3.960852143124745</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.538902791554903</v>
+        <v>11.63782317472828</v>
       </c>
       <c r="E5" t="n">
-        <v>-1.696489707723484</v>
+        <v>-2.874666055545951</v>
       </c>
       <c r="F5" t="n">
-        <v>-6.01696512759136</v>
+        <v>-5.88072052451553</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.366030980056644</v>
+        <v>-9.854683101642273</v>
       </c>
       <c r="H5" t="n">
-        <v>-5.29411341515751</v>
+        <v>-7.579142008861329</v>
       </c>
       <c r="I5" t="n">
-        <v>2.659417280774077</v>
+        <v>-5.441419785172628</v>
       </c>
       <c r="J5" t="n">
-        <v>1.347202974463557</v>
+        <v>-12.24745033867998</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.347155340269099</v>
+        <v>-2.758200424467303</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.2693136180314641</v>
+        <v>0.6386539452380897</v>
       </c>
       <c r="M5" t="n">
-        <v>-2.607267524055779</v>
+        <v>-10.04986174426841</v>
       </c>
       <c r="N5" t="n">
-        <v>-5.186609815790632</v>
+        <v>2.421679588557495</v>
       </c>
       <c r="O5" t="n">
-        <v>-6.137336998777203</v>
+        <v>-11.09788884453676</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.8161989857089593</v>
+        <v>12.41993644687087</v>
       </c>
       <c r="Q5" t="n">
-        <v>-5.737629479667218</v>
+        <v>-0.2694367631813863</v>
       </c>
       <c r="R5" t="n">
-        <v>-2.219859090578889</v>
+        <v>0.5287904391495082</v>
       </c>
       <c r="S5" t="n">
-        <v>-7.67366129674391</v>
+        <v>-5.223851350041984</v>
       </c>
       <c r="T5" t="n">
-        <v>0.2518619436150629</v>
+        <v>-11.8183949118914</v>
       </c>
       <c r="U5" t="n">
-        <v>-4.460728774141926</v>
+        <v>-23.32188977949148</v>
       </c>
       <c r="V5" t="n">
-        <v>-8.890726976779979</v>
+        <v>-11.71704153148101</v>
       </c>
       <c r="W5" t="n">
-        <v>-6.017905914702954</v>
+        <v>1.878504122858046</v>
       </c>
       <c r="X5" t="n">
-        <v>-6.595175764148705</v>
+        <v>11.50825371926567</v>
       </c>
       <c r="Y5" t="n">
-        <v>-1.956286616815378</v>
+        <v>-7.449219830824827</v>
       </c>
       <c r="Z5" t="n">
-        <v>-9.555561328293841</v>
+        <v>-12.95515539044828</v>
       </c>
       <c r="AA5" t="n">
-        <v>-6.634191122382017</v>
+        <v>-11.56530209778902</v>
       </c>
       <c r="AB5" t="n">
-        <v>-7.982494735583884</v>
+        <v>-3.980173554835531</v>
       </c>
       <c r="AC5" t="n">
-        <v>-2.900855680143348</v>
+        <v>12.13697562998332</v>
       </c>
     </row>
     <row r="6">
@@ -1877,88 +1877,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4683299132077314</v>
+        <v>3.70507261626849</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.151189683488103</v>
+        <v>-1.381839918165332</v>
       </c>
       <c r="D6" t="n">
-        <v>1.993095467518601</v>
+        <v>-0.262783674211847</v>
       </c>
       <c r="E6" t="n">
-        <v>1.967641343959416</v>
+        <v>7.033408741614167</v>
       </c>
       <c r="F6" t="n">
-        <v>-5.810249663947443</v>
+        <v>10.94435450282626</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.89400144013814</v>
+        <v>5.161931831737084</v>
       </c>
       <c r="H6" t="n">
-        <v>-2.633359213206711</v>
+        <v>30.27271627606967</v>
       </c>
       <c r="I6" t="n">
-        <v>3.621102886878688</v>
+        <v>11.21409471753609</v>
       </c>
       <c r="J6" t="n">
-        <v>4.826653512521098</v>
+        <v>13.61846681316532</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2785647415433309</v>
+        <v>-15.75977444263446</v>
       </c>
       <c r="L6" t="n">
-        <v>5.426513348954369</v>
+        <v>10.14517500081242</v>
       </c>
       <c r="M6" t="n">
-        <v>-1.258992020779643</v>
+        <v>5.221967997563754</v>
       </c>
       <c r="N6" t="n">
-        <v>-4.696988852796188</v>
+        <v>-12.51317707568159</v>
       </c>
       <c r="O6" t="n">
-        <v>-6.649920924719382</v>
+        <v>-11.12651674820394</v>
       </c>
       <c r="P6" t="n">
-        <v>0.90462590098412</v>
+        <v>-9.097981903312263</v>
       </c>
       <c r="Q6" t="n">
-        <v>-3.747442024131419</v>
+        <v>-13.64919685473582</v>
       </c>
       <c r="R6" t="n">
-        <v>1.167596770552644</v>
+        <v>-5.457306400852035</v>
       </c>
       <c r="S6" t="n">
-        <v>-5.700473351068956</v>
+        <v>-3.965489553756658</v>
       </c>
       <c r="T6" t="n">
-        <v>3.707032800708575</v>
+        <v>9.01806345443859</v>
       </c>
       <c r="U6" t="n">
-        <v>-1.166850646729945</v>
+        <v>-7.337898290975676</v>
       </c>
       <c r="V6" t="n">
-        <v>-4.853371777422474</v>
+        <v>-5.821327532760394</v>
       </c>
       <c r="W6" t="n">
-        <v>-2.756233678319231</v>
+        <v>-5.959073337819023</v>
       </c>
       <c r="X6" t="n">
-        <v>-1.846325856985123</v>
+        <v>3.949457095319229</v>
       </c>
       <c r="Y6" t="n">
-        <v>-2.049913512606953</v>
+        <v>3.243873566077246</v>
       </c>
       <c r="Z6" t="n">
-        <v>-6.822136772544708</v>
+        <v>-14.75186850904108</v>
       </c>
       <c r="AA6" t="n">
-        <v>-4.537102851954559</v>
+        <v>-12.84231597838886</v>
       </c>
       <c r="AB6" t="n">
-        <v>-3.845915617003623</v>
+        <v>2.291523643989886</v>
       </c>
       <c r="AC6" t="n">
-        <v>-2.959013717010996</v>
+        <v>-4.693053744453721</v>
       </c>
     </row>
     <row r="7">
@@ -1966,88 +1966,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-3.364582431218789</v>
+        <v>1.42827446156997</v>
       </c>
       <c r="C7" t="n">
-        <v>-5.365074799214037</v>
+        <v>-12.09706887775689</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.251646666721208</v>
+        <v>6.138641273755568</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3712906616832337</v>
+        <v>7.306089305422544</v>
       </c>
       <c r="F7" t="n">
-        <v>-6.195861075786995</v>
+        <v>-5.660533534343763</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.323470309610887</v>
+        <v>-5.437660351635305</v>
       </c>
       <c r="H7" t="n">
-        <v>-5.464993774120474</v>
+        <v>-7.799080526790589</v>
       </c>
       <c r="I7" t="n">
-        <v>0.744277775470084</v>
+        <v>9.524509851850004</v>
       </c>
       <c r="J7" t="n">
-        <v>1.876313548577223</v>
+        <v>-23.71570398620651</v>
       </c>
       <c r="K7" t="n">
-        <v>-3.691751757443634</v>
+        <v>-7.290019172497827</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2189978260785557</v>
+        <v>12.32553392691972</v>
       </c>
       <c r="M7" t="n">
-        <v>-5.178884295615966</v>
+        <v>3.370161640343375</v>
       </c>
       <c r="N7" t="n">
-        <v>-5.640932627454033</v>
+        <v>-19.98389699832071</v>
       </c>
       <c r="O7" t="n">
-        <v>-6.826137920366616</v>
+        <v>-23.37119647897549</v>
       </c>
       <c r="P7" t="n">
-        <v>-2.848134178028599</v>
+        <v>-2.627641344210239</v>
       </c>
       <c r="Q7" t="n">
-        <v>-5.826668785744792</v>
+        <v>-14.18293281140459</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.9912499525140346</v>
+        <v>-14.00393935191288</v>
       </c>
       <c r="S7" t="n">
-        <v>-8.424242434813214</v>
+        <v>-9.067715306225567</v>
       </c>
       <c r="T7" t="n">
-        <v>0.7032485832593904</v>
+        <v>-17.46075139794996</v>
       </c>
       <c r="U7" t="n">
-        <v>-4.781484338996088</v>
+        <v>9.154638046664799</v>
       </c>
       <c r="V7" t="n">
-        <v>-7.674722865299287</v>
+        <v>-15.37916530580897</v>
       </c>
       <c r="W7" t="n">
-        <v>-6.299893078623837</v>
+        <v>-12.37859514684922</v>
       </c>
       <c r="X7" t="n">
-        <v>-7.793060266505037</v>
+        <v>1.226075765726867</v>
       </c>
       <c r="Y7" t="n">
-        <v>-3.006497557325553</v>
+        <v>-8.679509930546459</v>
       </c>
       <c r="Z7" t="n">
-        <v>-10.44138074068182</v>
+        <v>9.749051433975604</v>
       </c>
       <c r="AA7" t="n">
-        <v>-5.426406458900496</v>
+        <v>-1.217514805952707</v>
       </c>
       <c r="AB7" t="n">
-        <v>-8.116127393969599</v>
+        <v>-17.13258988907408</v>
       </c>
       <c r="AC7" t="n">
-        <v>-2.649513293292382</v>
+        <v>-8.842249278383303</v>
       </c>
     </row>
     <row r="8">
@@ -2055,88 +2055,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.151928855012915</v>
+        <v>-5.330704726777368</v>
       </c>
       <c r="C8" t="n">
-        <v>-6.712168170167446</v>
+        <v>-4.519151848161956</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.939505007477458</v>
+        <v>-4.081352189690449</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.973500984068051</v>
+        <v>11.74523690251984</v>
       </c>
       <c r="F8" t="n">
-        <v>-8.55453910652844</v>
+        <v>9.817668142333531</v>
       </c>
       <c r="G8" t="n">
-        <v>-5.340705304355114</v>
+        <v>-1.225931875383419</v>
       </c>
       <c r="H8" t="n">
-        <v>-5.751725889451284</v>
+        <v>-2.198321913564483</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.2951434199068377</v>
+        <v>-4.666185249626632</v>
       </c>
       <c r="J8" t="n">
-        <v>2.155639943072104</v>
+        <v>18.72595686775902</v>
       </c>
       <c r="K8" t="n">
-        <v>-4.777627846130311</v>
+        <v>0.1571253335280023</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.4381315294280279</v>
+        <v>16.91168581537648</v>
       </c>
       <c r="M8" t="n">
-        <v>-3.068535045654614</v>
+        <v>2.775564745992778</v>
       </c>
       <c r="N8" t="n">
-        <v>-6.194831164878726</v>
+        <v>3.543911812809109</v>
       </c>
       <c r="O8" t="n">
-        <v>-4.826068548369197</v>
+        <v>-5.666233526079113</v>
       </c>
       <c r="P8" t="n">
-        <v>-3.335220534160649</v>
+        <v>-4.363121037335343</v>
       </c>
       <c r="Q8" t="n">
-        <v>-6.392210266356443</v>
+        <v>-12.92430069286218</v>
       </c>
       <c r="R8" t="n">
-        <v>-4.472700731445444</v>
+        <v>10.60702180735076</v>
       </c>
       <c r="S8" t="n">
-        <v>-10.19737072423963</v>
+        <v>-3.322755861894566</v>
       </c>
       <c r="T8" t="n">
-        <v>0.4363259740397512</v>
+        <v>-47.78461091136714</v>
       </c>
       <c r="U8" t="n">
-        <v>-6.25692392523174</v>
+        <v>-2.009945127749143</v>
       </c>
       <c r="V8" t="n">
-        <v>-9.142923664611034</v>
+        <v>-7.888922532946338</v>
       </c>
       <c r="W8" t="n">
-        <v>-5.756023599520257</v>
+        <v>-9.19363984460751</v>
       </c>
       <c r="X8" t="n">
-        <v>-6.556907206943179</v>
+        <v>-22.81527558274766</v>
       </c>
       <c r="Y8" t="n">
-        <v>-4.545511640807442</v>
+        <v>2.80548843590297</v>
       </c>
       <c r="Z8" t="n">
-        <v>-9.765283025942765</v>
+        <v>2.857021008741796</v>
       </c>
       <c r="AA8" t="n">
-        <v>-8.920434811837552</v>
+        <v>-7.968612397842811</v>
       </c>
       <c r="AB8" t="n">
-        <v>-6.150568038110202</v>
+        <v>-16.3673410893232</v>
       </c>
       <c r="AC8" t="n">
-        <v>-5.237999960502909</v>
+        <v>-15.64926925732307</v>
       </c>
     </row>
     <row r="9">
@@ -2144,88 +2144,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>3.294036055565201</v>
+        <v>-5.77116871419472</v>
       </c>
       <c r="C9" t="n">
-        <v>-4.03544236651368</v>
+        <v>0.3835229681466603</v>
       </c>
       <c r="D9" t="n">
-        <v>2.887108148939694</v>
+        <v>-5.077277941748504</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8349422396149982</v>
+        <v>10.58220971252026</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.678743982927048</v>
+        <v>-2.560137315708124</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.283663988995016</v>
+        <v>1.977224388791319</v>
       </c>
       <c r="H9" t="n">
-        <v>-2.360589818967857</v>
+        <v>-0.4376201449978383</v>
       </c>
       <c r="I9" t="n">
-        <v>5.506072891581881</v>
+        <v>1.720598213288802</v>
       </c>
       <c r="J9" t="n">
-        <v>6.270010181094366</v>
+        <v>-5.888642863644638</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8265834545038613</v>
+        <v>-1.435066866711035</v>
       </c>
       <c r="L9" t="n">
-        <v>4.466762987505165</v>
+        <v>9.204582151514565</v>
       </c>
       <c r="M9" t="n">
-        <v>0.08699924037136542</v>
+        <v>-1.430917340798474</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.41840326662469</v>
+        <v>-1.858227012805996</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.3261443576926659</v>
+        <v>-3.111367483250241</v>
       </c>
       <c r="P9" t="n">
-        <v>0.1262952755579858</v>
+        <v>-17.29578295122531</v>
       </c>
       <c r="Q9" t="n">
-        <v>-1.454038725977885</v>
+        <v>-3.895978054363177</v>
       </c>
       <c r="R9" t="n">
-        <v>1.585602337049582</v>
+        <v>3.164117546113995</v>
       </c>
       <c r="S9" t="n">
-        <v>-4.078409997820755</v>
+        <v>2.324795353095822</v>
       </c>
       <c r="T9" t="n">
-        <v>3.722052844033621</v>
+        <v>-27.1492750122496</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.9053400810041508</v>
+        <v>3.02268747896009</v>
       </c>
       <c r="V9" t="n">
-        <v>-4.051051373324423</v>
+        <v>-15.20793207699926</v>
       </c>
       <c r="W9" t="n">
-        <v>-1.154515731908194</v>
+        <v>2.549872646573152</v>
       </c>
       <c r="X9" t="n">
-        <v>-3.049138132097052</v>
+        <v>1.267769117770126</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.7082186751469424</v>
+        <v>5.543563507585228</v>
       </c>
       <c r="Z9" t="n">
-        <v>-4.431813274623834</v>
+        <v>19.5109965996788</v>
       </c>
       <c r="AA9" t="n">
-        <v>-3.340264898982113</v>
+        <v>-26.21720476614697</v>
       </c>
       <c r="AB9" t="n">
-        <v>-2.374692917244388</v>
+        <v>0.3250440229087728</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.4293236260848747</v>
+        <v>-4.130669470851165</v>
       </c>
     </row>
     <row r="10">
@@ -2233,88 +2233,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.725297013619782</v>
+        <v>5.85183078329058</v>
       </c>
       <c r="C10" t="n">
-        <v>-7.399430661741725</v>
+        <v>-2.036422818493087</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.665218982159704</v>
+        <v>5.732097484873239</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.822543998315759</v>
+        <v>14.35214588689497</v>
       </c>
       <c r="F10" t="n">
-        <v>-6.630894962721269</v>
+        <v>0.4107274639278828</v>
       </c>
       <c r="G10" t="n">
-        <v>-6.594332402743688</v>
+        <v>-16.41902439642324</v>
       </c>
       <c r="H10" t="n">
-        <v>-6.941292067383948</v>
+        <v>-5.203070700484404</v>
       </c>
       <c r="I10" t="n">
-        <v>1.494776028795632</v>
+        <v>0.725977728086626</v>
       </c>
       <c r="J10" t="n">
-        <v>2.760364574123642</v>
+        <v>12.25831051092192</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.433876776190391</v>
+        <v>-17.95278853768609</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.4197669463957685</v>
+        <v>-6.604652166040962</v>
       </c>
       <c r="M10" t="n">
-        <v>-3.404381288330781</v>
+        <v>9.005612043795542</v>
       </c>
       <c r="N10" t="n">
-        <v>-6.019830491810713</v>
+        <v>-23.921301090478</v>
       </c>
       <c r="O10" t="n">
-        <v>-5.514133026952914</v>
+        <v>-7.144283016752768</v>
       </c>
       <c r="P10" t="n">
-        <v>-3.519758916737507</v>
+        <v>2.799508430708887</v>
       </c>
       <c r="Q10" t="n">
-        <v>-5.871276859825762</v>
+        <v>12.38511400870316</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.8416680767292708</v>
+        <v>2.373691011512811</v>
       </c>
       <c r="S10" t="n">
-        <v>-7.294988249217768</v>
+        <v>-7.366289821557237</v>
       </c>
       <c r="T10" t="n">
-        <v>0.6046493393941939</v>
+        <v>19.05009207525833</v>
       </c>
       <c r="U10" t="n">
-        <v>-5.023561797487723</v>
+        <v>-16.22099764242396</v>
       </c>
       <c r="V10" t="n">
-        <v>-7.155287482795969</v>
+        <v>11.33912381355767</v>
       </c>
       <c r="W10" t="n">
-        <v>-8.290605270723443</v>
+        <v>8.470214456947028</v>
       </c>
       <c r="X10" t="n">
-        <v>-6.683563278380445</v>
+        <v>0.3468571448880846</v>
       </c>
       <c r="Y10" t="n">
-        <v>-5.239108832892147</v>
+        <v>-33.68641356089268</v>
       </c>
       <c r="Z10" t="n">
-        <v>-8.23768116089933</v>
+        <v>0.5741448929776931</v>
       </c>
       <c r="AA10" t="n">
-        <v>-5.689109214518346</v>
+        <v>-26.43656511071521</v>
       </c>
       <c r="AB10" t="n">
-        <v>-5.736658490743015</v>
+        <v>-15.29608504540723</v>
       </c>
       <c r="AC10" t="n">
-        <v>-4.380497780280019</v>
+        <v>-4.152946078693965</v>
       </c>
     </row>
     <row r="11">
@@ -2322,88 +2322,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-3.601479636925513</v>
+        <v>-7.803805675006642</v>
       </c>
       <c r="C11" t="n">
-        <v>-3.724157481580981</v>
+        <v>12.26302218760857</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.696326747531093</v>
+        <v>-9.246691115505206</v>
       </c>
       <c r="E11" t="n">
-        <v>-3.099282033884496</v>
+        <v>3.665147861656605</v>
       </c>
       <c r="F11" t="n">
-        <v>-7.248501734385076</v>
+        <v>1.30163600830967</v>
       </c>
       <c r="G11" t="n">
-        <v>-4.925649236810915</v>
+        <v>5.053475332051267</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.091917474263788</v>
+        <v>2.645366136854734</v>
       </c>
       <c r="I11" t="n">
-        <v>3.219100756492281</v>
+        <v>6.702309322528359</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8483566578949082</v>
+        <v>4.282218729702221</v>
       </c>
       <c r="K11" t="n">
-        <v>-4.13415356830274</v>
+        <v>-0.4853418980845121</v>
       </c>
       <c r="L11" t="n">
-        <v>0.3248323156686816</v>
+        <v>-17.7042177112452</v>
       </c>
       <c r="M11" t="n">
-        <v>-2.073059512804826</v>
+        <v>7.662157359426617</v>
       </c>
       <c r="N11" t="n">
-        <v>-4.880883402141144</v>
+        <v>0.143246720603289</v>
       </c>
       <c r="O11" t="n">
-        <v>-6.38643072016721</v>
+        <v>-9.538213193488369</v>
       </c>
       <c r="P11" t="n">
-        <v>-2.556152152859179</v>
+        <v>3.534338503732497</v>
       </c>
       <c r="Q11" t="n">
-        <v>-5.535600573067315</v>
+        <v>-2.547399780728361</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.3246452611715669</v>
+        <v>-26.60058146220826</v>
       </c>
       <c r="S11" t="n">
-        <v>-8.181687225033309</v>
+        <v>4.153749037396857</v>
       </c>
       <c r="T11" t="n">
-        <v>0.7635704509762169</v>
+        <v>-3.240602590318008</v>
       </c>
       <c r="U11" t="n">
-        <v>-4.810424512911117</v>
+        <v>-11.12106969437727</v>
       </c>
       <c r="V11" t="n">
-        <v>-6.960356767389039</v>
+        <v>-1.901512772442379</v>
       </c>
       <c r="W11" t="n">
-        <v>-6.086088554031262</v>
+        <v>-9.190135546460136</v>
       </c>
       <c r="X11" t="n">
-        <v>-7.189900749072761</v>
+        <v>0.1321704543242745</v>
       </c>
       <c r="Y11" t="n">
-        <v>-4.345189628026935</v>
+        <v>-19.16408372188281</v>
       </c>
       <c r="Z11" t="n">
-        <v>-8.713029219376653</v>
+        <v>-11.38115579510432</v>
       </c>
       <c r="AA11" t="n">
-        <v>-6.921023741428662</v>
+        <v>-9.374369738834472</v>
       </c>
       <c r="AB11" t="n">
-        <v>-5.589694479656585</v>
+        <v>-2.073077524193826</v>
       </c>
       <c r="AC11" t="n">
-        <v>-3.472248717910272</v>
+        <v>2.70910961666495</v>
       </c>
     </row>
   </sheetData>
@@ -2516,88 +2516,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.2192360798642401</v>
+        <v>-0.02796128671746834</v>
       </c>
       <c r="C2" t="n">
-        <v>3.932829207289005</v>
+        <v>0.3819729061633046</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.5497069068155274</v>
+        <v>6.158412738630259</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.3688396474673852</v>
+        <v>-3.571026170150949</v>
       </c>
       <c r="F2" t="n">
-        <v>-3.315153807549311</v>
+        <v>14.69610895412941</v>
       </c>
       <c r="G2" t="n">
-        <v>-3.850868759059056</v>
+        <v>-24.94549553353305</v>
       </c>
       <c r="H2" t="n">
-        <v>-4.19932036599381</v>
+        <v>15.44251054128004</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.8840779232556</v>
+        <v>16.96559620804861</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.3644486126276298</v>
+        <v>0.5285972873336195</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7920757472293483</v>
+        <v>10.12342215840299</v>
       </c>
       <c r="L2" t="n">
-        <v>-3.338293812148726</v>
+        <v>6.869751002594024</v>
       </c>
       <c r="M2" t="n">
-        <v>-5.779200440115058</v>
+        <v>0.0272309797578989</v>
       </c>
       <c r="N2" t="n">
-        <v>-2.084545132723243</v>
+        <v>4.831513807268457</v>
       </c>
       <c r="O2" t="n">
-        <v>-4.944836424646981</v>
+        <v>-1.299918245749157</v>
       </c>
       <c r="P2" t="n">
-        <v>-1.787918613131159</v>
+        <v>11.10475875479897</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.433325943204848</v>
+        <v>-0.9645870158577077</v>
       </c>
       <c r="R2" t="n">
-        <v>-2.409601001138493</v>
+        <v>-5.910161174662545</v>
       </c>
       <c r="S2" t="n">
-        <v>-1.833102456807632</v>
+        <v>-15.80997580891831</v>
       </c>
       <c r="T2" t="n">
-        <v>-5.279972693434644</v>
+        <v>-5.250052265624571</v>
       </c>
       <c r="U2" t="n">
-        <v>-1.606754036742478</v>
+        <v>-18.22018211046048</v>
       </c>
       <c r="V2" t="n">
-        <v>-3.073784580791491</v>
+        <v>-2.33860320145459</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.8225710767341248</v>
+        <v>-16.19060902078101</v>
       </c>
       <c r="X2" t="n">
-        <v>-2.739185998660152</v>
+        <v>-14.1784933237859</v>
       </c>
       <c r="Y2" t="n">
-        <v>-3.64781884626753</v>
+        <v>-3.744748366608281</v>
       </c>
       <c r="Z2" t="n">
-        <v>-6.904062910307508</v>
+        <v>-19.27076290826347</v>
       </c>
       <c r="AA2" t="n">
-        <v>-13.11511786421644</v>
+        <v>-12.99155232557535</v>
       </c>
       <c r="AB2" t="n">
-        <v>-12.19734349013965</v>
+        <v>-19.15845325215755</v>
       </c>
       <c r="AC2" t="n">
-        <v>-26.77351080235648</v>
+        <v>-48.69242371231837</v>
       </c>
     </row>
     <row r="3">
@@ -2605,88 +2605,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-4.488234091521339</v>
+        <v>-1.864285279106787</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9339154178312921</v>
+        <v>2.537458523216923</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.91070662986446</v>
+        <v>2.452914214781187</v>
       </c>
       <c r="E3" t="n">
-        <v>-4.870848464669735</v>
+        <v>-17.4858354434803</v>
       </c>
       <c r="F3" t="n">
-        <v>-7.190109679316423</v>
+        <v>12.43925176592394</v>
       </c>
       <c r="G3" t="n">
-        <v>-8.787236897861955</v>
+        <v>-21.38770548687035</v>
       </c>
       <c r="H3" t="n">
-        <v>-11.38112766444931</v>
+        <v>-3.899287853765309</v>
       </c>
       <c r="I3" t="n">
-        <v>-6.480512682866273</v>
+        <v>12.43863297633446</v>
       </c>
       <c r="J3" t="n">
-        <v>-4.997010370269642</v>
+        <v>-16.7364659883492</v>
       </c>
       <c r="K3" t="n">
-        <v>-4.785361840741272</v>
+        <v>-12.24553154205508</v>
       </c>
       <c r="L3" t="n">
-        <v>-8.563848579015117</v>
+        <v>-9.166445308372442</v>
       </c>
       <c r="M3" t="n">
-        <v>-11.48972087050335</v>
+        <v>-9.912836727230022</v>
       </c>
       <c r="N3" t="n">
-        <v>-6.605096512894963</v>
+        <v>1.132475227795443</v>
       </c>
       <c r="O3" t="n">
-        <v>-6.796962517912295</v>
+        <v>-10.16648633217011</v>
       </c>
       <c r="P3" t="n">
-        <v>-8.391116120410548</v>
+        <v>-27.73472465557443</v>
       </c>
       <c r="Q3" t="n">
-        <v>-5.087295131984782</v>
+        <v>-11.54505730852585</v>
       </c>
       <c r="R3" t="n">
-        <v>-6.747174498243846</v>
+        <v>7.407364383536129</v>
       </c>
       <c r="S3" t="n">
-        <v>-7.537533357603952</v>
+        <v>-19.60227041315398</v>
       </c>
       <c r="T3" t="n">
-        <v>-10.62296631719891</v>
+        <v>-9.212951220424173</v>
       </c>
       <c r="U3" t="n">
-        <v>-6.671499566544768</v>
+        <v>-7.780376082551659</v>
       </c>
       <c r="V3" t="n">
-        <v>-8.191181385388584</v>
+        <v>-17.26344355364227</v>
       </c>
       <c r="W3" t="n">
-        <v>-7.862039044823195</v>
+        <v>-12.04405378100707</v>
       </c>
       <c r="X3" t="n">
-        <v>-6.056807672408887</v>
+        <v>-11.72352800892578</v>
       </c>
       <c r="Y3" t="n">
-        <v>-10.61578322207663</v>
+        <v>-15.37514147951346</v>
       </c>
       <c r="Z3" t="n">
-        <v>-10.07794347628271</v>
+        <v>6.499954834011596</v>
       </c>
       <c r="AA3" t="n">
-        <v>-18.12394404799697</v>
+        <v>-21.81947082817397</v>
       </c>
       <c r="AB3" t="n">
-        <v>-18.03838776936672</v>
+        <v>-17.41401704346037</v>
       </c>
       <c r="AC3" t="n">
-        <v>-29.99186591685859</v>
+        <v>-30.99878697137235</v>
       </c>
     </row>
     <row r="4">
@@ -2694,88 +2694,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8884027924239324</v>
+        <v>19.56122267201161</v>
       </c>
       <c r="C4" t="n">
-        <v>3.094157592811216</v>
+        <v>9.787938783755033</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.731124630146192</v>
+        <v>10.61719230059232</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1667799561675105</v>
+        <v>-6.720387893558975</v>
       </c>
       <c r="F4" t="n">
-        <v>-4.198143015164398</v>
+        <v>11.04728824075062</v>
       </c>
       <c r="G4" t="n">
-        <v>-6.789096264620001</v>
+        <v>2.307943224358645</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.890938398931994</v>
+        <v>10.59037338469633</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.399985638104661</v>
+        <v>-4.068827223717409</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1718709096857269</v>
+        <v>-13.48238533019636</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.5836572902495778</v>
+        <v>-7.15021327159322</v>
       </c>
       <c r="L4" t="n">
-        <v>-4.974185944031365</v>
+        <v>19.47654306802843</v>
       </c>
       <c r="M4" t="n">
-        <v>-8.398400501097933</v>
+        <v>-12.68972735006388</v>
       </c>
       <c r="N4" t="n">
-        <v>-3.752713624733567</v>
+        <v>-6.336013583167611</v>
       </c>
       <c r="O4" t="n">
-        <v>-3.551037719549174</v>
+        <v>-4.445443749083811</v>
       </c>
       <c r="P4" t="n">
-        <v>-1.994631289746989</v>
+        <v>-6.726183534159651</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2868211069140063</v>
+        <v>5.570600441491376</v>
       </c>
       <c r="R4" t="n">
-        <v>-1.993688388556705</v>
+        <v>-19.09842838530822</v>
       </c>
       <c r="S4" t="n">
-        <v>-4.481105334496869</v>
+        <v>12.71744728321571</v>
       </c>
       <c r="T4" t="n">
-        <v>-7.391729438522151</v>
+        <v>-8.317129588566498</v>
       </c>
       <c r="U4" t="n">
-        <v>-1.446513957212687</v>
+        <v>0.9167027316866552</v>
       </c>
       <c r="V4" t="n">
-        <v>-3.544553176232637</v>
+        <v>-17.14792614358366</v>
       </c>
       <c r="W4" t="n">
-        <v>-3.486902211223833</v>
+        <v>4.240344592620594</v>
       </c>
       <c r="X4" t="n">
-        <v>-2.352193530868212</v>
+        <v>-5.752376774945507</v>
       </c>
       <c r="Y4" t="n">
-        <v>-6.463080794596896</v>
+        <v>7.115398159945938</v>
       </c>
       <c r="Z4" t="n">
-        <v>-6.817761357164551</v>
+        <v>-6.993770536651587</v>
       </c>
       <c r="AA4" t="n">
-        <v>-14.6541137446198</v>
+        <v>-22.25605726647287</v>
       </c>
       <c r="AB4" t="n">
-        <v>-13.78455156276005</v>
+        <v>-5.317112574682394</v>
       </c>
       <c r="AC4" t="n">
-        <v>-24.7093680593986</v>
+        <v>1.744823645115162</v>
       </c>
     </row>
     <row r="5">
@@ -2783,88 +2783,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.037232961635761</v>
+        <v>2.888665530931882</v>
       </c>
       <c r="C5" t="n">
-        <v>1.498204538189374</v>
+        <v>-14.5970437626127</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.57304656248288</v>
+        <v>1.817772545787577</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.7662261628781515</v>
+        <v>-6.423102560515957</v>
       </c>
       <c r="F5" t="n">
-        <v>-7.958019404157573</v>
+        <v>-13.43687034715616</v>
       </c>
       <c r="G5" t="n">
-        <v>-7.328858568074191</v>
+        <v>1.085805627200021</v>
       </c>
       <c r="H5" t="n">
-        <v>-7.49095144434194</v>
+        <v>-8.434663814425543</v>
       </c>
       <c r="I5" t="n">
-        <v>-5.538477767960431</v>
+        <v>14.09617639151763</v>
       </c>
       <c r="J5" t="n">
-        <v>-2.079440786600828</v>
+        <v>-33.01457735337762</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.095781272762849</v>
+        <v>-2.86474935386199</v>
       </c>
       <c r="L5" t="n">
-        <v>-4.580864851266332</v>
+        <v>-4.454960310658699</v>
       </c>
       <c r="M5" t="n">
-        <v>-10.11524399592979</v>
+        <v>-10.55961550159377</v>
       </c>
       <c r="N5" t="n">
-        <v>-3.424050486577362</v>
+        <v>-10.69566619817071</v>
       </c>
       <c r="O5" t="n">
-        <v>-7.406950457591426</v>
+        <v>1.767221905274162</v>
       </c>
       <c r="P5" t="n">
-        <v>-4.807863627142798</v>
+        <v>-1.010237605224116</v>
       </c>
       <c r="Q5" t="n">
-        <v>-3.104856758257314</v>
+        <v>-10.14461799588224</v>
       </c>
       <c r="R5" t="n">
-        <v>-3.531187525354487</v>
+        <v>-8.403374546435654</v>
       </c>
       <c r="S5" t="n">
-        <v>-3.161285610915692</v>
+        <v>-11.04991280750325</v>
       </c>
       <c r="T5" t="n">
-        <v>-9.758337188923399</v>
+        <v>-14.20477415246652</v>
       </c>
       <c r="U5" t="n">
-        <v>-1.921037151353009</v>
+        <v>-8.348920194449562</v>
       </c>
       <c r="V5" t="n">
-        <v>-5.587218360518044</v>
+        <v>-1.72758425666037</v>
       </c>
       <c r="W5" t="n">
-        <v>-5.829926035968189</v>
+        <v>8.008206220835174</v>
       </c>
       <c r="X5" t="n">
-        <v>-3.105121635137797</v>
+        <v>8.78302359981549</v>
       </c>
       <c r="Y5" t="n">
-        <v>-8.583134664853862</v>
+        <v>-7.791261222540793</v>
       </c>
       <c r="Z5" t="n">
-        <v>-8.56640528861355</v>
+        <v>1.814503218890684</v>
       </c>
       <c r="AA5" t="n">
-        <v>-16.03787911358906</v>
+        <v>-8.417437376829961</v>
       </c>
       <c r="AB5" t="n">
-        <v>-12.45074434123308</v>
+        <v>-24.05767008040989</v>
       </c>
       <c r="AC5" t="n">
-        <v>-28.26911494309371</v>
+        <v>-8.677197093655046</v>
       </c>
     </row>
     <row r="6">
@@ -2872,88 +2872,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.6034087560317271</v>
+        <v>18.25984761615328</v>
       </c>
       <c r="C6" t="n">
-        <v>3.608772351893525</v>
+        <v>-11.70807136236171</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.587877247904891</v>
+        <v>8.967226534571175</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5328880856347098</v>
+        <v>-13.62376397950574</v>
       </c>
       <c r="F6" t="n">
-        <v>-5.266820642874016</v>
+        <v>1.462837751716841</v>
       </c>
       <c r="G6" t="n">
-        <v>-4.233105935655685</v>
+        <v>19.29205687024721</v>
       </c>
       <c r="H6" t="n">
-        <v>-4.923560195624421</v>
+        <v>9.239676056687101</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.788851658672323</v>
+        <v>2.730652856024066</v>
       </c>
       <c r="J6" t="n">
-        <v>1.549468797036089</v>
+        <v>11.79309436827856</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.8435752911074741</v>
+        <v>9.107769842422151</v>
       </c>
       <c r="L6" t="n">
-        <v>-4.030379559876737</v>
+        <v>1.052016906885443</v>
       </c>
       <c r="M6" t="n">
-        <v>-5.448280178912725</v>
+        <v>-12.07524355350391</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.97354529949793</v>
+        <v>-14.36490040191739</v>
       </c>
       <c r="O6" t="n">
-        <v>-3.525291279374967</v>
+        <v>9.731448930476498</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.776391393425492</v>
+        <v>12.48987501028055</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.365520101088945</v>
+        <v>-2.084424055198647</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.6101121198049158</v>
+        <v>6.151423196632913</v>
       </c>
       <c r="S6" t="n">
-        <v>-1.45787135006529</v>
+        <v>-3.874096545667936</v>
       </c>
       <c r="T6" t="n">
-        <v>-6.766277295167809</v>
+        <v>-6.326336195271618</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.7842643825244875</v>
+        <v>-9.301082347478378</v>
       </c>
       <c r="V6" t="n">
-        <v>-5.199802727947398</v>
+        <v>2.686584690881761</v>
       </c>
       <c r="W6" t="n">
-        <v>-2.454565653844468</v>
+        <v>-0.3772993042880008</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.9141262114064901</v>
+        <v>-7.804796341241982</v>
       </c>
       <c r="Y6" t="n">
-        <v>-4.177194629668987</v>
+        <v>9.003723784571372</v>
       </c>
       <c r="Z6" t="n">
-        <v>-6.776632629782704</v>
+        <v>-6.859229640652614</v>
       </c>
       <c r="AA6" t="n">
-        <v>-15.32328572484093</v>
+        <v>-28.28539383306158</v>
       </c>
       <c r="AB6" t="n">
-        <v>-11.07144868839621</v>
+        <v>-35.23895702924737</v>
       </c>
       <c r="AC6" t="n">
-        <v>-24.99009975284665</v>
+        <v>-15.1099630904546</v>
       </c>
     </row>
     <row r="7">
@@ -2961,88 +2961,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7797687191348519</v>
+        <v>-9.400270174058097</v>
       </c>
       <c r="C7" t="n">
-        <v>1.106334910732926</v>
+        <v>-5.45825684432053</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.742807381729604</v>
+        <v>12.25767304154306</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.172274040444718</v>
+        <v>-5.090433125477024</v>
       </c>
       <c r="F7" t="n">
-        <v>-6.788913905299843</v>
+        <v>-10.84131825839479</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.451501018197147</v>
+        <v>-6.897749560717534</v>
       </c>
       <c r="H7" t="n">
-        <v>-6.848694357175392</v>
+        <v>4.206673694839168</v>
       </c>
       <c r="I7" t="n">
-        <v>-4.568478152164185</v>
+        <v>11.56536068492468</v>
       </c>
       <c r="J7" t="n">
-        <v>-2.420810783583923</v>
+        <v>-7.996958900622339</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.211215949903835</v>
+        <v>4.829409560544027</v>
       </c>
       <c r="L7" t="n">
-        <v>-7.04504626075967</v>
+        <v>-2.350410321544017</v>
       </c>
       <c r="M7" t="n">
-        <v>-8.985282189256296</v>
+        <v>5.062343604394859</v>
       </c>
       <c r="N7" t="n">
-        <v>-4.309646323802127</v>
+        <v>-5.363748184455617</v>
       </c>
       <c r="O7" t="n">
-        <v>-5.733333714847717</v>
+        <v>3.658192911289466</v>
       </c>
       <c r="P7" t="n">
-        <v>-3.649857681957848</v>
+        <v>-2.122798518479216</v>
       </c>
       <c r="Q7" t="n">
-        <v>-2.398966627333301</v>
+        <v>7.727013396924283</v>
       </c>
       <c r="R7" t="n">
-        <v>-3.71105062168416</v>
+        <v>0.183672656981078</v>
       </c>
       <c r="S7" t="n">
-        <v>-3.281995397817633</v>
+        <v>15.25568694523747</v>
       </c>
       <c r="T7" t="n">
-        <v>-9.051621248072951</v>
+        <v>3.098848849550146</v>
       </c>
       <c r="U7" t="n">
-        <v>-2.110602738547324</v>
+        <v>-13.91396628875824</v>
       </c>
       <c r="V7" t="n">
-        <v>-5.258446576359384</v>
+        <v>-20.52635407306135</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.775776825046653</v>
+        <v>-0.1691557168959958</v>
       </c>
       <c r="X7" t="n">
-        <v>-4.45923251081748</v>
+        <v>1.780340904439996</v>
       </c>
       <c r="Y7" t="n">
-        <v>-7.921096470270614</v>
+        <v>-6.158505276676626</v>
       </c>
       <c r="Z7" t="n">
-        <v>-8.232438927948863</v>
+        <v>-15.12098462356028</v>
       </c>
       <c r="AA7" t="n">
-        <v>-16.01684205806386</v>
+        <v>-11.12535312508352</v>
       </c>
       <c r="AB7" t="n">
-        <v>-13.87592365556315</v>
+        <v>-15.93689480275167</v>
       </c>
       <c r="AC7" t="n">
-        <v>-29.24522953562117</v>
+        <v>-24.5319681629065</v>
       </c>
     </row>
     <row r="8">
@@ -3050,88 +3050,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.497336815771669</v>
+        <v>4.021828577099516</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.4239202831708275</v>
+        <v>-15.57150013571733</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.915619286817837</v>
+        <v>-10.90100584127949</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.808758189121256</v>
+        <v>-9.532806578230469</v>
       </c>
       <c r="F8" t="n">
-        <v>-8.859571336999316</v>
+        <v>5.380777959619917</v>
       </c>
       <c r="G8" t="n">
-        <v>-7.497996013633128</v>
+        <v>-3.966695784140096</v>
       </c>
       <c r="H8" t="n">
-        <v>-8.638247214112791</v>
+        <v>-13.80372525548442</v>
       </c>
       <c r="I8" t="n">
-        <v>-5.826058566477866</v>
+        <v>6.903014175706676</v>
       </c>
       <c r="J8" t="n">
-        <v>-3.351854447657033</v>
+        <v>3.737830451403293</v>
       </c>
       <c r="K8" t="n">
-        <v>-3.520943813695574</v>
+        <v>-10.14583607433364</v>
       </c>
       <c r="L8" t="n">
-        <v>-7.298203767088231</v>
+        <v>10.12108663168484</v>
       </c>
       <c r="M8" t="n">
-        <v>-10.11405260438208</v>
+        <v>-1.175534995679448</v>
       </c>
       <c r="N8" t="n">
-        <v>-4.650484887787235</v>
+        <v>9.418545050546875</v>
       </c>
       <c r="O8" t="n">
-        <v>-8.198477053385536</v>
+        <v>4.79733000313057</v>
       </c>
       <c r="P8" t="n">
-        <v>-4.131974037610242</v>
+        <v>-22.66207779661712</v>
       </c>
       <c r="Q8" t="n">
-        <v>-3.799895232953336</v>
+        <v>-27.60158824197346</v>
       </c>
       <c r="R8" t="n">
-        <v>-5.56535431268846</v>
+        <v>-9.020877123377094</v>
       </c>
       <c r="S8" t="n">
-        <v>-3.323443410330103</v>
+        <v>-2.67277044729423</v>
       </c>
       <c r="T8" t="n">
-        <v>-10.68541104799367</v>
+        <v>-0.9949539095172604</v>
       </c>
       <c r="U8" t="n">
-        <v>-3.685594501379578</v>
+        <v>1.963444593972111</v>
       </c>
       <c r="V8" t="n">
-        <v>-6.683597180356361</v>
+        <v>15.83405985412469</v>
       </c>
       <c r="W8" t="n">
-        <v>-5.552075227323503</v>
+        <v>-4.090238182457748</v>
       </c>
       <c r="X8" t="n">
-        <v>-4.680844823062698</v>
+        <v>3.940077898503061</v>
       </c>
       <c r="Y8" t="n">
-        <v>-9.09638942610278</v>
+        <v>5.075906835506263</v>
       </c>
       <c r="Z8" t="n">
-        <v>-9.61643843507588</v>
+        <v>-24.54736583830473</v>
       </c>
       <c r="AA8" t="n">
-        <v>-17.24362768393093</v>
+        <v>3.382393359971921</v>
       </c>
       <c r="AB8" t="n">
-        <v>-15.52905326032036</v>
+        <v>13.26159594525128</v>
       </c>
       <c r="AC8" t="n">
-        <v>-27.96833972160688</v>
+        <v>-35.27512345550768</v>
       </c>
     </row>
     <row r="9">
@@ -3139,88 +3139,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.321501256468058</v>
+        <v>6.269515856870319</v>
       </c>
       <c r="C9" t="n">
-        <v>5.69916095847807</v>
+        <v>12.79173233313985</v>
       </c>
       <c r="D9" t="n">
-        <v>2.583575356621776</v>
+        <v>8.085249421617675</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.1740157010920926</v>
+        <v>-9.275949688719011</v>
       </c>
       <c r="F9" t="n">
-        <v>-4.776107512678346</v>
+        <v>8.649575766948651</v>
       </c>
       <c r="G9" t="n">
-        <v>-4.155097487360514</v>
+        <v>1.677623424502451</v>
       </c>
       <c r="H9" t="n">
-        <v>-2.137165300884776</v>
+        <v>0.3830083663432577</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.5747391816900782</v>
+        <v>3.746715309277513</v>
       </c>
       <c r="J9" t="n">
-        <v>1.334646507418773</v>
+        <v>7.906083034421179</v>
       </c>
       <c r="K9" t="n">
-        <v>2.042390564867019</v>
+        <v>-1.596864294706822</v>
       </c>
       <c r="L9" t="n">
-        <v>-3.925979211153975</v>
+        <v>4.996236950505045</v>
       </c>
       <c r="M9" t="n">
-        <v>-2.592985237143178</v>
+        <v>23.31865223718261</v>
       </c>
       <c r="N9" t="n">
-        <v>1.752773815858947</v>
+        <v>-14.91237988418367</v>
       </c>
       <c r="O9" t="n">
-        <v>-3.460114593620195</v>
+        <v>-4.480070834574482</v>
       </c>
       <c r="P9" t="n">
-        <v>1.356270484092342</v>
+        <v>-10.51494155498331</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.970256309676699</v>
+        <v>1.760379797523174</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.6189053137788862</v>
+        <v>14.19717418662423</v>
       </c>
       <c r="S9" t="n">
-        <v>0.7373017505634403</v>
+        <v>-11.84456519236306</v>
       </c>
       <c r="T9" t="n">
-        <v>-4.478120751656885</v>
+        <v>-18.98251447515292</v>
       </c>
       <c r="U9" t="n">
-        <v>1.484942009588107</v>
+        <v>0.4588773697953181</v>
       </c>
       <c r="V9" t="n">
-        <v>-3.210674440675641</v>
+        <v>-1.4748855129997</v>
       </c>
       <c r="W9" t="n">
-        <v>-2.91737069566406</v>
+        <v>1.121617004501341</v>
       </c>
       <c r="X9" t="n">
-        <v>0.3413780882800248</v>
+        <v>1.769586141850215</v>
       </c>
       <c r="Y9" t="n">
-        <v>-3.571726143339256</v>
+        <v>3.084211235105146</v>
       </c>
       <c r="Z9" t="n">
-        <v>-5.29260045955489</v>
+        <v>-8.828305185935811</v>
       </c>
       <c r="AA9" t="n">
-        <v>-13.9698963679016</v>
+        <v>-1.726647795188482</v>
       </c>
       <c r="AB9" t="n">
-        <v>-11.01101969231705</v>
+        <v>-10.36351180430247</v>
       </c>
       <c r="AC9" t="n">
-        <v>-25.51130512839035</v>
+        <v>-23.4021632250989</v>
       </c>
     </row>
     <row r="10">
@@ -3228,88 +3228,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.18429866034467</v>
+        <v>11.40333347762263</v>
       </c>
       <c r="C10" t="n">
-        <v>1.224837972978936</v>
+        <v>-19.40297632081347</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.3874946663050038</v>
+        <v>-15.49442577911347</v>
       </c>
       <c r="E10" t="n">
-        <v>-3.282424587745585</v>
+        <v>-2.787244985784533</v>
       </c>
       <c r="F10" t="n">
-        <v>-6.418524223660762</v>
+        <v>8.104018910101932</v>
       </c>
       <c r="G10" t="n">
-        <v>-7.472617432156625</v>
+        <v>-2.923363419368509</v>
       </c>
       <c r="H10" t="n">
-        <v>-8.727713269742953</v>
+        <v>-0.8995158778785379</v>
       </c>
       <c r="I10" t="n">
-        <v>-4.648658900744808</v>
+        <v>2.943541966284124</v>
       </c>
       <c r="J10" t="n">
-        <v>-2.453924450183163</v>
+        <v>-3.248299954302061</v>
       </c>
       <c r="K10" t="n">
-        <v>-2.32272792044179</v>
+        <v>-10.06556452982133</v>
       </c>
       <c r="L10" t="n">
-        <v>-8.719745017539868</v>
+        <v>-3.934737693730447</v>
       </c>
       <c r="M10" t="n">
-        <v>-9.819081881922797</v>
+        <v>1.788535926974497</v>
       </c>
       <c r="N10" t="n">
-        <v>-5.793573051843848</v>
+        <v>-31.04291501580686</v>
       </c>
       <c r="O10" t="n">
-        <v>-6.973256633338111</v>
+        <v>0.9379417600441604</v>
       </c>
       <c r="P10" t="n">
-        <v>-3.490294642903228</v>
+        <v>-5.743591022915799</v>
       </c>
       <c r="Q10" t="n">
-        <v>-3.027931083028234</v>
+        <v>-1.579457424369115</v>
       </c>
       <c r="R10" t="n">
-        <v>-4.738397547942506</v>
+        <v>3.841860469328702</v>
       </c>
       <c r="S10" t="n">
-        <v>-4.502578436887663</v>
+        <v>-12.83182609148938</v>
       </c>
       <c r="T10" t="n">
-        <v>-8.835670671407389</v>
+        <v>-14.94267498829149</v>
       </c>
       <c r="U10" t="n">
-        <v>-4.586270557802048</v>
+        <v>4.772701091888765</v>
       </c>
       <c r="V10" t="n">
-        <v>-5.188276568780406</v>
+        <v>-13.49343271782719</v>
       </c>
       <c r="W10" t="n">
-        <v>-5.471715499594805</v>
+        <v>-12.13984831530327</v>
       </c>
       <c r="X10" t="n">
-        <v>-3.216295149262013</v>
+        <v>1.883293403757542</v>
       </c>
       <c r="Y10" t="n">
-        <v>-8.23692341309609</v>
+        <v>-10.51233326280028</v>
       </c>
       <c r="Z10" t="n">
-        <v>-6.56580015135967</v>
+        <v>-5.893805636593873</v>
       </c>
       <c r="AA10" t="n">
-        <v>-16.64282593384941</v>
+        <v>-6.762626022146755</v>
       </c>
       <c r="AB10" t="n">
-        <v>-14.93569811352126</v>
+        <v>-5.352132222903689</v>
       </c>
       <c r="AC10" t="n">
-        <v>-27.65758951528124</v>
+        <v>-43.72985997995779</v>
       </c>
     </row>
     <row r="11">
@@ -3317,88 +3317,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.427574238537269</v>
+        <v>7.831376394154908</v>
       </c>
       <c r="C11" t="n">
-        <v>1.834311427721602</v>
+        <v>-21.0642464989096</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.20908447411592</v>
+        <v>-9.961359641291317</v>
       </c>
       <c r="E11" t="n">
-        <v>-1.876431349391078</v>
+        <v>26.40677120197054</v>
       </c>
       <c r="F11" t="n">
-        <v>-6.274967331157087</v>
+        <v>11.27905895440771</v>
       </c>
       <c r="G11" t="n">
-        <v>-6.292649487229951</v>
+        <v>-23.53344213623977</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.023530873417693</v>
+        <v>15.15789577084045</v>
       </c>
       <c r="I11" t="n">
-        <v>-2.835144882608922</v>
+        <v>23.38439969422071</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.3773303055323507</v>
+        <v>-9.597023242825912</v>
       </c>
       <c r="K11" t="n">
-        <v>-3.085385939272279</v>
+        <v>-2.341675386682333</v>
       </c>
       <c r="L11" t="n">
-        <v>-6.622315321303926</v>
+        <v>-22.07651375006833</v>
       </c>
       <c r="M11" t="n">
-        <v>-8.903854797820317</v>
+        <v>-7.147187888313028</v>
       </c>
       <c r="N11" t="n">
-        <v>-3.131205046106939</v>
+        <v>9.501437736417291</v>
       </c>
       <c r="O11" t="n">
-        <v>-5.881692863159792</v>
+        <v>-13.41179577267494</v>
       </c>
       <c r="P11" t="n">
-        <v>-3.044897046998348</v>
+        <v>-6.462026141411836</v>
       </c>
       <c r="Q11" t="n">
-        <v>-1.35365637659571</v>
+        <v>-8.197364476642338</v>
       </c>
       <c r="R11" t="n">
-        <v>-2.972124630295163</v>
+        <v>-3.011768147076992</v>
       </c>
       <c r="S11" t="n">
-        <v>-2.921828440919924</v>
+        <v>-1.954634682999003</v>
       </c>
       <c r="T11" t="n">
-        <v>-8.346154121525259</v>
+        <v>-19.97772370560151</v>
       </c>
       <c r="U11" t="n">
-        <v>-1.777682462215355</v>
+        <v>-14.63130628144851</v>
       </c>
       <c r="V11" t="n">
-        <v>-5.124824071675583</v>
+        <v>-10.54824901786116</v>
       </c>
       <c r="W11" t="n">
-        <v>-3.733242597350861</v>
+        <v>-11.10741499854274</v>
       </c>
       <c r="X11" t="n">
-        <v>-3.494789141003109</v>
+        <v>2.005400795856137</v>
       </c>
       <c r="Y11" t="n">
-        <v>-8.941951593334956</v>
+        <v>-5.887670106272041</v>
       </c>
       <c r="Z11" t="n">
-        <v>-7.579562262884042</v>
+        <v>-18.43227521952509</v>
       </c>
       <c r="AA11" t="n">
-        <v>-15.68790848862102</v>
+        <v>-24.21259068899837</v>
       </c>
       <c r="AB11" t="n">
-        <v>-13.90828500375036</v>
+        <v>-16.89810946691512</v>
       </c>
       <c r="AC11" t="n">
-        <v>-27.0040873750091</v>
+        <v>-24.83698325106778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected alignment for scenario generation, new graphs for verify filter
</commit_message>
<xml_diff>
--- a/Data/intermediate.xlsx
+++ b/Data/intermediate.xlsx
@@ -526,88 +526,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-4.37591544257347</v>
+        <v>-8.812779424184445</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.5092474554787</v>
+        <v>17.11756676259009</v>
       </c>
       <c r="D2" t="n">
-        <v>-10.6775589220017</v>
+        <v>-7.058713283447916</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8047639845420127</v>
+        <v>-8.557142356912657</v>
       </c>
       <c r="F2" t="n">
-        <v>-25.94493367425536</v>
+        <v>-3.594502164640295</v>
       </c>
       <c r="G2" t="n">
-        <v>4.712077593405253</v>
+        <v>10.99744732886962</v>
       </c>
       <c r="H2" t="n">
-        <v>-8.858828769114027</v>
+        <v>-16.61037207634313</v>
       </c>
       <c r="I2" t="n">
-        <v>-8.761903243228208</v>
+        <v>5.218337347991672</v>
       </c>
       <c r="J2" t="n">
-        <v>-9.309517779741665</v>
+        <v>0.525139647150322</v>
       </c>
       <c r="K2" t="n">
-        <v>-16.13152142690379</v>
+        <v>-6.032539788860974</v>
       </c>
       <c r="L2" t="n">
-        <v>11.4773704467009</v>
+        <v>-25.47886495471957</v>
       </c>
       <c r="M2" t="n">
-        <v>18.17000083693042</v>
+        <v>8.738558707719651</v>
       </c>
       <c r="N2" t="n">
-        <v>-20.00891666409281</v>
+        <v>3.302091071496324</v>
       </c>
       <c r="O2" t="n">
-        <v>4.476413056415514</v>
+        <v>9.605454348211776</v>
       </c>
       <c r="P2" t="n">
-        <v>-9.098167601125553</v>
+        <v>-9.259411444262277</v>
       </c>
       <c r="Q2" t="n">
-        <v>-36.01736496307453</v>
+        <v>19.7699877127707</v>
       </c>
       <c r="R2" t="n">
-        <v>-21.47533216878614</v>
+        <v>-9.129912367950297</v>
       </c>
       <c r="S2" t="n">
-        <v>-10.45804644929309</v>
+        <v>-13.22284843517242</v>
       </c>
       <c r="T2" t="n">
-        <v>-16.01245750865135</v>
+        <v>-6.655821250537621</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7813625545734695</v>
+        <v>-13.27355879584231</v>
       </c>
       <c r="V2" t="n">
-        <v>-26.62515184771175</v>
+        <v>-14.22625658999419</v>
       </c>
       <c r="W2" t="n">
-        <v>-15.52034828190498</v>
+        <v>-6.644221128353055</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.5020175502479347</v>
+        <v>-5.890039758440476</v>
       </c>
       <c r="Y2" t="n">
-        <v>-12.85078204446999</v>
+        <v>-14.0566877390623</v>
       </c>
       <c r="Z2" t="n">
-        <v>-18.15836164984467</v>
+        <v>-35.32259626621381</v>
       </c>
       <c r="AA2" t="n">
-        <v>-32.39532213677237</v>
+        <v>-21.83004257515117</v>
       </c>
       <c r="AB2" t="n">
-        <v>-34.07759786032231</v>
+        <v>-17.41989721487705</v>
       </c>
       <c r="AC2" t="n">
-        <v>-57.6812284706039</v>
+        <v>-47.52835376535336</v>
       </c>
     </row>
     <row r="3">
@@ -615,88 +615,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-4.063010489990986</v>
+        <v>-5.741461213172084</v>
       </c>
       <c r="C3" t="n">
-        <v>-14.58972326207568</v>
+        <v>1.250483475167204</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.33509712439794</v>
+        <v>-13.52450348750358</v>
       </c>
       <c r="E3" t="n">
-        <v>-16.61498428529804</v>
+        <v>-13.18389582763616</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.033556914543943</v>
+        <v>-7.461952877128537</v>
       </c>
       <c r="G3" t="n">
-        <v>-8.553711421441452</v>
+        <v>-12.78440265303405</v>
       </c>
       <c r="H3" t="n">
-        <v>-8.893636849855813</v>
+        <v>-5.966039781277625</v>
       </c>
       <c r="I3" t="n">
-        <v>-20.03468273796431</v>
+        <v>-8.996582694776825</v>
       </c>
       <c r="J3" t="n">
-        <v>-12.96211843727084</v>
+        <v>-14.33726609939034</v>
       </c>
       <c r="K3" t="n">
-        <v>-7.373708908702452</v>
+        <v>-18.95871153275746</v>
       </c>
       <c r="L3" t="n">
-        <v>-6.541550494639615</v>
+        <v>-14.42501588398642</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8117726577368547</v>
+        <v>-6.852405415713553</v>
       </c>
       <c r="N3" t="n">
-        <v>-14.45042625462476</v>
+        <v>-13.02532793824343</v>
       </c>
       <c r="O3" t="n">
-        <v>0.3073484110631561</v>
+        <v>3.677201255883681</v>
       </c>
       <c r="P3" t="n">
-        <v>6.5292622775694</v>
+        <v>-19.32398865577915</v>
       </c>
       <c r="Q3" t="n">
-        <v>-24.88975093632032</v>
+        <v>-27.93768776871568</v>
       </c>
       <c r="R3" t="n">
-        <v>2.099808890607038</v>
+        <v>-3.777657297778002</v>
       </c>
       <c r="S3" t="n">
-        <v>-15.86453964635165</v>
+        <v>-28.98481682210415</v>
       </c>
       <c r="T3" t="n">
-        <v>-6.532304355495157</v>
+        <v>-19.14776711416241</v>
       </c>
       <c r="U3" t="n">
-        <v>9.644747568714397</v>
+        <v>-33.05396947232694</v>
       </c>
       <c r="V3" t="n">
-        <v>-25.35123354601576</v>
+        <v>-16.59139585123468</v>
       </c>
       <c r="W3" t="n">
-        <v>-21.13599954500621</v>
+        <v>-21.72572513394365</v>
       </c>
       <c r="X3" t="n">
-        <v>-7.019099586132585</v>
+        <v>-21.04043228443193</v>
       </c>
       <c r="Y3" t="n">
-        <v>-15.7846468738178</v>
+        <v>-23.54569298786582</v>
       </c>
       <c r="Z3" t="n">
-        <v>-21.48307123688756</v>
+        <v>-22.98266608733261</v>
       </c>
       <c r="AA3" t="n">
-        <v>-27.14350978935121</v>
+        <v>-22.0146684999642</v>
       </c>
       <c r="AB3" t="n">
-        <v>-50.28035575625257</v>
+        <v>-42.76753636561547</v>
       </c>
       <c r="AC3" t="n">
-        <v>-61.17809135906398</v>
+        <v>-47.75328740501817</v>
       </c>
     </row>
     <row r="4">
@@ -704,88 +704,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-8.480295553239328</v>
+        <v>6.022772527081343</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.92896102930693</v>
+        <v>6.976168701760161</v>
       </c>
       <c r="D4" t="n">
-        <v>-12.64462357470505</v>
+        <v>-2.447248192114507</v>
       </c>
       <c r="E4" t="n">
-        <v>16.15567612381698</v>
+        <v>4.408413611006896</v>
       </c>
       <c r="F4" t="n">
-        <v>-11.98326467407366</v>
+        <v>-19.56551522344432</v>
       </c>
       <c r="G4" t="n">
-        <v>-11.81537870629669</v>
+        <v>-8.502105137517841</v>
       </c>
       <c r="H4" t="n">
-        <v>8.858438959390604</v>
+        <v>-11.72609121189239</v>
       </c>
       <c r="I4" t="n">
-        <v>-19.02617518715093</v>
+        <v>-10.33343157800917</v>
       </c>
       <c r="J4" t="n">
-        <v>2.349010856270377</v>
+        <v>-0.5609008847496169</v>
       </c>
       <c r="K4" t="n">
-        <v>9.19041089342587</v>
+        <v>-7.804422357898893</v>
       </c>
       <c r="L4" t="n">
-        <v>3.029128311970418</v>
+        <v>-6.764455079141137</v>
       </c>
       <c r="M4" t="n">
-        <v>10.06670575705137</v>
+        <v>-21.01380300536228</v>
       </c>
       <c r="N4" t="n">
-        <v>7.096687042644453</v>
+        <v>-3.672479346840388</v>
       </c>
       <c r="O4" t="n">
-        <v>0.544051541062994</v>
+        <v>-9.293895538956981</v>
       </c>
       <c r="P4" t="n">
-        <v>7.792403652397224</v>
+        <v>-1.143465379249979</v>
       </c>
       <c r="Q4" t="n">
-        <v>-6.716750778266237</v>
+        <v>0.3529789371306578</v>
       </c>
       <c r="R4" t="n">
-        <v>-10.56547620930952</v>
+        <v>-10.42292625476901</v>
       </c>
       <c r="S4" t="n">
-        <v>-13.76918406124377</v>
+        <v>2.358552203403535</v>
       </c>
       <c r="T4" t="n">
-        <v>6.883864650183005</v>
+        <v>-19.75747571287381</v>
       </c>
       <c r="U4" t="n">
-        <v>-15.90336389134866</v>
+        <v>-23.15147422497265</v>
       </c>
       <c r="V4" t="n">
-        <v>-10.49625149105573</v>
+        <v>-10.49223775469964</v>
       </c>
       <c r="W4" t="n">
-        <v>1.683100753678101</v>
+        <v>-11.88585340621532</v>
       </c>
       <c r="X4" t="n">
-        <v>-20.49927566315812</v>
+        <v>-13.2936323404691</v>
       </c>
       <c r="Y4" t="n">
-        <v>-19.10121772574955</v>
+        <v>-31.16314101429282</v>
       </c>
       <c r="Z4" t="n">
-        <v>-23.01106231801046</v>
+        <v>-31.47363410395297</v>
       </c>
       <c r="AA4" t="n">
-        <v>-37.71254339838866</v>
+        <v>-6.625514569927279</v>
       </c>
       <c r="AB4" t="n">
-        <v>-30.43881386098379</v>
+        <v>-52.92811036104301</v>
       </c>
       <c r="AC4" t="n">
-        <v>-72.27396180730634</v>
+        <v>-46.85255844873348</v>
       </c>
     </row>
     <row r="5">
@@ -793,88 +793,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-6.514432803468567</v>
+        <v>2.096962369033812</v>
       </c>
       <c r="C5" t="n">
-        <v>-6.03029964765697</v>
+        <v>14.57555102440856</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.203884008147706</v>
+        <v>-23.5745591773492</v>
       </c>
       <c r="E5" t="n">
-        <v>5.271493969412774</v>
+        <v>-1.033559171613133</v>
       </c>
       <c r="F5" t="n">
-        <v>-11.35423320469122</v>
+        <v>-15.91758556250333</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.1906325831874849</v>
+        <v>-2.57199913612783</v>
       </c>
       <c r="H5" t="n">
-        <v>16.61733239844433</v>
+        <v>-16.04550684505481</v>
       </c>
       <c r="I5" t="n">
-        <v>6.092366318221879</v>
+        <v>-5.96923248036609</v>
       </c>
       <c r="J5" t="n">
-        <v>13.29259879633245</v>
+        <v>-9.110304262026849</v>
       </c>
       <c r="K5" t="n">
-        <v>4.265814979213212</v>
+        <v>-23.39711590823227</v>
       </c>
       <c r="L5" t="n">
-        <v>-1.200491553542308</v>
+        <v>-5.479627662700837</v>
       </c>
       <c r="M5" t="n">
-        <v>11.24216929016774</v>
+        <v>-8.235865476313478</v>
       </c>
       <c r="N5" t="n">
-        <v>-21.29987182580024</v>
+        <v>-8.948366307192604</v>
       </c>
       <c r="O5" t="n">
-        <v>-11.45574796621661</v>
+        <v>-21.67989243069401</v>
       </c>
       <c r="P5" t="n">
-        <v>12.35680904889786</v>
+        <v>-21.49112010601729</v>
       </c>
       <c r="Q5" t="n">
-        <v>-6.625120376681697</v>
+        <v>-4.176915716718425</v>
       </c>
       <c r="R5" t="n">
-        <v>-9.897871270323863</v>
+        <v>2.133818501362063</v>
       </c>
       <c r="S5" t="n">
-        <v>-8.295285168413102</v>
+        <v>-5.426947188468064</v>
       </c>
       <c r="T5" t="n">
-        <v>-20.14937447522136</v>
+        <v>-8.392782186380437</v>
       </c>
       <c r="U5" t="n">
-        <v>-2.891619169236591</v>
+        <v>-13.16378559554878</v>
       </c>
       <c r="V5" t="n">
-        <v>-28.88858880236882</v>
+        <v>-14.37318454791788</v>
       </c>
       <c r="W5" t="n">
-        <v>-8.612915827974213</v>
+        <v>-20.0509995774255</v>
       </c>
       <c r="X5" t="n">
-        <v>-15.75866497703221</v>
+        <v>-32.2639725421937</v>
       </c>
       <c r="Y5" t="n">
-        <v>-19.43376117543467</v>
+        <v>-21.37721676942371</v>
       </c>
       <c r="Z5" t="n">
-        <v>-36.01968923130091</v>
+        <v>-16.62468406663643</v>
       </c>
       <c r="AA5" t="n">
-        <v>-40.62279518827542</v>
+        <v>-34.65360233279628</v>
       </c>
       <c r="AB5" t="n">
-        <v>-46.42335489417393</v>
+        <v>-23.91687352070372</v>
       </c>
       <c r="AC5" t="n">
-        <v>-67.16519021547086</v>
+        <v>-36.79521894131058</v>
       </c>
     </row>
     <row r="6">
@@ -882,88 +882,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>10.58583409348475</v>
+        <v>7.135814955431026</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.813020252595602</v>
+        <v>5.56044112588655</v>
       </c>
       <c r="D6" t="n">
-        <v>1.38204868618796</v>
+        <v>-24.30612410185532</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3556670601226912</v>
+        <v>-6.313216051853364</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8761676410622545</v>
+        <v>6.472574054261148</v>
       </c>
       <c r="G6" t="n">
-        <v>-7.603800524141286</v>
+        <v>2.929975878031675</v>
       </c>
       <c r="H6" t="n">
-        <v>-24.95302445806139</v>
+        <v>-18.95797203404481</v>
       </c>
       <c r="I6" t="n">
-        <v>-12.61560441472351</v>
+        <v>-9.908327420051155</v>
       </c>
       <c r="J6" t="n">
-        <v>-7.023304154540126</v>
+        <v>24.19563821344937</v>
       </c>
       <c r="K6" t="n">
-        <v>10.61850521068024</v>
+        <v>-26.02303599435923</v>
       </c>
       <c r="L6" t="n">
-        <v>-8.948597453863627</v>
+        <v>-18.91498097573676</v>
       </c>
       <c r="M6" t="n">
-        <v>-1.012251091251839</v>
+        <v>-3.633567507636424</v>
       </c>
       <c r="N6" t="n">
-        <v>-13.80168817539048</v>
+        <v>7.901911128187672</v>
       </c>
       <c r="O6" t="n">
-        <v>-1.27526077772191</v>
+        <v>-14.03003306103507</v>
       </c>
       <c r="P6" t="n">
-        <v>4.236960576359035</v>
+        <v>-0.2562100030331109</v>
       </c>
       <c r="Q6" t="n">
-        <v>-9.068325612685737</v>
+        <v>-13.11333180700851</v>
       </c>
       <c r="R6" t="n">
-        <v>-19.82039512375609</v>
+        <v>-20.59626496618199</v>
       </c>
       <c r="S6" t="n">
-        <v>-8.372214487470018</v>
+        <v>-18.26400392199824</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8860997667161801</v>
+        <v>-10.89527507925232</v>
       </c>
       <c r="U6" t="n">
-        <v>7.507043707401792</v>
+        <v>3.451104592111074</v>
       </c>
       <c r="V6" t="n">
-        <v>-15.93467410195335</v>
+        <v>-14.59444872892221</v>
       </c>
       <c r="W6" t="n">
-        <v>10.90430728606896</v>
+        <v>-22.75047699907367</v>
       </c>
       <c r="X6" t="n">
-        <v>-20.85554751773277</v>
+        <v>-15.78606036267524</v>
       </c>
       <c r="Y6" t="n">
-        <v>-23.80932198369081</v>
+        <v>-20.08673377348418</v>
       </c>
       <c r="Z6" t="n">
-        <v>-8.900998484560759</v>
+        <v>-7.565154646360496</v>
       </c>
       <c r="AA6" t="n">
-        <v>-33.76229991865128</v>
+        <v>0.9378814045714599</v>
       </c>
       <c r="AB6" t="n">
-        <v>-27.62015160288553</v>
+        <v>-28.85101561615434</v>
       </c>
       <c r="AC6" t="n">
-        <v>-40.68782081676954</v>
+        <v>-52.62002631754913</v>
       </c>
     </row>
     <row r="7">
@@ -971,88 +971,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-13.50912164734515</v>
+        <v>8.796666149667619</v>
       </c>
       <c r="C7" t="n">
-        <v>2.742686468307664</v>
+        <v>5.268555221427171</v>
       </c>
       <c r="D7" t="n">
-        <v>-21.02855482354231</v>
+        <v>-19.14724627072031</v>
       </c>
       <c r="E7" t="n">
-        <v>-3.269777592439826</v>
+        <v>0.8374461163785805</v>
       </c>
       <c r="F7" t="n">
-        <v>-21.09100152941513</v>
+        <v>0.6609881448083961</v>
       </c>
       <c r="G7" t="n">
-        <v>8.203620266184315</v>
+        <v>-4.780525359676183</v>
       </c>
       <c r="H7" t="n">
-        <v>2.191978974877195</v>
+        <v>-5.063827041921656</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8275864364836529</v>
+        <v>-16.99681034156701</v>
       </c>
       <c r="J7" t="n">
-        <v>-10.31885591180059</v>
+        <v>6.355972393606649</v>
       </c>
       <c r="K7" t="n">
-        <v>-8.657778478643923</v>
+        <v>-15.21853197419455</v>
       </c>
       <c r="L7" t="n">
-        <v>-3.112986162740213</v>
+        <v>-4.794189392778666</v>
       </c>
       <c r="M7" t="n">
-        <v>-14.53852278144884</v>
+        <v>-3.783132834497415</v>
       </c>
       <c r="N7" t="n">
-        <v>-14.57623623588075</v>
+        <v>-3.0349358142398</v>
       </c>
       <c r="O7" t="n">
-        <v>-10.84601140055648</v>
+        <v>-0.4981420101134679</v>
       </c>
       <c r="P7" t="n">
-        <v>-8.809656663413886</v>
+        <v>7.01864943365276</v>
       </c>
       <c r="Q7" t="n">
-        <v>-3.789717818090438</v>
+        <v>1.189513772469379</v>
       </c>
       <c r="R7" t="n">
-        <v>-30.82405352970963</v>
+        <v>-19.40599719847911</v>
       </c>
       <c r="S7" t="n">
-        <v>-5.334509474949088</v>
+        <v>-4.61587994828213</v>
       </c>
       <c r="T7" t="n">
-        <v>-11.44686908682296</v>
+        <v>-16.23149027048957</v>
       </c>
       <c r="U7" t="n">
-        <v>-4.224021093043688</v>
+        <v>-1.315656117354049</v>
       </c>
       <c r="V7" t="n">
-        <v>-9.868984942385104</v>
+        <v>-23.74967368708842</v>
       </c>
       <c r="W7" t="n">
-        <v>-2.172540265266409</v>
+        <v>-4.859122061115725</v>
       </c>
       <c r="X7" t="n">
-        <v>-12.84491459467034</v>
+        <v>-16.97843307202257</v>
       </c>
       <c r="Y7" t="n">
-        <v>-21.60957075188134</v>
+        <v>-39.56701082707624</v>
       </c>
       <c r="Z7" t="n">
-        <v>-24.30194808925436</v>
+        <v>-23.26056358901563</v>
       </c>
       <c r="AA7" t="n">
-        <v>-20.95779663091692</v>
+        <v>-5.252824718505618</v>
       </c>
       <c r="AB7" t="n">
-        <v>-32.31744176244015</v>
+        <v>-28.54647792440355</v>
       </c>
       <c r="AC7" t="n">
-        <v>-49.38574241686479</v>
+        <v>-46.10307480874474</v>
       </c>
     </row>
     <row r="8">
@@ -1060,88 +1060,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-21.74579774609886</v>
+        <v>-6.503055484048042</v>
       </c>
       <c r="C8" t="n">
-        <v>-16.66140304492159</v>
+        <v>3.410204092652535</v>
       </c>
       <c r="D8" t="n">
-        <v>-8.463095333944704</v>
+        <v>-13.60521653594496</v>
       </c>
       <c r="E8" t="n">
-        <v>-27.00053580668978</v>
+        <v>-4.865481326417701</v>
       </c>
       <c r="F8" t="n">
-        <v>-7.272145494635935</v>
+        <v>-21.45838570904424</v>
       </c>
       <c r="G8" t="n">
-        <v>1.720325511493761</v>
+        <v>-13.39909843819251</v>
       </c>
       <c r="H8" t="n">
-        <v>-10.53671531190081</v>
+        <v>-20.68034006856332</v>
       </c>
       <c r="I8" t="n">
-        <v>3.088387972016882</v>
+        <v>-23.71172804470534</v>
       </c>
       <c r="J8" t="n">
-        <v>-5.648815570560104</v>
+        <v>22.89649497897013</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.5118187192190504</v>
+        <v>-9.865883255861675</v>
       </c>
       <c r="L8" t="n">
-        <v>-27.69311034929306</v>
+        <v>-1.860075801079909</v>
       </c>
       <c r="M8" t="n">
-        <v>1.812100420334327</v>
+        <v>1.339787468278868</v>
       </c>
       <c r="N8" t="n">
-        <v>-20.21292428513679</v>
+        <v>-15.56988817448469</v>
       </c>
       <c r="O8" t="n">
-        <v>-31.83788255582397</v>
+        <v>-6.165700901007051</v>
       </c>
       <c r="P8" t="n">
-        <v>-6.596491684253561</v>
+        <v>-33.37841804739845</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.3246477018886385</v>
+        <v>5.160379188073643</v>
       </c>
       <c r="R8" t="n">
-        <v>-15.15752119745722</v>
+        <v>-22.79611594594778</v>
       </c>
       <c r="S8" t="n">
-        <v>-3.429996753950915</v>
+        <v>-17.4536107322315</v>
       </c>
       <c r="T8" t="n">
-        <v>-14.74403305597108</v>
+        <v>-16.85978909655059</v>
       </c>
       <c r="U8" t="n">
-        <v>-10.99564347329052</v>
+        <v>-20.43972447335449</v>
       </c>
       <c r="V8" t="n">
-        <v>-24.449778853974</v>
+        <v>-1.154100944017992</v>
       </c>
       <c r="W8" t="n">
-        <v>-18.64797930701799</v>
+        <v>-31.50353870547752</v>
       </c>
       <c r="X8" t="n">
-        <v>-31.77945370848727</v>
+        <v>-26.73711804179469</v>
       </c>
       <c r="Y8" t="n">
-        <v>-29.18440779283829</v>
+        <v>-23.77685665758916</v>
       </c>
       <c r="Z8" t="n">
-        <v>-1.318337237077987</v>
+        <v>-23.50642080077673</v>
       </c>
       <c r="AA8" t="n">
-        <v>-33.42827029575906</v>
+        <v>-3.925871058089328</v>
       </c>
       <c r="AB8" t="n">
-        <v>-27.85723368103619</v>
+        <v>-30.21473839097254</v>
       </c>
       <c r="AC8" t="n">
-        <v>-52.81369881654733</v>
+        <v>-60.1822604868297</v>
       </c>
     </row>
     <row r="9">
@@ -1149,88 +1149,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.596773594175547</v>
+        <v>-1.679403765209468</v>
       </c>
       <c r="C9" t="n">
-        <v>5.379898603605952</v>
+        <v>15.24683649981244</v>
       </c>
       <c r="D9" t="n">
-        <v>20.44671816392555</v>
+        <v>-0.2160900397866339</v>
       </c>
       <c r="E9" t="n">
-        <v>-14.55783700058184</v>
+        <v>2.77963089150523</v>
       </c>
       <c r="F9" t="n">
-        <v>-10.36873564921872</v>
+        <v>9.572928907133624</v>
       </c>
       <c r="G9" t="n">
-        <v>4.517563803014924</v>
+        <v>-17.79339323225614</v>
       </c>
       <c r="H9" t="n">
-        <v>-4.816679300868488</v>
+        <v>-1.680137652675097</v>
       </c>
       <c r="I9" t="n">
-        <v>13.98308318949527</v>
+        <v>-1.924447945238266</v>
       </c>
       <c r="J9" t="n">
-        <v>-14.62803372186307</v>
+        <v>-26.47461480123049</v>
       </c>
       <c r="K9" t="n">
-        <v>9.502966938102897</v>
+        <v>-4.705903887903705</v>
       </c>
       <c r="L9" t="n">
-        <v>-6.007936796419272</v>
+        <v>-9.555874570218897</v>
       </c>
       <c r="M9" t="n">
-        <v>7.001057196308612</v>
+        <v>-12.72654122833984</v>
       </c>
       <c r="N9" t="n">
-        <v>-5.921539543420183</v>
+        <v>0.5273448630426198</v>
       </c>
       <c r="O9" t="n">
-        <v>-20.63732225348218</v>
+        <v>-12.75350153142142</v>
       </c>
       <c r="P9" t="n">
-        <v>-12.07213413740535</v>
+        <v>-4.261498304332386</v>
       </c>
       <c r="Q9" t="n">
-        <v>17.62201255184491</v>
+        <v>4.567488117211578</v>
       </c>
       <c r="R9" t="n">
-        <v>3.856698151289178</v>
+        <v>4.462154535301048</v>
       </c>
       <c r="S9" t="n">
-        <v>-14.31335348880412</v>
+        <v>-5.200443228670458</v>
       </c>
       <c r="T9" t="n">
-        <v>-15.75987092263796</v>
+        <v>-0.6590800824816476</v>
       </c>
       <c r="U9" t="n">
-        <v>-6.469454658889955</v>
+        <v>-12.41800917122425</v>
       </c>
       <c r="V9" t="n">
-        <v>1.447613092556734</v>
+        <v>-8.19097373794386</v>
       </c>
       <c r="W9" t="n">
-        <v>-30.57798287353074</v>
+        <v>-22.33377106455513</v>
       </c>
       <c r="X9" t="n">
-        <v>-12.79368794761072</v>
+        <v>-15.32646191027227</v>
       </c>
       <c r="Y9" t="n">
-        <v>-25.7857790821601</v>
+        <v>-30.60768759773033</v>
       </c>
       <c r="Z9" t="n">
-        <v>-34.96312404761855</v>
+        <v>-20.46411527554369</v>
       </c>
       <c r="AA9" t="n">
-        <v>-22.19671755981662</v>
+        <v>-23.22764307299513</v>
       </c>
       <c r="AB9" t="n">
-        <v>-40.22438644770011</v>
+        <v>-31.97048834550982</v>
       </c>
       <c r="AC9" t="n">
-        <v>-60.69967746103092</v>
+        <v>-41.01208512287833</v>
       </c>
     </row>
     <row r="10">
@@ -1238,88 +1238,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-10.91708287244365</v>
+        <v>-19.79819545194769</v>
       </c>
       <c r="C10" t="n">
-        <v>-13.43363550177162</v>
+        <v>-6.902620810424926</v>
       </c>
       <c r="D10" t="n">
-        <v>-2.629801609906425</v>
+        <v>-4.76221881550526</v>
       </c>
       <c r="E10" t="n">
-        <v>16.65608577528276</v>
+        <v>0.4223071288471765</v>
       </c>
       <c r="F10" t="n">
-        <v>-12.66860246768684</v>
+        <v>2.849102781583942</v>
       </c>
       <c r="G10" t="n">
-        <v>-12.75563055005234</v>
+        <v>2.28912769641107</v>
       </c>
       <c r="H10" t="n">
-        <v>-5.365146776386793</v>
+        <v>-25.73666185244208</v>
       </c>
       <c r="I10" t="n">
-        <v>14.48308914207417</v>
+        <v>-5.330575029396122</v>
       </c>
       <c r="J10" t="n">
-        <v>-14.62154342483526</v>
+        <v>-21.22193682019407</v>
       </c>
       <c r="K10" t="n">
-        <v>-18.92452028896291</v>
+        <v>-6.303878829915901</v>
       </c>
       <c r="L10" t="n">
-        <v>-3.886024555525826</v>
+        <v>-20.90383080263397</v>
       </c>
       <c r="M10" t="n">
-        <v>6.17018561991532</v>
+        <v>-19.63985550215957</v>
       </c>
       <c r="N10" t="n">
-        <v>19.34085352294499</v>
+        <v>-14.53743141211644</v>
       </c>
       <c r="O10" t="n">
-        <v>-21.16665124422441</v>
+        <v>-30.16439051557035</v>
       </c>
       <c r="P10" t="n">
-        <v>0.2796491528482701</v>
+        <v>-24.08480920057367</v>
       </c>
       <c r="Q10" t="n">
-        <v>-14.80517159254043</v>
+        <v>-21.10283190301825</v>
       </c>
       <c r="R10" t="n">
-        <v>10.36458046664092</v>
+        <v>-7.272683277192602</v>
       </c>
       <c r="S10" t="n">
-        <v>-15.98245042028558</v>
+        <v>-9.698866220380282</v>
       </c>
       <c r="T10" t="n">
-        <v>-28.84901982645899</v>
+        <v>-25.07942328693183</v>
       </c>
       <c r="U10" t="n">
-        <v>-5.858264975682322</v>
+        <v>-6.065514002900872</v>
       </c>
       <c r="V10" t="n">
-        <v>-10.59607057114103</v>
+        <v>-16.48770860505826</v>
       </c>
       <c r="W10" t="n">
-        <v>-14.19691473768326</v>
+        <v>-27.69687227940149</v>
       </c>
       <c r="X10" t="n">
-        <v>-24.59244362525473</v>
+        <v>-17.41143834635319</v>
       </c>
       <c r="Y10" t="n">
-        <v>-32.50160311751056</v>
+        <v>-7.825362645180187</v>
       </c>
       <c r="Z10" t="n">
-        <v>-23.7708578843086</v>
+        <v>-25.34189778581194</v>
       </c>
       <c r="AA10" t="n">
-        <v>-25.30730275392791</v>
+        <v>-20.06159077635053</v>
       </c>
       <c r="AB10" t="n">
-        <v>-35.79605981899367</v>
+        <v>-16.46329472551048</v>
       </c>
       <c r="AC10" t="n">
-        <v>-52.35480746120744</v>
+        <v>-56.50039570520566</v>
       </c>
     </row>
     <row r="11">
@@ -1327,88 +1327,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-7.438279216612668</v>
+        <v>1.283811050688735</v>
       </c>
       <c r="C11" t="n">
-        <v>-15.57534266806742</v>
+        <v>-8.244503331564836</v>
       </c>
       <c r="D11" t="n">
-        <v>-15.84403293409424</v>
+        <v>-24.92069436001444</v>
       </c>
       <c r="E11" t="n">
-        <v>-6.395560689778394</v>
+        <v>-5.491207259887902</v>
       </c>
       <c r="F11" t="n">
-        <v>-13.45025334629554</v>
+        <v>-4.598493789137732</v>
       </c>
       <c r="G11" t="n">
-        <v>-7.192563180471688</v>
+        <v>-13.33353959572788</v>
       </c>
       <c r="H11" t="n">
-        <v>-1.786060692122788</v>
+        <v>-9.275083549139813</v>
       </c>
       <c r="I11" t="n">
-        <v>-6.115630983832726</v>
+        <v>-4.528529035564008</v>
       </c>
       <c r="J11" t="n">
-        <v>5.974395419075162</v>
+        <v>-11.28418063421509</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2551007902877345</v>
+        <v>-2.841061189802809</v>
       </c>
       <c r="L11" t="n">
-        <v>-3.857617771833592</v>
+        <v>-19.5033934991747</v>
       </c>
       <c r="M11" t="n">
-        <v>13.39888581348286</v>
+        <v>-9.662547941524112</v>
       </c>
       <c r="N11" t="n">
-        <v>-17.29652414679305</v>
+        <v>0.6583618569473071</v>
       </c>
       <c r="O11" t="n">
-        <v>-8.248244939274135</v>
+        <v>0.4949692679927216</v>
       </c>
       <c r="P11" t="n">
-        <v>-10.73928019881163</v>
+        <v>1.586705627760564</v>
       </c>
       <c r="Q11" t="n">
-        <v>-7.811845471884364</v>
+        <v>-1.465949834745182</v>
       </c>
       <c r="R11" t="n">
-        <v>0.5232552771941368</v>
+        <v>-7.956253408544852</v>
       </c>
       <c r="S11" t="n">
-        <v>-6.339811832216146</v>
+        <v>-31.53236511050618</v>
       </c>
       <c r="T11" t="n">
-        <v>-3.921304934591928</v>
+        <v>-5.369294585568845</v>
       </c>
       <c r="U11" t="n">
-        <v>-1.289565758957272</v>
+        <v>-1.083194744395557</v>
       </c>
       <c r="V11" t="n">
-        <v>-1.359823021296673</v>
+        <v>-23.33229816093734</v>
       </c>
       <c r="W11" t="n">
-        <v>-13.47856713210816</v>
+        <v>-22.05189009004159</v>
       </c>
       <c r="X11" t="n">
-        <v>-13.13646435321342</v>
+        <v>-24.23231031288725</v>
       </c>
       <c r="Y11" t="n">
-        <v>-34.1076081222966</v>
+        <v>-27.09881683208349</v>
       </c>
       <c r="Z11" t="n">
-        <v>-16.81324086423653</v>
+        <v>-24.47042017577613</v>
       </c>
       <c r="AA11" t="n">
-        <v>-22.76399274279718</v>
+        <v>-19.90809009207921</v>
       </c>
       <c r="AB11" t="n">
-        <v>-30.82755430005296</v>
+        <v>-38.58700187047955</v>
       </c>
       <c r="AC11" t="n">
-        <v>-56.46165494482593</v>
+        <v>-64.18381610591747</v>
       </c>
     </row>
   </sheetData>
@@ -1521,88 +1521,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.172052827782203</v>
+        <v>-8.445699459704631</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.674239514764215</v>
+        <v>-4.862194063725537</v>
       </c>
       <c r="D2" t="n">
-        <v>9.230211477795908</v>
+        <v>-15.89688220623006</v>
       </c>
       <c r="E2" t="n">
-        <v>8.391353905848883</v>
+        <v>11.77947903359717</v>
       </c>
       <c r="F2" t="n">
-        <v>1.420214415521063</v>
+        <v>-6.66564250290854</v>
       </c>
       <c r="G2" t="n">
-        <v>-17.78135057820563</v>
+        <v>2.563856657654434</v>
       </c>
       <c r="H2" t="n">
-        <v>1.35555889739316</v>
+        <v>-7.525171312768133</v>
       </c>
       <c r="I2" t="n">
-        <v>-9.420699302424801</v>
+        <v>1.078057486706943</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.521874756177716</v>
+        <v>4.671951277104801</v>
       </c>
       <c r="K2" t="n">
-        <v>-4.288209367836984</v>
+        <v>6.33926806330791</v>
       </c>
       <c r="L2" t="n">
-        <v>5.881083591827855</v>
+        <v>16.66427753005458</v>
       </c>
       <c r="M2" t="n">
-        <v>-3.940134067118988</v>
+        <v>-3.522338165741361</v>
       </c>
       <c r="N2" t="n">
-        <v>8.29212387821878</v>
+        <v>-5.447083475939571</v>
       </c>
       <c r="O2" t="n">
-        <v>4.647742389256814</v>
+        <v>-1.232763537488992</v>
       </c>
       <c r="P2" t="n">
-        <v>31.67549457351596</v>
+        <v>-2.259433602552217</v>
       </c>
       <c r="Q2" t="n">
-        <v>-3.157243490686982</v>
+        <v>19.39683600957655</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.8554140405675237</v>
+        <v>9.205135260614771</v>
       </c>
       <c r="S2" t="n">
-        <v>3.487180593396078</v>
+        <v>-6.14441831949676</v>
       </c>
       <c r="T2" t="n">
-        <v>-9.33366002243206</v>
+        <v>11.18054610266636</v>
       </c>
       <c r="U2" t="n">
-        <v>-2.877685234021543</v>
+        <v>1.651402166182923</v>
       </c>
       <c r="V2" t="n">
-        <v>5.023193999845203</v>
+        <v>-8.056800272561631</v>
       </c>
       <c r="W2" t="n">
-        <v>-16.94335248371687</v>
+        <v>-0.1033516370600798</v>
       </c>
       <c r="X2" t="n">
-        <v>-15.9275501834807</v>
+        <v>-13.85436283191828</v>
       </c>
       <c r="Y2" t="n">
-        <v>5.578681963972844</v>
+        <v>3.492158701691356</v>
       </c>
       <c r="Z2" t="n">
-        <v>-7.163841325317901</v>
+        <v>-0.4898191886065604</v>
       </c>
       <c r="AA2" t="n">
-        <v>-14.1083254406283</v>
+        <v>-4.144477416462786</v>
       </c>
       <c r="AB2" t="n">
-        <v>-7.312932864920183</v>
+        <v>-8.076866511191284</v>
       </c>
       <c r="AC2" t="n">
-        <v>-4.869424213048415</v>
+        <v>1.967220948076386</v>
       </c>
     </row>
     <row r="3">
@@ -1610,88 +1610,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2711978450583876</v>
+        <v>-4.703918524380742</v>
       </c>
       <c r="C3" t="n">
-        <v>5.782068509114335</v>
+        <v>-7.384701731819304</v>
       </c>
       <c r="D3" t="n">
-        <v>-22.79759651781352</v>
+        <v>-17.12908476817802</v>
       </c>
       <c r="E3" t="n">
-        <v>-10.1142992142409</v>
+        <v>13.1006902674003</v>
       </c>
       <c r="F3" t="n">
-        <v>-13.90412239175617</v>
+        <v>-8.919978352751468</v>
       </c>
       <c r="G3" t="n">
-        <v>-12.29609346028762</v>
+        <v>-7.793667272376371</v>
       </c>
       <c r="H3" t="n">
-        <v>-18.68230122739583</v>
+        <v>-15.46447442159888</v>
       </c>
       <c r="I3" t="n">
-        <v>-8.204210351252447</v>
+        <v>-7.596156118479681</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.955508387658559</v>
+        <v>-16.6511084491566</v>
       </c>
       <c r="K3" t="n">
-        <v>-2.597572777081974</v>
+        <v>2.329175800029099</v>
       </c>
       <c r="L3" t="n">
-        <v>8.433556386321923</v>
+        <v>-15.42391788323441</v>
       </c>
       <c r="M3" t="n">
-        <v>7.395550828650586</v>
+        <v>-1.772978384570476</v>
       </c>
       <c r="N3" t="n">
-        <v>-20.4486835971118</v>
+        <v>-2.279131274530956</v>
       </c>
       <c r="O3" t="n">
-        <v>-5.220465495851476</v>
+        <v>-11.49730449259545</v>
       </c>
       <c r="P3" t="n">
-        <v>-15.94230880726302</v>
+        <v>9.172175386560804</v>
       </c>
       <c r="Q3" t="n">
-        <v>-22.60172143529551</v>
+        <v>11.15910059004865</v>
       </c>
       <c r="R3" t="n">
-        <v>10.41754143523284</v>
+        <v>0.3791650468645855</v>
       </c>
       <c r="S3" t="n">
-        <v>-13.41587956276643</v>
+        <v>-5.518081377613904</v>
       </c>
       <c r="T3" t="n">
-        <v>-18.97599535320375</v>
+        <v>1.194147547211803</v>
       </c>
       <c r="U3" t="n">
-        <v>23.27792071788025</v>
+        <v>-3.464616300116811</v>
       </c>
       <c r="V3" t="n">
-        <v>2.162399182685979</v>
+        <v>-11.71753612733431</v>
       </c>
       <c r="W3" t="n">
-        <v>4.002488632455426</v>
+        <v>7.210459328607246</v>
       </c>
       <c r="X3" t="n">
-        <v>0.151221073887263</v>
+        <v>-7.309279403474726</v>
       </c>
       <c r="Y3" t="n">
-        <v>7.90381324545683</v>
+        <v>-1.74135169750864</v>
       </c>
       <c r="Z3" t="n">
-        <v>-12.35283355612831</v>
+        <v>6.953424874641135</v>
       </c>
       <c r="AA3" t="n">
-        <v>-6.580300712313051</v>
+        <v>-9.566716004939725</v>
       </c>
       <c r="AB3" t="n">
-        <v>-2.447200808198393</v>
+        <v>-9.829166651699715</v>
       </c>
       <c r="AC3" t="n">
-        <v>-20.03917596007695</v>
+        <v>-3.294978376047523</v>
       </c>
     </row>
     <row r="4">
@@ -1699,88 +1699,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>6.650664101859102</v>
+        <v>1.96788411156886</v>
       </c>
       <c r="C4" t="n">
-        <v>4.076919366636142</v>
+        <v>9.793360833426242</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.997678503444531</v>
+        <v>2.449572975446845</v>
       </c>
       <c r="E4" t="n">
-        <v>16.26727439537065</v>
+        <v>19.70452590623813</v>
       </c>
       <c r="F4" t="n">
-        <v>-6.097601829750767</v>
+        <v>-18.00356596829654</v>
       </c>
       <c r="G4" t="n">
-        <v>5.271944894311501</v>
+        <v>1.060555171804593</v>
       </c>
       <c r="H4" t="n">
-        <v>12.08844386476253</v>
+        <v>-8.927318896318944</v>
       </c>
       <c r="I4" t="n">
-        <v>5.09278737077323</v>
+        <v>0.7766874153775793</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1430472864025039</v>
+        <v>-21.40813162777153</v>
       </c>
       <c r="K4" t="n">
-        <v>4.362995175143578</v>
+        <v>-5.750874529090413</v>
       </c>
       <c r="L4" t="n">
-        <v>-2.32672068768579</v>
+        <v>-11.29953055288927</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.2184415262802164</v>
+        <v>-11.74913540106592</v>
       </c>
       <c r="N4" t="n">
-        <v>-10.79448668590727</v>
+        <v>-9.687024275935931</v>
       </c>
       <c r="O4" t="n">
-        <v>-8.376869410176342</v>
+        <v>21.44633726923782</v>
       </c>
       <c r="P4" t="n">
-        <v>-4.21170665847609</v>
+        <v>-4.333644245300228</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.986073171958389</v>
+        <v>14.15437335288479</v>
       </c>
       <c r="R4" t="n">
-        <v>-10.12670115101325</v>
+        <v>-2.477744217123757</v>
       </c>
       <c r="S4" t="n">
-        <v>-13.42571283757013</v>
+        <v>0.7085105858664238</v>
       </c>
       <c r="T4" t="n">
-        <v>-8.669741518657286</v>
+        <v>-15.07960216819733</v>
       </c>
       <c r="U4" t="n">
-        <v>-11.45315938717332</v>
+        <v>6.456702166358234</v>
       </c>
       <c r="V4" t="n">
-        <v>-25.69143254894173</v>
+        <v>0.6040383845647335</v>
       </c>
       <c r="W4" t="n">
-        <v>-8.201658587415928</v>
+        <v>8.524903913752267</v>
       </c>
       <c r="X4" t="n">
-        <v>5.117105522678567</v>
+        <v>-11.25129838446836</v>
       </c>
       <c r="Y4" t="n">
-        <v>4.702209281265961</v>
+        <v>-6.163730165653814</v>
       </c>
       <c r="Z4" t="n">
-        <v>-9.364580267616407</v>
+        <v>18.99136237158999</v>
       </c>
       <c r="AA4" t="n">
-        <v>4.472078255486279</v>
+        <v>-6.320691244116416</v>
       </c>
       <c r="AB4" t="n">
-        <v>-17.51896094098132</v>
+        <v>7.458478334669625</v>
       </c>
       <c r="AC4" t="n">
-        <v>14.62062055063519</v>
+        <v>1.350437266684461</v>
       </c>
     </row>
     <row r="5">
@@ -1788,88 +1788,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7.249801312035705</v>
+        <v>5.69540421259098</v>
       </c>
       <c r="C5" t="n">
-        <v>3.960852143124745</v>
+        <v>15.8443387737497</v>
       </c>
       <c r="D5" t="n">
-        <v>11.63782317472828</v>
+        <v>-9.041383510662909</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.874666055545951</v>
+        <v>-1.807895692866627</v>
       </c>
       <c r="F5" t="n">
-        <v>-5.88072052451553</v>
+        <v>-22.93028848654954</v>
       </c>
       <c r="G5" t="n">
-        <v>-9.854683101642273</v>
+        <v>-3.67392416836885</v>
       </c>
       <c r="H5" t="n">
-        <v>-7.579142008861329</v>
+        <v>-19.0499390696505</v>
       </c>
       <c r="I5" t="n">
-        <v>-5.441419785172628</v>
+        <v>2.007711050085545</v>
       </c>
       <c r="J5" t="n">
-        <v>-12.24745033867998</v>
+        <v>-20.86281846529436</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.758200424467303</v>
+        <v>2.397143887738131</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6386539452380897</v>
+        <v>-8.921630328835224</v>
       </c>
       <c r="M5" t="n">
-        <v>-10.04986174426841</v>
+        <v>-12.69261308317471</v>
       </c>
       <c r="N5" t="n">
-        <v>2.421679588557495</v>
+        <v>7.454930149248398</v>
       </c>
       <c r="O5" t="n">
-        <v>-11.09788884453676</v>
+        <v>13.8524889489197</v>
       </c>
       <c r="P5" t="n">
-        <v>12.41993644687087</v>
+        <v>4.97633624219995</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.2694367631813863</v>
+        <v>-3.269501203145849</v>
       </c>
       <c r="R5" t="n">
-        <v>0.5287904391495082</v>
+        <v>-2.254427120216117</v>
       </c>
       <c r="S5" t="n">
-        <v>-5.223851350041984</v>
+        <v>-22.30869218413394</v>
       </c>
       <c r="T5" t="n">
-        <v>-11.8183949118914</v>
+        <v>5.404724735478939</v>
       </c>
       <c r="U5" t="n">
-        <v>-23.32188977949148</v>
+        <v>-14.55394099190735</v>
       </c>
       <c r="V5" t="n">
-        <v>-11.71704153148101</v>
+        <v>4.267262617854231</v>
       </c>
       <c r="W5" t="n">
-        <v>1.878504122858046</v>
+        <v>8.569253848633311</v>
       </c>
       <c r="X5" t="n">
-        <v>11.50825371926567</v>
+        <v>-11.05058435546473</v>
       </c>
       <c r="Y5" t="n">
-        <v>-7.449219830824827</v>
+        <v>-7.364367792150111</v>
       </c>
       <c r="Z5" t="n">
-        <v>-12.95515539044828</v>
+        <v>7.071670998689303</v>
       </c>
       <c r="AA5" t="n">
-        <v>-11.56530209778902</v>
+        <v>14.14281613981135</v>
       </c>
       <c r="AB5" t="n">
-        <v>-3.980173554835531</v>
+        <v>-11.20883218985977</v>
       </c>
       <c r="AC5" t="n">
-        <v>12.13697562998332</v>
+        <v>0.04303784302254421</v>
       </c>
     </row>
     <row r="6">
@@ -1877,88 +1877,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3.70507261626849</v>
+        <v>3.179892551929328</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.381839918165332</v>
+        <v>7.304041360956223</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.262783674211847</v>
+        <v>2.139503181013015</v>
       </c>
       <c r="E6" t="n">
-        <v>7.033408741614167</v>
+        <v>21.32115225012946</v>
       </c>
       <c r="F6" t="n">
-        <v>10.94435450282626</v>
+        <v>-6.922125838414118</v>
       </c>
       <c r="G6" t="n">
-        <v>5.161931831737084</v>
+        <v>-16.90753063634777</v>
       </c>
       <c r="H6" t="n">
-        <v>30.27271627606967</v>
+        <v>8.67484141237636</v>
       </c>
       <c r="I6" t="n">
-        <v>11.21409471753609</v>
+        <v>-9.511256722667447</v>
       </c>
       <c r="J6" t="n">
-        <v>13.61846681316532</v>
+        <v>-13.27015633037353</v>
       </c>
       <c r="K6" t="n">
-        <v>-15.75977444263446</v>
+        <v>-1.125013270616859</v>
       </c>
       <c r="L6" t="n">
-        <v>10.14517500081242</v>
+        <v>-10.67015299958825</v>
       </c>
       <c r="M6" t="n">
-        <v>5.221967997563754</v>
+        <v>-10.58432324433678</v>
       </c>
       <c r="N6" t="n">
-        <v>-12.51317707568159</v>
+        <v>-11.15310070730012</v>
       </c>
       <c r="O6" t="n">
-        <v>-11.12651674820394</v>
+        <v>-1.360848297030258</v>
       </c>
       <c r="P6" t="n">
-        <v>-9.097981903312263</v>
+        <v>-10.31030141346771</v>
       </c>
       <c r="Q6" t="n">
-        <v>-13.64919685473582</v>
+        <v>0.4360796688477184</v>
       </c>
       <c r="R6" t="n">
-        <v>-5.457306400852035</v>
+        <v>16.38307383072669</v>
       </c>
       <c r="S6" t="n">
-        <v>-3.965489553756658</v>
+        <v>-3.628815292795601</v>
       </c>
       <c r="T6" t="n">
-        <v>9.01806345443859</v>
+        <v>20.16238805919677</v>
       </c>
       <c r="U6" t="n">
-        <v>-7.337898290975676</v>
+        <v>2.975537069133482</v>
       </c>
       <c r="V6" t="n">
-        <v>-5.821327532760394</v>
+        <v>3.318608173135195</v>
       </c>
       <c r="W6" t="n">
-        <v>-5.959073337819023</v>
+        <v>4.287128448840129</v>
       </c>
       <c r="X6" t="n">
-        <v>3.949457095319229</v>
+        <v>4.297348869863408</v>
       </c>
       <c r="Y6" t="n">
-        <v>3.243873566077246</v>
+        <v>13.36251912857334</v>
       </c>
       <c r="Z6" t="n">
-        <v>-14.75186850904108</v>
+        <v>-1.325818190106531</v>
       </c>
       <c r="AA6" t="n">
-        <v>-12.84231597838886</v>
+        <v>1.067634855129112</v>
       </c>
       <c r="AB6" t="n">
-        <v>2.291523643989886</v>
+        <v>-0.4388569801243412</v>
       </c>
       <c r="AC6" t="n">
-        <v>-4.693053744453721</v>
+        <v>-5.850561563560658</v>
       </c>
     </row>
     <row r="7">
@@ -1966,88 +1966,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.42827446156997</v>
+        <v>-11.5491570097279</v>
       </c>
       <c r="C7" t="n">
-        <v>-12.09706887775689</v>
+        <v>-3.164142161908076</v>
       </c>
       <c r="D7" t="n">
-        <v>6.138641273755568</v>
+        <v>-0.09112492226020219</v>
       </c>
       <c r="E7" t="n">
-        <v>7.306089305422544</v>
+        <v>-0.4896661936531359</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.660533534343763</v>
+        <v>-2.965875791902664</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.437660351635305</v>
+        <v>-18.64874809014069</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.799080526790589</v>
+        <v>-5.363887656098617</v>
       </c>
       <c r="I7" t="n">
-        <v>9.524509851850004</v>
+        <v>24.15670224402538</v>
       </c>
       <c r="J7" t="n">
-        <v>-23.71570398620651</v>
+        <v>-12.30721989073341</v>
       </c>
       <c r="K7" t="n">
-        <v>-7.290019172497827</v>
+        <v>-3.420981975518997</v>
       </c>
       <c r="L7" t="n">
-        <v>12.32553392691972</v>
+        <v>-5.738221092061988</v>
       </c>
       <c r="M7" t="n">
-        <v>3.370161640343375</v>
+        <v>-2.333185794503485</v>
       </c>
       <c r="N7" t="n">
-        <v>-19.98389699832071</v>
+        <v>1.841576508904545</v>
       </c>
       <c r="O7" t="n">
-        <v>-23.37119647897549</v>
+        <v>3.647772968113578</v>
       </c>
       <c r="P7" t="n">
-        <v>-2.627641344210239</v>
+        <v>-6.750752307649845</v>
       </c>
       <c r="Q7" t="n">
-        <v>-14.18293281140459</v>
+        <v>-5.484008345445941</v>
       </c>
       <c r="R7" t="n">
-        <v>-14.00393935191288</v>
+        <v>-1.787946318722657</v>
       </c>
       <c r="S7" t="n">
-        <v>-9.067715306225567</v>
+        <v>7.847697987326093</v>
       </c>
       <c r="T7" t="n">
-        <v>-17.46075139794996</v>
+        <v>-0.700916487006209</v>
       </c>
       <c r="U7" t="n">
-        <v>9.154638046664799</v>
+        <v>-18.02223587003803</v>
       </c>
       <c r="V7" t="n">
-        <v>-15.37916530580897</v>
+        <v>-5.703493722650853</v>
       </c>
       <c r="W7" t="n">
-        <v>-12.37859514684922</v>
+        <v>-10.93386618612735</v>
       </c>
       <c r="X7" t="n">
-        <v>1.226075765726867</v>
+        <v>2.191117502207945</v>
       </c>
       <c r="Y7" t="n">
-        <v>-8.679509930546459</v>
+        <v>4.260841497552554</v>
       </c>
       <c r="Z7" t="n">
-        <v>9.749051433975604</v>
+        <v>19.29557750612478</v>
       </c>
       <c r="AA7" t="n">
-        <v>-1.217514805952707</v>
+        <v>13.36508815014068</v>
       </c>
       <c r="AB7" t="n">
-        <v>-17.13258988907408</v>
+        <v>-29.7526954062402</v>
       </c>
       <c r="AC7" t="n">
-        <v>-8.842249278383303</v>
+        <v>-6.410806346881802</v>
       </c>
     </row>
     <row r="8">
@@ -2055,88 +2055,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-5.330704726777368</v>
+        <v>-9.487714368200098</v>
       </c>
       <c r="C8" t="n">
-        <v>-4.519151848161956</v>
+        <v>-10.54629348498882</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.081352189690449</v>
+        <v>-18.01023692089304</v>
       </c>
       <c r="E8" t="n">
-        <v>11.74523690251984</v>
+        <v>0.5010206421787267</v>
       </c>
       <c r="F8" t="n">
-        <v>9.817668142333531</v>
+        <v>3.520693305133928</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.225931875383419</v>
+        <v>-16.93469311297584</v>
       </c>
       <c r="H8" t="n">
-        <v>-2.198321913564483</v>
+        <v>-4.19833907938612</v>
       </c>
       <c r="I8" t="n">
-        <v>-4.666185249626632</v>
+        <v>2.131827916228263</v>
       </c>
       <c r="J8" t="n">
-        <v>18.72595686775902</v>
+        <v>-1.307299684998619</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1571253335280023</v>
+        <v>15.14158828693672</v>
       </c>
       <c r="L8" t="n">
-        <v>16.91168581537648</v>
+        <v>-3.230046673618826</v>
       </c>
       <c r="M8" t="n">
-        <v>2.775564745992778</v>
+        <v>-25.35596339003044</v>
       </c>
       <c r="N8" t="n">
-        <v>3.543911812809109</v>
+        <v>12.63027632621623</v>
       </c>
       <c r="O8" t="n">
-        <v>-5.666233526079113</v>
+        <v>-23.43030145702912</v>
       </c>
       <c r="P8" t="n">
-        <v>-4.363121037335343</v>
+        <v>10.86481008290672</v>
       </c>
       <c r="Q8" t="n">
-        <v>-12.92430069286218</v>
+        <v>4.128037866053131</v>
       </c>
       <c r="R8" t="n">
-        <v>10.60702180735076</v>
+        <v>3.820237975486838</v>
       </c>
       <c r="S8" t="n">
-        <v>-3.322755861894566</v>
+        <v>-16.09448771596702</v>
       </c>
       <c r="T8" t="n">
-        <v>-47.78461091136714</v>
+        <v>9.895866262690834</v>
       </c>
       <c r="U8" t="n">
-        <v>-2.009945127749143</v>
+        <v>2.317334035479305</v>
       </c>
       <c r="V8" t="n">
-        <v>-7.888922532946338</v>
+        <v>-1.253336303752502</v>
       </c>
       <c r="W8" t="n">
-        <v>-9.19363984460751</v>
+        <v>-15.29957968862895</v>
       </c>
       <c r="X8" t="n">
-        <v>-22.81527558274766</v>
+        <v>-3.679666939968412</v>
       </c>
       <c r="Y8" t="n">
-        <v>2.80548843590297</v>
+        <v>-4.03339461842495</v>
       </c>
       <c r="Z8" t="n">
-        <v>2.857021008741796</v>
+        <v>6.703046720289267</v>
       </c>
       <c r="AA8" t="n">
-        <v>-7.968612397842811</v>
+        <v>-9.617241695780034</v>
       </c>
       <c r="AB8" t="n">
-        <v>-16.3673410893232</v>
+        <v>-18.55429033488829</v>
       </c>
       <c r="AC8" t="n">
-        <v>-15.64926925732307</v>
+        <v>-9.630250198531394</v>
       </c>
     </row>
     <row r="9">
@@ -2144,88 +2144,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.77116871419472</v>
+        <v>-1.898984775211348</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3835229681466603</v>
+        <v>-5.050551684939466</v>
       </c>
       <c r="D9" t="n">
-        <v>-5.077277941748504</v>
+        <v>-9.504131979289451</v>
       </c>
       <c r="E9" t="n">
-        <v>10.58220971252026</v>
+        <v>10.59053926534656</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.560137315708124</v>
+        <v>-18.134787500035</v>
       </c>
       <c r="G9" t="n">
-        <v>1.977224388791319</v>
+        <v>-6.773941278092058</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.4376201449978383</v>
+        <v>3.985371424650133</v>
       </c>
       <c r="I9" t="n">
-        <v>1.720598213288802</v>
+        <v>2.257050013888467</v>
       </c>
       <c r="J9" t="n">
-        <v>-5.888642863644638</v>
+        <v>-3.131228081658928</v>
       </c>
       <c r="K9" t="n">
-        <v>-1.435066866711035</v>
+        <v>7.262278955497596</v>
       </c>
       <c r="L9" t="n">
-        <v>9.204582151514565</v>
+        <v>9.49733374703329</v>
       </c>
       <c r="M9" t="n">
-        <v>-1.430917340798474</v>
+        <v>-4.908057935475792</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.858227012805996</v>
+        <v>13.57883974637917</v>
       </c>
       <c r="O9" t="n">
-        <v>-3.111367483250241</v>
+        <v>-5.784824944697171</v>
       </c>
       <c r="P9" t="n">
-        <v>-17.29578295122531</v>
+        <v>-8.356984217585614</v>
       </c>
       <c r="Q9" t="n">
-        <v>-3.895978054363177</v>
+        <v>4.775874178313871</v>
       </c>
       <c r="R9" t="n">
-        <v>3.164117546113995</v>
+        <v>17.37444926907451</v>
       </c>
       <c r="S9" t="n">
-        <v>2.324795353095822</v>
+        <v>-21.88207193513947</v>
       </c>
       <c r="T9" t="n">
-        <v>-27.1492750122496</v>
+        <v>-3.098411724621789</v>
       </c>
       <c r="U9" t="n">
-        <v>3.02268747896009</v>
+        <v>2.89438987340292</v>
       </c>
       <c r="V9" t="n">
-        <v>-15.20793207699926</v>
+        <v>-17.32848166671971</v>
       </c>
       <c r="W9" t="n">
-        <v>2.549872646573152</v>
+        <v>26.03938190446221</v>
       </c>
       <c r="X9" t="n">
-        <v>1.267769117770126</v>
+        <v>-3.298573616297135</v>
       </c>
       <c r="Y9" t="n">
-        <v>5.543563507585228</v>
+        <v>-7.960698470846839</v>
       </c>
       <c r="Z9" t="n">
-        <v>19.5109965996788</v>
+        <v>-7.734410007691003</v>
       </c>
       <c r="AA9" t="n">
-        <v>-26.21720476614697</v>
+        <v>-15.34293803644868</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.3250440229087728</v>
+        <v>1.937934573012914</v>
       </c>
       <c r="AC9" t="n">
-        <v>-4.130669470851165</v>
+        <v>-3.218760903742135</v>
       </c>
     </row>
     <row r="10">
@@ -2233,88 +2233,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>5.85183078329058</v>
+        <v>-5.417532623322577</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.036422818493087</v>
+        <v>-11.69386591171691</v>
       </c>
       <c r="D10" t="n">
-        <v>5.732097484873239</v>
+        <v>-16.1455796190507</v>
       </c>
       <c r="E10" t="n">
-        <v>14.35214588689497</v>
+        <v>-0.2707313298397902</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4107274639278828</v>
+        <v>-1.885623856261962</v>
       </c>
       <c r="G10" t="n">
-        <v>-16.41902439642324</v>
+        <v>3.558987314318966</v>
       </c>
       <c r="H10" t="n">
-        <v>-5.203070700484404</v>
+        <v>-1.305763515458318</v>
       </c>
       <c r="I10" t="n">
-        <v>0.725977728086626</v>
+        <v>-0.09936650621417309</v>
       </c>
       <c r="J10" t="n">
-        <v>12.25831051092192</v>
+        <v>-19.67477106923535</v>
       </c>
       <c r="K10" t="n">
-        <v>-17.95278853768609</v>
+        <v>0.2850805195645716</v>
       </c>
       <c r="L10" t="n">
-        <v>-6.604652166040962</v>
+        <v>-11.52912951906626</v>
       </c>
       <c r="M10" t="n">
-        <v>9.005612043795542</v>
+        <v>-13.89887660964032</v>
       </c>
       <c r="N10" t="n">
-        <v>-23.921301090478</v>
+        <v>-10.88851491126718</v>
       </c>
       <c r="O10" t="n">
-        <v>-7.144283016752768</v>
+        <v>2.845491638898932</v>
       </c>
       <c r="P10" t="n">
-        <v>2.799508430708887</v>
+        <v>11.58799355520798</v>
       </c>
       <c r="Q10" t="n">
-        <v>12.38511400870316</v>
+        <v>14.88826541100849</v>
       </c>
       <c r="R10" t="n">
-        <v>2.373691011512811</v>
+        <v>13.62925126979036</v>
       </c>
       <c r="S10" t="n">
-        <v>-7.366289821557237</v>
+        <v>10.23127818649927</v>
       </c>
       <c r="T10" t="n">
-        <v>19.05009207525833</v>
+        <v>-3.55600514412768</v>
       </c>
       <c r="U10" t="n">
-        <v>-16.22099764242396</v>
+        <v>1.976515574589449</v>
       </c>
       <c r="V10" t="n">
-        <v>11.33912381355767</v>
+        <v>-0.8952782819515051</v>
       </c>
       <c r="W10" t="n">
-        <v>8.470214456947028</v>
+        <v>-10.22231149647097</v>
       </c>
       <c r="X10" t="n">
-        <v>0.3468571448880846</v>
+        <v>-13.99694840141624</v>
       </c>
       <c r="Y10" t="n">
-        <v>-33.68641356089268</v>
+        <v>-9.380937028547269</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.5741448929776931</v>
+        <v>-9.990080843538729</v>
       </c>
       <c r="AA10" t="n">
-        <v>-26.43656511071521</v>
+        <v>2.307297557052507</v>
       </c>
       <c r="AB10" t="n">
-        <v>-15.29608504540723</v>
+        <v>1.154772315805278</v>
       </c>
       <c r="AC10" t="n">
-        <v>-4.152946078693965</v>
+        <v>-3.211795851472504</v>
       </c>
     </row>
     <row r="11">
@@ -2322,88 +2322,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-7.803805675006642</v>
+        <v>-5.803780916214143</v>
       </c>
       <c r="C11" t="n">
-        <v>12.26302218760857</v>
+        <v>2.30433470568707</v>
       </c>
       <c r="D11" t="n">
-        <v>-9.246691115505206</v>
+        <v>5.894405827213402</v>
       </c>
       <c r="E11" t="n">
-        <v>3.665147861656605</v>
+        <v>6.607366362117334</v>
       </c>
       <c r="F11" t="n">
-        <v>1.30163600830967</v>
+        <v>0.1795947928747172</v>
       </c>
       <c r="G11" t="n">
-        <v>5.053475332051267</v>
+        <v>-9.946795262272431</v>
       </c>
       <c r="H11" t="n">
-        <v>2.645366136854734</v>
+        <v>-10.84170992544662</v>
       </c>
       <c r="I11" t="n">
-        <v>6.702309322528359</v>
+        <v>0.09090767135536426</v>
       </c>
       <c r="J11" t="n">
-        <v>4.282218729702221</v>
+        <v>-17.4453570347133</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.4853418980845121</v>
+        <v>16.18535308066385</v>
       </c>
       <c r="L11" t="n">
-        <v>-17.7042177112452</v>
+        <v>-13.41977381348576</v>
       </c>
       <c r="M11" t="n">
-        <v>7.662157359426617</v>
+        <v>-6.960191808726066</v>
       </c>
       <c r="N11" t="n">
-        <v>0.143246720603289</v>
+        <v>-15.58782468688498</v>
       </c>
       <c r="O11" t="n">
-        <v>-9.538213193488369</v>
+        <v>19.47823103185367</v>
       </c>
       <c r="P11" t="n">
-        <v>3.534338503732497</v>
+        <v>-10.39249478609842</v>
       </c>
       <c r="Q11" t="n">
-        <v>-2.547399780728361</v>
+        <v>1.679285639895129</v>
       </c>
       <c r="R11" t="n">
-        <v>-26.60058146220826</v>
+        <v>5.792273192994559</v>
       </c>
       <c r="S11" t="n">
-        <v>4.153749037396857</v>
+        <v>-6.428430438611606</v>
       </c>
       <c r="T11" t="n">
-        <v>-3.240602590318008</v>
+        <v>-3.290580108857488</v>
       </c>
       <c r="U11" t="n">
-        <v>-11.12106969437727</v>
+        <v>-4.01387247521526</v>
       </c>
       <c r="V11" t="n">
-        <v>-1.901512772442379</v>
+        <v>-9.774757416276827</v>
       </c>
       <c r="W11" t="n">
-        <v>-9.190135546460136</v>
+        <v>-8.087235273940696</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1321704543242745</v>
+        <v>-10.80958925113302</v>
       </c>
       <c r="Y11" t="n">
-        <v>-19.16408372188281</v>
+        <v>18.99561005351461</v>
       </c>
       <c r="Z11" t="n">
-        <v>-11.38115579510432</v>
+        <v>-2.703777173911718</v>
       </c>
       <c r="AA11" t="n">
-        <v>-9.374369738834472</v>
+        <v>0.5165469295324172</v>
       </c>
       <c r="AB11" t="n">
-        <v>-2.073077524193826</v>
+        <v>-2.938647882657365</v>
       </c>
       <c r="AC11" t="n">
-        <v>2.70910961666495</v>
+        <v>24.14875703831298</v>
       </c>
     </row>
   </sheetData>
@@ -2516,88 +2516,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.02796128671746834</v>
+        <v>-11.82067171103876</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3819729061633046</v>
+        <v>8.726748548575348</v>
       </c>
       <c r="D2" t="n">
-        <v>6.158412738630259</v>
+        <v>4.267524925961021</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.571026170150949</v>
+        <v>-0.6536713277386399</v>
       </c>
       <c r="F2" t="n">
-        <v>14.69610895412941</v>
+        <v>4.119206919697215</v>
       </c>
       <c r="G2" t="n">
-        <v>-24.94549553353305</v>
+        <v>-0.7704658907991684</v>
       </c>
       <c r="H2" t="n">
-        <v>15.44251054128004</v>
+        <v>2.930229259348289</v>
       </c>
       <c r="I2" t="n">
-        <v>16.96559620804861</v>
+        <v>-19.74581047170735</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5285972873336195</v>
+        <v>7.625541190602304</v>
       </c>
       <c r="K2" t="n">
-        <v>10.12342215840299</v>
+        <v>7.175884822735918</v>
       </c>
       <c r="L2" t="n">
-        <v>6.869751002594024</v>
+        <v>-20.63894792286762</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0272309797578989</v>
+        <v>3.881828170585614</v>
       </c>
       <c r="N2" t="n">
-        <v>4.831513807268457</v>
+        <v>-15.49147567784482</v>
       </c>
       <c r="O2" t="n">
-        <v>-1.299918245749157</v>
+        <v>8.079012344252993</v>
       </c>
       <c r="P2" t="n">
-        <v>11.10475875479897</v>
+        <v>-13.25388363211106</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.9645870158577077</v>
+        <v>-14.18745537687296</v>
       </c>
       <c r="R2" t="n">
-        <v>-5.910161174662545</v>
+        <v>7.263392546524384</v>
       </c>
       <c r="S2" t="n">
-        <v>-15.80997580891831</v>
+        <v>-15.77921126800205</v>
       </c>
       <c r="T2" t="n">
-        <v>-5.250052265624571</v>
+        <v>4.320778800946329</v>
       </c>
       <c r="U2" t="n">
-        <v>-18.22018211046048</v>
+        <v>-11.47399778578884</v>
       </c>
       <c r="V2" t="n">
-        <v>-2.33860320145459</v>
+        <v>-10.97064856577721</v>
       </c>
       <c r="W2" t="n">
-        <v>-16.19060902078101</v>
+        <v>-1.857933487979964</v>
       </c>
       <c r="X2" t="n">
-        <v>-14.1784933237859</v>
+        <v>-1.429640772471988</v>
       </c>
       <c r="Y2" t="n">
-        <v>-3.744748366608281</v>
+        <v>-5.944332643392298</v>
       </c>
       <c r="Z2" t="n">
-        <v>-19.27076290826347</v>
+        <v>4.175096498703073</v>
       </c>
       <c r="AA2" t="n">
-        <v>-12.99155232557535</v>
+        <v>-28.39176124135981</v>
       </c>
       <c r="AB2" t="n">
-        <v>-19.15845325215755</v>
+        <v>-8.803471318909994</v>
       </c>
       <c r="AC2" t="n">
-        <v>-48.69242371231837</v>
+        <v>-41.39606310740389</v>
       </c>
     </row>
     <row r="3">
@@ -2605,88 +2605,88 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.864285279106787</v>
+        <v>-16.94790968237312</v>
       </c>
       <c r="C3" t="n">
-        <v>2.537458523216923</v>
+        <v>-11.62188119921013</v>
       </c>
       <c r="D3" t="n">
-        <v>2.452914214781187</v>
+        <v>-5.358798950098826</v>
       </c>
       <c r="E3" t="n">
-        <v>-17.4858354434803</v>
+        <v>-4.683155295688005</v>
       </c>
       <c r="F3" t="n">
-        <v>12.43925176592394</v>
+        <v>-14.42090544026057</v>
       </c>
       <c r="G3" t="n">
-        <v>-21.38770548687035</v>
+        <v>-15.67730812338714</v>
       </c>
       <c r="H3" t="n">
-        <v>-3.899287853765309</v>
+        <v>-17.98741896048194</v>
       </c>
       <c r="I3" t="n">
-        <v>12.43863297633446</v>
+        <v>-7.834353487757377</v>
       </c>
       <c r="J3" t="n">
-        <v>-16.7364659883492</v>
+        <v>-4.9669640013528</v>
       </c>
       <c r="K3" t="n">
-        <v>-12.24553154205508</v>
+        <v>-28.75006310376186</v>
       </c>
       <c r="L3" t="n">
-        <v>-9.166445308372442</v>
+        <v>2.031988676315429</v>
       </c>
       <c r="M3" t="n">
-        <v>-9.912836727230022</v>
+        <v>15.50820611764182</v>
       </c>
       <c r="N3" t="n">
-        <v>1.132475227795443</v>
+        <v>0.6109380571451677</v>
       </c>
       <c r="O3" t="n">
-        <v>-10.16648633217011</v>
+        <v>-10.69841352279428</v>
       </c>
       <c r="P3" t="n">
-        <v>-27.73472465557443</v>
+        <v>-21.86771121364729</v>
       </c>
       <c r="Q3" t="n">
-        <v>-11.54505730852585</v>
+        <v>-10.3821520385503</v>
       </c>
       <c r="R3" t="n">
-        <v>7.407364383536129</v>
+        <v>3.4819536462878</v>
       </c>
       <c r="S3" t="n">
-        <v>-19.60227041315398</v>
+        <v>-6.601069874086791</v>
       </c>
       <c r="T3" t="n">
-        <v>-9.212951220424173</v>
+        <v>-1.648739501752539</v>
       </c>
       <c r="U3" t="n">
-        <v>-7.780376082551659</v>
+        <v>-7.932649576409164</v>
       </c>
       <c r="V3" t="n">
-        <v>-17.26344355364227</v>
+        <v>-29.00389214601918</v>
       </c>
       <c r="W3" t="n">
-        <v>-12.04405378100707</v>
+        <v>-13.75756075645067</v>
       </c>
       <c r="X3" t="n">
-        <v>-11.72352800892578</v>
+        <v>-2.585793525559178</v>
       </c>
       <c r="Y3" t="n">
-        <v>-15.37514147951346</v>
+        <v>-7.676320221983371</v>
       </c>
       <c r="Z3" t="n">
-        <v>6.499954834011596</v>
+        <v>-10.08209651484703</v>
       </c>
       <c r="AA3" t="n">
-        <v>-21.81947082817397</v>
+        <v>-22.16813334412639</v>
       </c>
       <c r="AB3" t="n">
-        <v>-17.41401704346037</v>
+        <v>-4.600520653722944</v>
       </c>
       <c r="AC3" t="n">
-        <v>-30.99878697137235</v>
+        <v>-31.07035354616133</v>
       </c>
     </row>
     <row r="4">
@@ -2694,88 +2694,88 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19.56122267201161</v>
+        <v>-4.839513657942192</v>
       </c>
       <c r="C4" t="n">
-        <v>9.787938783755033</v>
+        <v>6.53967324899368</v>
       </c>
       <c r="D4" t="n">
-        <v>10.61719230059232</v>
+        <v>19.11750044879022</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.720387893558975</v>
+        <v>-10.31826086516283</v>
       </c>
       <c r="F4" t="n">
-        <v>11.04728824075062</v>
+        <v>-6.806026926225879</v>
       </c>
       <c r="G4" t="n">
-        <v>2.307943224358645</v>
+        <v>-25.0526589369119</v>
       </c>
       <c r="H4" t="n">
-        <v>10.59037338469633</v>
+        <v>-21.21735327493536</v>
       </c>
       <c r="I4" t="n">
-        <v>-4.068827223717409</v>
+        <v>2.911602225575698</v>
       </c>
       <c r="J4" t="n">
-        <v>-13.48238533019636</v>
+        <v>9.620448230639152</v>
       </c>
       <c r="K4" t="n">
-        <v>-7.15021327159322</v>
+        <v>15.97331702273044</v>
       </c>
       <c r="L4" t="n">
-        <v>19.47654306802843</v>
+        <v>-0.400615693395614</v>
       </c>
       <c r="M4" t="n">
-        <v>-12.68972735006388</v>
+        <v>-12.25883270681523</v>
       </c>
       <c r="N4" t="n">
-        <v>-6.336013583167611</v>
+        <v>-13.11748496073857</v>
       </c>
       <c r="O4" t="n">
-        <v>-4.445443749083811</v>
+        <v>-0.1392639755792497</v>
       </c>
       <c r="P4" t="n">
-        <v>-6.726183534159651</v>
+        <v>-5.977484828873105</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.570600441491376</v>
+        <v>-19.44668051854613</v>
       </c>
       <c r="R4" t="n">
-        <v>-19.09842838530822</v>
+        <v>-8.80673940794882</v>
       </c>
       <c r="S4" t="n">
-        <v>12.71744728321571</v>
+        <v>-15.97015419744475</v>
       </c>
       <c r="T4" t="n">
-        <v>-8.317129588566498</v>
+        <v>-2.597338392924615</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9167027316866552</v>
+        <v>-3.092388827180172</v>
       </c>
       <c r="V4" t="n">
-        <v>-17.14792614358366</v>
+        <v>8.443310182828382</v>
       </c>
       <c r="W4" t="n">
-        <v>4.240344592620594</v>
+        <v>12.75622526377611</v>
       </c>
       <c r="X4" t="n">
-        <v>-5.752376774945507</v>
+        <v>3.176632091714088</v>
       </c>
       <c r="Y4" t="n">
-        <v>7.115398159945938</v>
+        <v>-20.5756990460565</v>
       </c>
       <c r="Z4" t="n">
-        <v>-6.993770536651587</v>
+        <v>0.1350901041329546</v>
       </c>
       <c r="AA4" t="n">
-        <v>-22.25605726647287</v>
+        <v>-5.121551253197074</v>
       </c>
       <c r="AB4" t="n">
-        <v>-5.317112574682394</v>
+        <v>-11.45179433426688</v>
       </c>
       <c r="AC4" t="n">
-        <v>1.744823645115162</v>
+        <v>-35.66936050847141</v>
       </c>
     </row>
     <row r="5">
@@ -2783,88 +2783,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2.888665530931882</v>
+        <v>0.8564241484497042</v>
       </c>
       <c r="C5" t="n">
-        <v>-14.5970437626127</v>
+        <v>-7.476852344089739</v>
       </c>
       <c r="D5" t="n">
-        <v>1.817772545787577</v>
+        <v>-12.49013320649768</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.423102560515957</v>
+        <v>6.107314116929471</v>
       </c>
       <c r="F5" t="n">
-        <v>-13.43687034715616</v>
+        <v>-8.903138175978349</v>
       </c>
       <c r="G5" t="n">
-        <v>1.085805627200021</v>
+        <v>-16.91077507026007</v>
       </c>
       <c r="H5" t="n">
-        <v>-8.434663814425543</v>
+        <v>-15.47305673262009</v>
       </c>
       <c r="I5" t="n">
-        <v>14.09617639151763</v>
+        <v>-1.515991562119174</v>
       </c>
       <c r="J5" t="n">
-        <v>-33.01457735337762</v>
+        <v>-1.427247358790395</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.86474935386199</v>
+        <v>-22.76224368886097</v>
       </c>
       <c r="L5" t="n">
-        <v>-4.454960310658699</v>
+        <v>15.06103336748857</v>
       </c>
       <c r="M5" t="n">
-        <v>-10.55961550159377</v>
+        <v>-17.52531352008921</v>
       </c>
       <c r="N5" t="n">
-        <v>-10.69566619817071</v>
+        <v>-15.4839363322223</v>
       </c>
       <c r="O5" t="n">
-        <v>1.767221905274162</v>
+        <v>-7.994138963824208</v>
       </c>
       <c r="P5" t="n">
-        <v>-1.010237605224116</v>
+        <v>-14.12427060111342</v>
       </c>
       <c r="Q5" t="n">
-        <v>-10.14461799588224</v>
+        <v>-9.974912337127002</v>
       </c>
       <c r="R5" t="n">
-        <v>-8.403374546435654</v>
+        <v>7.831240285440626</v>
       </c>
       <c r="S5" t="n">
-        <v>-11.04991280750325</v>
+        <v>-7.589247767652509</v>
       </c>
       <c r="T5" t="n">
-        <v>-14.20477415246652</v>
+        <v>-11.3840530590101</v>
       </c>
       <c r="U5" t="n">
-        <v>-8.348920194449562</v>
+        <v>-4.507649000703443</v>
       </c>
       <c r="V5" t="n">
-        <v>-1.72758425666037</v>
+        <v>-11.87654273985714</v>
       </c>
       <c r="W5" t="n">
-        <v>8.008206220835174</v>
+        <v>-13.58343908620171</v>
       </c>
       <c r="X5" t="n">
-        <v>8.78302359981549</v>
+        <v>8.27726142643284</v>
       </c>
       <c r="Y5" t="n">
-        <v>-7.791261222540793</v>
+        <v>-21.36000318293432</v>
       </c>
       <c r="Z5" t="n">
-        <v>1.814503218890684</v>
+        <v>13.11023386972459</v>
       </c>
       <c r="AA5" t="n">
-        <v>-8.417437376829961</v>
+        <v>-16.74469773150762</v>
       </c>
       <c r="AB5" t="n">
-        <v>-24.05767008040989</v>
+        <v>-16.90650244946344</v>
       </c>
       <c r="AC5" t="n">
-        <v>-8.677197093655046</v>
+        <v>-54.68863172876889</v>
       </c>
     </row>
     <row r="6">
@@ -2872,88 +2872,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>18.25984761615328</v>
+        <v>7.651614100858552</v>
       </c>
       <c r="C6" t="n">
-        <v>-11.70807136236171</v>
+        <v>2.982350242261731</v>
       </c>
       <c r="D6" t="n">
-        <v>8.967226534571175</v>
+        <v>-9.423333829321006</v>
       </c>
       <c r="E6" t="n">
-        <v>-13.62376397950574</v>
+        <v>-2.123044486343237</v>
       </c>
       <c r="F6" t="n">
-        <v>1.462837751716841</v>
+        <v>10.52802277054863</v>
       </c>
       <c r="G6" t="n">
-        <v>19.29205687024721</v>
+        <v>-7.064597153999751</v>
       </c>
       <c r="H6" t="n">
-        <v>9.239676056687101</v>
+        <v>12.70408493941412</v>
       </c>
       <c r="I6" t="n">
-        <v>2.730652856024066</v>
+        <v>-0.771879458547382</v>
       </c>
       <c r="J6" t="n">
-        <v>11.79309436827856</v>
+        <v>7.55024441805049</v>
       </c>
       <c r="K6" t="n">
-        <v>9.107769842422151</v>
+        <v>-6.732961033964751</v>
       </c>
       <c r="L6" t="n">
-        <v>1.052016906885443</v>
+        <v>1.01804234719919</v>
       </c>
       <c r="M6" t="n">
-        <v>-12.07524355350391</v>
+        <v>6.049847242443797</v>
       </c>
       <c r="N6" t="n">
-        <v>-14.36490040191739</v>
+        <v>-19.79404415843948</v>
       </c>
       <c r="O6" t="n">
-        <v>9.731448930476498</v>
+        <v>18.19490563739133</v>
       </c>
       <c r="P6" t="n">
-        <v>12.48987501028055</v>
+        <v>16.65774256994644</v>
       </c>
       <c r="Q6" t="n">
-        <v>-2.084424055198647</v>
+        <v>-9.963191788770876</v>
       </c>
       <c r="R6" t="n">
-        <v>6.151423196632913</v>
+        <v>-8.739759981814199</v>
       </c>
       <c r="S6" t="n">
-        <v>-3.874096545667936</v>
+        <v>0.7120890284270835</v>
       </c>
       <c r="T6" t="n">
-        <v>-6.326336195271618</v>
+        <v>-18.61659693709531</v>
       </c>
       <c r="U6" t="n">
-        <v>-9.301082347478378</v>
+        <v>1.768827057095822</v>
       </c>
       <c r="V6" t="n">
-        <v>2.686584690881761</v>
+        <v>9.178223178747952</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.3772993042880008</v>
+        <v>0.1670004055298744</v>
       </c>
       <c r="X6" t="n">
-        <v>-7.804796341241982</v>
+        <v>11.98721579785152</v>
       </c>
       <c r="Y6" t="n">
-        <v>9.003723784571372</v>
+        <v>-0.1143203181843759</v>
       </c>
       <c r="Z6" t="n">
-        <v>-6.859229640652614</v>
+        <v>-4.017185308309948</v>
       </c>
       <c r="AA6" t="n">
-        <v>-28.28539383306158</v>
+        <v>-27.4778044891386</v>
       </c>
       <c r="AB6" t="n">
-        <v>-35.23895702924737</v>
+        <v>3.514931842842902</v>
       </c>
       <c r="AC6" t="n">
-        <v>-15.1099630904546</v>
+        <v>-28.30841831843108</v>
       </c>
     </row>
     <row r="7">
@@ -2961,88 +2961,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-9.400270174058097</v>
+        <v>3.435242626192617</v>
       </c>
       <c r="C7" t="n">
-        <v>-5.45825684432053</v>
+        <v>-6.211067367464246</v>
       </c>
       <c r="D7" t="n">
-        <v>12.25767304154306</v>
+        <v>2.428545967542385</v>
       </c>
       <c r="E7" t="n">
-        <v>-5.090433125477024</v>
+        <v>2.845883260940616</v>
       </c>
       <c r="F7" t="n">
-        <v>-10.84131825839479</v>
+        <v>1.974166652740444</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.897749560717534</v>
+        <v>-24.05439544074044</v>
       </c>
       <c r="H7" t="n">
-        <v>4.206673694839168</v>
+        <v>-13.9390486926758</v>
       </c>
       <c r="I7" t="n">
-        <v>11.56536068492468</v>
+        <v>3.938970407756906</v>
       </c>
       <c r="J7" t="n">
-        <v>-7.996958900622339</v>
+        <v>-5.411435738014069</v>
       </c>
       <c r="K7" t="n">
-        <v>4.829409560544027</v>
+        <v>14.03817134799943</v>
       </c>
       <c r="L7" t="n">
-        <v>-2.350410321544017</v>
+        <v>-12.23764753788003</v>
       </c>
       <c r="M7" t="n">
-        <v>5.062343604394859</v>
+        <v>-11.83969584341656</v>
       </c>
       <c r="N7" t="n">
-        <v>-5.363748184455617</v>
+        <v>0.7780602366001466</v>
       </c>
       <c r="O7" t="n">
-        <v>3.658192911289466</v>
+        <v>-8.661515140153124</v>
       </c>
       <c r="P7" t="n">
-        <v>-2.122798518479216</v>
+        <v>-3.739563792826059</v>
       </c>
       <c r="Q7" t="n">
-        <v>7.727013396924283</v>
+        <v>-3.781839073044715</v>
       </c>
       <c r="R7" t="n">
-        <v>0.183672656981078</v>
+        <v>28.66428693032623</v>
       </c>
       <c r="S7" t="n">
-        <v>15.25568694523747</v>
+        <v>-17.2511790601209</v>
       </c>
       <c r="T7" t="n">
-        <v>3.098848849550146</v>
+        <v>17.99735417640368</v>
       </c>
       <c r="U7" t="n">
-        <v>-13.91396628875824</v>
+        <v>14.64027564218928</v>
       </c>
       <c r="V7" t="n">
-        <v>-20.52635407306135</v>
+        <v>-6.760386987332817</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.1691557168959958</v>
+        <v>5.550619223956054</v>
       </c>
       <c r="X7" t="n">
-        <v>1.780340904439996</v>
+        <v>-17.66053870660931</v>
       </c>
       <c r="Y7" t="n">
-        <v>-6.158505276676626</v>
+        <v>1.747568439450616</v>
       </c>
       <c r="Z7" t="n">
-        <v>-15.12098462356028</v>
+        <v>-1.746637291183712</v>
       </c>
       <c r="AA7" t="n">
-        <v>-11.12535312508352</v>
+        <v>-7.447814022222066</v>
       </c>
       <c r="AB7" t="n">
-        <v>-15.93689480275167</v>
+        <v>6.502737954629477</v>
       </c>
       <c r="AC7" t="n">
-        <v>-24.5319681629065</v>
+        <v>-44.61830314407507</v>
       </c>
     </row>
     <row r="8">
@@ -3050,88 +3050,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>4.021828577099516</v>
+        <v>-15.90971247723647</v>
       </c>
       <c r="C8" t="n">
-        <v>-15.57150013571733</v>
+        <v>-5.627722207001062</v>
       </c>
       <c r="D8" t="n">
-        <v>-10.90100584127949</v>
+        <v>-12.32611370703521</v>
       </c>
       <c r="E8" t="n">
-        <v>-9.532806578230469</v>
+        <v>-0.3795358579761849</v>
       </c>
       <c r="F8" t="n">
-        <v>5.380777959619917</v>
+        <v>8.115925983291984</v>
       </c>
       <c r="G8" t="n">
-        <v>-3.966695784140096</v>
+        <v>-2.260290485882043</v>
       </c>
       <c r="H8" t="n">
-        <v>-13.80372525548442</v>
+        <v>-0.2571779570006747</v>
       </c>
       <c r="I8" t="n">
-        <v>6.903014175706676</v>
+        <v>-10.3045238777016</v>
       </c>
       <c r="J8" t="n">
-        <v>3.737830451403293</v>
+        <v>-11.69028729091807</v>
       </c>
       <c r="K8" t="n">
-        <v>-10.14583607433364</v>
+        <v>-8.196146027751176</v>
       </c>
       <c r="L8" t="n">
-        <v>10.12108663168484</v>
+        <v>8.770715706558148</v>
       </c>
       <c r="M8" t="n">
-        <v>-1.175534995679448</v>
+        <v>-3.814599226789914</v>
       </c>
       <c r="N8" t="n">
-        <v>9.418545050546875</v>
+        <v>-15.32574933173023</v>
       </c>
       <c r="O8" t="n">
-        <v>4.79733000313057</v>
+        <v>15.14069079071709</v>
       </c>
       <c r="P8" t="n">
-        <v>-22.66207779661712</v>
+        <v>3.841486808113955</v>
       </c>
       <c r="Q8" t="n">
-        <v>-27.60158824197346</v>
+        <v>-13.6211795266525</v>
       </c>
       <c r="R8" t="n">
-        <v>-9.020877123377094</v>
+        <v>-8.340118181411874</v>
       </c>
       <c r="S8" t="n">
-        <v>-2.67277044729423</v>
+        <v>16.88046091869175</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.9949539095172604</v>
+        <v>-17.84889762987029</v>
       </c>
       <c r="U8" t="n">
-        <v>1.963444593972111</v>
+        <v>-7.90959243971433</v>
       </c>
       <c r="V8" t="n">
-        <v>15.83405985412469</v>
+        <v>-8.300117785792489</v>
       </c>
       <c r="W8" t="n">
-        <v>-4.090238182457748</v>
+        <v>4.333612722154336</v>
       </c>
       <c r="X8" t="n">
-        <v>3.940077898503061</v>
+        <v>-16.77669573276757</v>
       </c>
       <c r="Y8" t="n">
-        <v>5.075906835506263</v>
+        <v>-20.11392220029712</v>
       </c>
       <c r="Z8" t="n">
-        <v>-24.54736583830473</v>
+        <v>-1.187253132140917</v>
       </c>
       <c r="AA8" t="n">
-        <v>3.382393359971921</v>
+        <v>-26.06129251246172</v>
       </c>
       <c r="AB8" t="n">
-        <v>13.26159594525128</v>
+        <v>-13.00989373662897</v>
       </c>
       <c r="AC8" t="n">
-        <v>-35.27512345550768</v>
+        <v>-46.79870026326006</v>
       </c>
     </row>
     <row r="9">
@@ -3139,88 +3139,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>6.269515856870319</v>
+        <v>-6.398822348157381</v>
       </c>
       <c r="C9" t="n">
-        <v>12.79173233313985</v>
+        <v>-1.632516700766025</v>
       </c>
       <c r="D9" t="n">
-        <v>8.085249421617675</v>
+        <v>5.376492440797194</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.275949688719011</v>
+        <v>8.296867895445702</v>
       </c>
       <c r="F9" t="n">
-        <v>8.649575766948651</v>
+        <v>13.19860333908353</v>
       </c>
       <c r="G9" t="n">
-        <v>1.677623424502451</v>
+        <v>-6.196503588947222</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3830083663432577</v>
+        <v>-5.045851777839451</v>
       </c>
       <c r="I9" t="n">
-        <v>3.746715309277513</v>
+        <v>-2.326403830537651</v>
       </c>
       <c r="J9" t="n">
-        <v>7.906083034421179</v>
+        <v>1.469569212263153</v>
       </c>
       <c r="K9" t="n">
-        <v>-1.596864294706822</v>
+        <v>-22.9771658577931</v>
       </c>
       <c r="L9" t="n">
-        <v>4.996236950505045</v>
+        <v>6.352417926464163</v>
       </c>
       <c r="M9" t="n">
-        <v>23.31865223718261</v>
+        <v>2.200206823091766</v>
       </c>
       <c r="N9" t="n">
-        <v>-14.91237988418367</v>
+        <v>-13.41507458488935</v>
       </c>
       <c r="O9" t="n">
-        <v>-4.480070834574482</v>
+        <v>-3.870263471076483</v>
       </c>
       <c r="P9" t="n">
-        <v>-10.51494155498331</v>
+        <v>6.076644119401887</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.760379797523174</v>
+        <v>-9.920983542701988</v>
       </c>
       <c r="R9" t="n">
-        <v>14.19717418662423</v>
+        <v>8.142713002255434</v>
       </c>
       <c r="S9" t="n">
-        <v>-11.84456519236306</v>
+        <v>5.247126404065011</v>
       </c>
       <c r="T9" t="n">
-        <v>-18.98251447515292</v>
+        <v>-3.013695264444169</v>
       </c>
       <c r="U9" t="n">
-        <v>0.4588773697953181</v>
+        <v>-3.233880748928969</v>
       </c>
       <c r="V9" t="n">
-        <v>-1.4748855129997</v>
+        <v>14.19083078680588</v>
       </c>
       <c r="W9" t="n">
-        <v>1.121617004501341</v>
+        <v>-1.77235388068868</v>
       </c>
       <c r="X9" t="n">
-        <v>1.769586141850215</v>
+        <v>0.4853980060014154</v>
       </c>
       <c r="Y9" t="n">
-        <v>3.084211235105146</v>
+        <v>-11.61245515257498</v>
       </c>
       <c r="Z9" t="n">
-        <v>-8.828305185935811</v>
+        <v>-20.00428048337838</v>
       </c>
       <c r="AA9" t="n">
-        <v>-1.726647795188482</v>
+        <v>3.852468463463529</v>
       </c>
       <c r="AB9" t="n">
-        <v>-10.36351180430247</v>
+        <v>-10.91824497776777</v>
       </c>
       <c r="AC9" t="n">
-        <v>-23.4021632250989</v>
+        <v>-27.42675730230798</v>
       </c>
     </row>
     <row r="10">
@@ -3228,88 +3228,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>11.40333347762263</v>
+        <v>-1.2164722392424</v>
       </c>
       <c r="C10" t="n">
-        <v>-19.40297632081347</v>
+        <v>-11.45050024574915</v>
       </c>
       <c r="D10" t="n">
-        <v>-15.49442577911347</v>
+        <v>5.379633434012145</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.787244985784533</v>
+        <v>1.057679041618949</v>
       </c>
       <c r="F10" t="n">
-        <v>8.104018910101932</v>
+        <v>-5.537130777064892</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.923363419368509</v>
+        <v>-8.400673372050916</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.8995158778785379</v>
+        <v>-19.05377386216486</v>
       </c>
       <c r="I10" t="n">
-        <v>2.943541966284124</v>
+        <v>-14.55442616776373</v>
       </c>
       <c r="J10" t="n">
-        <v>-3.248299954302061</v>
+        <v>11.95325502999418</v>
       </c>
       <c r="K10" t="n">
-        <v>-10.06556452982133</v>
+        <v>1.864724338770341</v>
       </c>
       <c r="L10" t="n">
-        <v>-3.934737693730447</v>
+        <v>1.431921363608129</v>
       </c>
       <c r="M10" t="n">
-        <v>1.788535926974497</v>
+        <v>8.1191116970252</v>
       </c>
       <c r="N10" t="n">
-        <v>-31.04291501580686</v>
+        <v>11.4832281287722</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9379417600441604</v>
+        <v>2.975096678117097</v>
       </c>
       <c r="P10" t="n">
-        <v>-5.743591022915799</v>
+        <v>-4.716339417692327</v>
       </c>
       <c r="Q10" t="n">
-        <v>-1.579457424369115</v>
+        <v>4.318105369722222</v>
       </c>
       <c r="R10" t="n">
-        <v>3.841860469328702</v>
+        <v>-5.074374610978587</v>
       </c>
       <c r="S10" t="n">
-        <v>-12.83182609148938</v>
+        <v>1.670406697499622</v>
       </c>
       <c r="T10" t="n">
-        <v>-14.94267498829149</v>
+        <v>-3.117679282614945</v>
       </c>
       <c r="U10" t="n">
-        <v>4.772701091888765</v>
+        <v>1.512155377507596</v>
       </c>
       <c r="V10" t="n">
-        <v>-13.49343271782719</v>
+        <v>-3.822074686890403</v>
       </c>
       <c r="W10" t="n">
-        <v>-12.13984831530327</v>
+        <v>1.728125437724763</v>
       </c>
       <c r="X10" t="n">
-        <v>1.883293403757542</v>
+        <v>-2.578661058575849</v>
       </c>
       <c r="Y10" t="n">
-        <v>-10.51233326280028</v>
+        <v>7.416582675570321</v>
       </c>
       <c r="Z10" t="n">
-        <v>-5.893805636593873</v>
+        <v>-2.173128685650406</v>
       </c>
       <c r="AA10" t="n">
-        <v>-6.762626022146755</v>
+        <v>-7.109385930832257</v>
       </c>
       <c r="AB10" t="n">
-        <v>-5.352132222903689</v>
+        <v>0.4591684464186017</v>
       </c>
       <c r="AC10" t="n">
-        <v>-43.72985997995779</v>
+        <v>-48.20252964268965</v>
       </c>
     </row>
     <row r="11">
@@ -3317,88 +3317,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>7.831376394154908</v>
+        <v>0.9288684790531327</v>
       </c>
       <c r="C11" t="n">
-        <v>-21.0642464989096</v>
+        <v>7.41153211312891</v>
       </c>
       <c r="D11" t="n">
-        <v>-9.961359641291317</v>
+        <v>-12.53722374355275</v>
       </c>
       <c r="E11" t="n">
-        <v>26.40677120197054</v>
+        <v>-13.12140189163336</v>
       </c>
       <c r="F11" t="n">
-        <v>11.27905895440771</v>
+        <v>-5.378012006363437</v>
       </c>
       <c r="G11" t="n">
-        <v>-23.53344213623977</v>
+        <v>-8.705409258735472</v>
       </c>
       <c r="H11" t="n">
-        <v>15.15789577084045</v>
+        <v>-6.828347155360569</v>
       </c>
       <c r="I11" t="n">
-        <v>23.38439969422071</v>
+        <v>-0.7041355133930995</v>
       </c>
       <c r="J11" t="n">
-        <v>-9.597023242825912</v>
+        <v>0.5244291281140994</v>
       </c>
       <c r="K11" t="n">
-        <v>-2.341675386682333</v>
+        <v>-5.85163348589084</v>
       </c>
       <c r="L11" t="n">
-        <v>-22.07651375006833</v>
+        <v>-1.619613858830224</v>
       </c>
       <c r="M11" t="n">
-        <v>-7.147187888313028</v>
+        <v>-16.12025393491743</v>
       </c>
       <c r="N11" t="n">
-        <v>9.501437736417291</v>
+        <v>-20.73276359946449</v>
       </c>
       <c r="O11" t="n">
-        <v>-13.41179577267494</v>
+        <v>-2.05317976063329</v>
       </c>
       <c r="P11" t="n">
-        <v>-6.462026141411836</v>
+        <v>3.333447273202541</v>
       </c>
       <c r="Q11" t="n">
-        <v>-8.197364476642338</v>
+        <v>-11.06278207010978</v>
       </c>
       <c r="R11" t="n">
-        <v>-3.011768147076992</v>
+        <v>13.90502491439268</v>
       </c>
       <c r="S11" t="n">
-        <v>-1.954634682999003</v>
+        <v>-1.551588885475272</v>
       </c>
       <c r="T11" t="n">
-        <v>-19.97772370560151</v>
+        <v>4.939989175108254</v>
       </c>
       <c r="U11" t="n">
-        <v>-14.63130628144851</v>
+        <v>1.081928499759411</v>
       </c>
       <c r="V11" t="n">
-        <v>-10.54824901786116</v>
+        <v>-5.652860501399569</v>
       </c>
       <c r="W11" t="n">
-        <v>-11.10741499854274</v>
+        <v>-3.641786494582059</v>
       </c>
       <c r="X11" t="n">
-        <v>2.005400795856137</v>
+        <v>-2.974145992229329</v>
       </c>
       <c r="Y11" t="n">
-        <v>-5.887670106272041</v>
+        <v>-19.52703952133388</v>
       </c>
       <c r="Z11" t="n">
-        <v>-18.43227521952509</v>
+        <v>-13.82790031539912</v>
       </c>
       <c r="AA11" t="n">
-        <v>-24.21259068899837</v>
+        <v>-25.81937297558348</v>
       </c>
       <c r="AB11" t="n">
-        <v>-16.89810946691512</v>
+        <v>-22.27632385803323</v>
       </c>
       <c r="AC11" t="n">
-        <v>-24.83698325106778</v>
+        <v>-35.46577332817661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>